<commit_message>
Agregando nuevmos metodos a la clase Util
</commit_message>
<xml_diff>
--- a/backup/cuenta_2200555126.xlsx
+++ b/backup/cuenta_2200555126.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="99">
   <si>
     <t>D</t>
   </si>
@@ -309,6 +309,18 @@
   </si>
   <si>
     <t>2513.07</t>
+  </si>
+  <si>
+    <t>CONSUMO VISA NA MI GASOLINERA</t>
+  </si>
+  <si>
+    <t>0008065921</t>
+  </si>
+  <si>
+    <t>15.26  </t>
+  </si>
+  <si>
+    <t>2497.81</t>
   </si>
 </sst>
 </file>
@@ -631,9 +643,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H28"/>
+  <dimension ref="A1:H29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
       <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
@@ -646,52 +658,52 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1">
-        <v>41670</v>
+        <v>41674</v>
       </c>
       <c r="B1" t="s">
-        <v>17</v>
+        <v>95</v>
       </c>
       <c r="C1" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>18</v>
+        <v>96</v>
       </c>
       <c r="E1" t="s">
-        <v>19</v>
+        <v>1</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>20</v>
+        <v>97</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="H1" t="str">
-        <f>CONCATENATE("array('mo_fecha' =&gt; new \DateTime('",TEXT(A1,"yyyy-mm-dd"),"'), 'mo_concepto' =&gt; '",B1,"', 'mo_tipo' =&gt; '",C1,"', 'mo_documento' =&gt; '",D1,"', 'mo_oficina' =&gt; '",E1,"', 'mo_monto' =&gt; ",F1,", 'mo_saldo' =&gt; ",G1,", 'mo_fecha_crea' =&gt; new \DateTime('2014-02-01 00:00:01'), 'mo_quien_crea' =&gt; 1, 'mo_fecha_modifica' =&gt; NULL, 'mo_quien_modifica' =&gt; NULL),")</f>
-        <v>array('mo_fecha' =&gt; new \DateTime('2014-01-31'), 'mo_concepto' =&gt; 'INTERES A SU FAVOR', 'mo_tipo' =&gt; 'C', 'mo_documento' =&gt; '0000963683', 'mo_oficina' =&gt; 'AGENCIA PARA PROCESOS BATCH', 'mo_monto' =&gt; 4.63  , 'mo_saldo' =&gt; 2513.07, 'mo_fecha_crea' =&gt; new \DateTime('2014-02-01 00:00:01'), 'mo_quien_crea' =&gt; 1, 'mo_fecha_modifica' =&gt; NULL, 'mo_quien_modifica' =&gt; NULL),</v>
+        <f>CONCATENATE("array('mo_fecha' =&gt; new \DateTime('",TEXT(A1,"yyyy-mm-dd"),"'), 'mo_concepto' =&gt; '",B1,"', 'mo_tipo' =&gt; '",C1,"', 'mo_documento' =&gt; '",D1,"', 'mo_oficina' =&gt; '",E1,"', 'mo_monto' =&gt; ",TRIM(F1),", 'mo_saldo' =&gt; ",G1,", 'mo_fecha_crea' =&gt; new \DateTime('2014-02-01 00:00:01'), 'mo_quien_crea' =&gt; 1, 'mo_fecha_modifica' =&gt; NULL, 'mo_quien_modifica' =&gt; NULL),")</f>
+        <v>array('mo_fecha' =&gt; new \DateTime('2014-02-04'), 'mo_concepto' =&gt; 'CONSUMO VISA NA MI GASOLINERA', 'mo_tipo' =&gt; 'D', 'mo_documento' =&gt; '0008065921', 'mo_oficina' =&gt; 'INSTITUCIONAL SS.CC.', 'mo_monto' =&gt; 15.26  , 'mo_saldo' =&gt; 2497.81, 'mo_fecha_crea' =&gt; new \DateTime('2014-02-01 00:00:01'), 'mo_quien_crea' =&gt; 1, 'mo_fecha_modifica' =&gt; NULL, 'mo_quien_modifica' =&gt; NULL),</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>41666</v>
+        <v>41670</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="C2" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="E2" t="s">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>71</v>
+        <v>20</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -699,22 +711,22 @@
         <v>41666</v>
       </c>
       <c r="B3" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C3" t="s">
         <v>0</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E3" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>23</v>
+        <v>71</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -722,22 +734,22 @@
         <v>41666</v>
       </c>
       <c r="B4" t="s">
-        <v>24</v>
+        <v>2</v>
       </c>
       <c r="C4" t="s">
         <v>0</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E4" t="s">
-        <v>26</v>
+        <v>1</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -745,45 +757,45 @@
         <v>41666</v>
       </c>
       <c r="B5" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C5" t="s">
         <v>0</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="E5" t="s">
-        <v>1</v>
+        <v>26</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
-        <v>41660</v>
+        <v>41666</v>
       </c>
       <c r="B6" t="s">
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="C6" t="s">
         <v>0</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E6" t="s">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>9</v>
+        <v>30</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -791,22 +803,22 @@
         <v>41660</v>
       </c>
       <c r="B7" t="s">
-        <v>32</v>
+        <v>11</v>
       </c>
       <c r="C7" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E7" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -814,68 +826,68 @@
         <v>41660</v>
       </c>
       <c r="B8" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C8" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E8" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>36</v>
+        <v>6</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
-        <v>41659</v>
+        <v>41660</v>
       </c>
       <c r="B9" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C9" t="s">
         <v>0</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="E9" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
-        <v>41655</v>
+        <v>41659</v>
       </c>
       <c r="B10" t="s">
-        <v>2</v>
+        <v>37</v>
       </c>
       <c r="C10" t="s">
         <v>0</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E10" t="s">
         <v>1</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -883,50 +895,50 @@
         <v>41655</v>
       </c>
       <c r="B11" t="s">
-        <v>42</v>
+        <v>2</v>
       </c>
       <c r="C11" t="s">
         <v>0</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="E11" t="s">
-        <v>44</v>
+        <v>1</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>6</v>
+        <v>41</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
-        <v>41652</v>
+        <v>41655</v>
       </c>
       <c r="B12" t="s">
-        <v>3</v>
+        <v>42</v>
       </c>
       <c r="C12" t="s">
         <v>0</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E12" t="s">
-        <v>5</v>
+        <v>44</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>46</v>
+        <v>6</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
-        <v>41649</v>
+        <v>41652</v>
       </c>
       <c r="B13" t="s">
         <v>3</v>
@@ -935,39 +947,39 @@
         <v>0</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>16</v>
+        <v>45</v>
       </c>
       <c r="E13" t="s">
         <v>5</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>15</v>
+        <v>46</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
-        <v>41648</v>
+        <v>41649</v>
       </c>
       <c r="B14" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C14" t="s">
         <v>0</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>47</v>
+        <v>16</v>
       </c>
       <c r="E14" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>48</v>
+        <v>15</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -975,68 +987,68 @@
         <v>41648</v>
       </c>
       <c r="B15" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="C15" t="s">
         <v>0</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E15" t="s">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>9</v>
+        <v>48</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
-        <v>41647</v>
+        <v>41648</v>
       </c>
       <c r="B16" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="C16" t="s">
         <v>0</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E16" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>51</v>
+        <v>9</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
-        <v>41646</v>
+        <v>41647</v>
       </c>
       <c r="B17" t="s">
-        <v>52</v>
+        <v>2</v>
       </c>
       <c r="C17" t="s">
         <v>0</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="E17" t="s">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>13</v>
+        <v>51</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
@@ -1044,22 +1056,22 @@
         <v>41646</v>
       </c>
       <c r="B18" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C18" t="s">
         <v>0</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E18" t="s">
         <v>12</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
@@ -1067,22 +1079,22 @@
         <v>41646</v>
       </c>
       <c r="B19" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C19" t="s">
         <v>0</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E19" t="s">
         <v>12</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>58</v>
+        <v>14</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
@@ -1090,95 +1102,115 @@
         <v>41646</v>
       </c>
       <c r="B20" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C20" t="s">
         <v>0</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E20" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
-        <v>41645</v>
+        <v>41646</v>
       </c>
       <c r="B21" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C21" t="s">
         <v>0</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="E21" t="s">
-        <v>64</v>
+        <v>5</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>9</v>
+        <v>61</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
-        <v>41642</v>
+        <v>41645</v>
       </c>
       <c r="B22" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C22" t="s">
         <v>0</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="E22" t="s">
-        <v>10</v>
+        <v>64</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>67</v>
+        <v>9</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
+        <v>41642</v>
+      </c>
+      <c r="B23" t="s">
+        <v>65</v>
+      </c>
+      <c r="C23" t="s">
+        <v>0</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="E23" t="s">
+        <v>10</v>
+      </c>
+      <c r="F23" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="G23" s="3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="1">
         <v>41641</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B24" t="s">
         <v>68</v>
       </c>
-      <c r="C23" t="s">
-        <v>0</v>
-      </c>
-      <c r="D23" s="2" t="s">
+      <c r="C24" t="s">
+        <v>0</v>
+      </c>
+      <c r="D24" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="E23" t="s">
+      <c r="E24" t="s">
         <v>1</v>
       </c>
-      <c r="F23" s="3" t="s">
+      <c r="F24" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="G23" s="3" t="s">
+      <c r="G24" s="3" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="1"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
@@ -1191,6 +1223,9 @@
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Evitando un poco el AJAX en la vista
</commit_message>
<xml_diff>
--- a/backup/cuenta_2200555126.xlsx
+++ b/backup/cuenta_2200555126.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="106">
   <si>
     <t>D</t>
   </si>
@@ -321,6 +321,27 @@
   </si>
   <si>
     <t>2497.81</t>
+  </si>
+  <si>
+    <t>0002420226</t>
+  </si>
+  <si>
+    <t>0000937060</t>
+  </si>
+  <si>
+    <t>281.05  </t>
+  </si>
+  <si>
+    <t>0004190618</t>
+  </si>
+  <si>
+    <t>2778.86</t>
+  </si>
+  <si>
+    <t>2597.81</t>
+  </si>
+  <si>
+    <t>0000952785</t>
   </si>
 </sst>
 </file>
@@ -643,10 +664,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H29"/>
+  <dimension ref="A1:H33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -658,333 +679,333 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1">
-        <v>41674</v>
+        <v>41680</v>
       </c>
       <c r="B1" t="s">
-        <v>95</v>
+        <v>3</v>
       </c>
       <c r="C1" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>96</v>
+        <v>105</v>
       </c>
       <c r="E1" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>97</v>
+        <v>6</v>
       </c>
       <c r="G1" s="3" t="s">
         <v>98</v>
       </c>
       <c r="H1" t="str">
-        <f>CONCATENATE("array('mo_fecha' =&gt; new \DateTime('",TEXT(A1,"yyyy-mm-dd"),"'), 'mo_concepto' =&gt; '",B1,"', 'mo_tipo' =&gt; '",C1,"', 'mo_documento' =&gt; '",D1,"', 'mo_oficina' =&gt; '",E1,"', 'mo_monto' =&gt; ",TRIM(F1),", 'mo_saldo' =&gt; ",G1,", 'mo_fecha_crea' =&gt; new \DateTime('2014-02-01 00:00:01'), 'mo_quien_crea' =&gt; 1, 'mo_fecha_modifica' =&gt; NULL, 'mo_quien_modifica' =&gt; NULL),")</f>
-        <v>array('mo_fecha' =&gt; new \DateTime('2014-02-04'), 'mo_concepto' =&gt; 'CONSUMO VISA NA MI GASOLINERA', 'mo_tipo' =&gt; 'D', 'mo_documento' =&gt; '0008065921', 'mo_oficina' =&gt; 'INSTITUCIONAL SS.CC.', 'mo_monto' =&gt; 15.26  , 'mo_saldo' =&gt; 2497.81, 'mo_fecha_crea' =&gt; new \DateTime('2014-02-01 00:00:01'), 'mo_quien_crea' =&gt; 1, 'mo_fecha_modifica' =&gt; NULL, 'mo_quien_modifica' =&gt; NULL),</v>
+        <f ca="1">CONCATENATE("array('mo_fecha' =&gt; new \DateTime('",TEXT(A1,"yyyy-mm-dd"),"'), 'mo_concepto' =&gt; '",B1,"', 'mo_tipo' =&gt; '",C1,"', 'mo_documento' =&gt; '",D1,"', 'mo_oficina' =&gt; '",E1,"', 'mo_monto' =&gt; ",TRIM(F1),", 'mo_saldo' =&gt; ",G1,", 'mo_fecha_crea' =&gt; new \DateTime('",TEXT(NOW(),"yyyy-mm-dd H:m:s"),"'), 'mo_quien_crea' =&gt; 1, 'mo_fecha_modifica' =&gt; NULL, 'mo_quien_modifica' =&gt; NULL),")</f>
+        <v>array('mo_fecha' =&gt; new \DateTime('2014-02-10'), 'mo_concepto' =&gt; '  TRANSFERENCIA INTERNET', 'mo_tipo' =&gt; 'D', 'mo_documento' =&gt; '0000952785', 'mo_oficina' =&gt; 'AG. NORTE', 'mo_monto' =&gt; 100.00  , 'mo_saldo' =&gt; 2497.81, 'mo_fecha_crea' =&gt; new \DateTime('2014-02-08 10:42:33'), 'mo_quien_crea' =&gt; 1, 'mo_fecha_modifica' =&gt; NULL, 'mo_quien_modifica' =&gt; NULL),</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>41670</v>
+        <v>41677</v>
       </c>
       <c r="B2" t="s">
-        <v>17</v>
+        <v>32</v>
       </c>
       <c r="C2" t="s">
         <v>4</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>18</v>
+        <v>99</v>
       </c>
       <c r="E2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>94</v>
+        <v>104</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>41666</v>
+        <v>41677</v>
       </c>
       <c r="B3" t="s">
-        <v>3</v>
+        <v>59</v>
       </c>
       <c r="C3" t="s">
         <v>0</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>21</v>
+        <v>100</v>
       </c>
       <c r="E3" t="s">
         <v>5</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>71</v>
+        <v>101</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
-        <v>41666</v>
+        <v>41676</v>
       </c>
       <c r="B4" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>22</v>
+        <v>102</v>
       </c>
       <c r="E4" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>23</v>
+        <v>101</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>92</v>
+        <v>103</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
-        <v>41666</v>
+        <v>41674</v>
       </c>
       <c r="B5" t="s">
-        <v>24</v>
+        <v>95</v>
       </c>
       <c r="C5" t="s">
         <v>0</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>25</v>
+        <v>96</v>
       </c>
       <c r="E5" t="s">
-        <v>26</v>
+        <v>1</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>27</v>
+        <v>97</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>91</v>
+        <v>98</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
-        <v>41666</v>
+        <v>41670</v>
       </c>
       <c r="B6" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="C6" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="E6" t="s">
-        <v>1</v>
+        <v>19</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
-        <v>41660</v>
+        <v>41666</v>
       </c>
       <c r="B7" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="C7" t="s">
         <v>0</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="E7" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>9</v>
+        <v>71</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
-        <v>41660</v>
+        <v>41666</v>
       </c>
       <c r="B8" t="s">
-        <v>32</v>
+        <v>2</v>
       </c>
       <c r="C8" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="E8" t="s">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
-        <v>41660</v>
+        <v>41666</v>
       </c>
       <c r="B9" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="C9" t="s">
         <v>0</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="E9" t="s">
-        <v>12</v>
+        <v>26</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
-        <v>41659</v>
+        <v>41666</v>
       </c>
       <c r="B10" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="C10" t="s">
         <v>0</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="E10" t="s">
         <v>1</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
-        <v>41655</v>
+        <v>41660</v>
       </c>
       <c r="B11" t="s">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="C11" t="s">
         <v>0</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="E11" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>41</v>
+        <v>9</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
-        <v>41655</v>
+        <v>41660</v>
       </c>
       <c r="B12" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="C12" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="E12" t="s">
-        <v>44</v>
+        <v>10</v>
       </c>
       <c r="F12" s="3" t="s">
         <v>6</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
-        <v>41652</v>
+        <v>41660</v>
       </c>
       <c r="B13" t="s">
-        <v>3</v>
+        <v>34</v>
       </c>
       <c r="C13" t="s">
         <v>0</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="E13" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
-        <v>41649</v>
+        <v>41659</v>
       </c>
       <c r="B14" t="s">
-        <v>3</v>
+        <v>37</v>
       </c>
       <c r="C14" t="s">
         <v>0</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>16</v>
+        <v>38</v>
       </c>
       <c r="E14" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>15</v>
+        <v>39</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
-        <v>41648</v>
+        <v>41655</v>
       </c>
       <c r="B15" t="s">
         <v>2</v>
@@ -993,239 +1014,331 @@
         <v>0</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="E15" t="s">
         <v>1</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
-        <v>41648</v>
+        <v>41655</v>
       </c>
       <c r="B16" t="s">
-        <v>7</v>
+        <v>42</v>
       </c>
       <c r="C16" t="s">
         <v>0</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="E16" t="s">
-        <v>8</v>
+        <v>44</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
-        <v>41647</v>
+        <v>41652</v>
       </c>
       <c r="B17" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C17" t="s">
         <v>0</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="E17" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
-        <v>41646</v>
+        <v>41649</v>
       </c>
       <c r="B18" t="s">
-        <v>52</v>
+        <v>3</v>
       </c>
       <c r="C18" t="s">
         <v>0</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>53</v>
+        <v>16</v>
       </c>
       <c r="E18" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
-        <v>41646</v>
+        <v>41648</v>
       </c>
       <c r="B19" t="s">
-        <v>54</v>
+        <v>2</v>
       </c>
       <c r="C19" t="s">
         <v>0</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="E19" t="s">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>14</v>
+        <v>48</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
-        <v>41646</v>
+        <v>41648</v>
       </c>
       <c r="B20" t="s">
-        <v>56</v>
+        <v>7</v>
       </c>
       <c r="C20" t="s">
         <v>0</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="E20" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>58</v>
+        <v>9</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
-        <v>41646</v>
+        <v>41647</v>
       </c>
       <c r="B21" t="s">
-        <v>59</v>
+        <v>2</v>
       </c>
       <c r="C21" t="s">
         <v>0</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="E21" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
-        <v>41645</v>
+        <v>41646</v>
       </c>
       <c r="B22" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="C22" t="s">
         <v>0</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="E22" t="s">
-        <v>64</v>
+        <v>12</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
-        <v>41642</v>
+        <v>41646</v>
       </c>
       <c r="B23" t="s">
-        <v>65</v>
+        <v>54</v>
       </c>
       <c r="C23" t="s">
         <v>0</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="E23" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>67</v>
+        <v>14</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
+        <v>41646</v>
+      </c>
+      <c r="B24" t="s">
+        <v>56</v>
+      </c>
+      <c r="C24" t="s">
+        <v>0</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="E24" t="s">
+        <v>12</v>
+      </c>
+      <c r="F24" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="G24" s="3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="1">
+        <v>41646</v>
+      </c>
+      <c r="B25" t="s">
+        <v>59</v>
+      </c>
+      <c r="C25" t="s">
+        <v>0</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="E25" t="s">
+        <v>5</v>
+      </c>
+      <c r="F25" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="G25" s="3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="1">
+        <v>41645</v>
+      </c>
+      <c r="B26" t="s">
+        <v>62</v>
+      </c>
+      <c r="C26" t="s">
+        <v>0</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="E26" t="s">
+        <v>64</v>
+      </c>
+      <c r="F26" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G26" s="3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="1">
+        <v>41642</v>
+      </c>
+      <c r="B27" t="s">
+        <v>65</v>
+      </c>
+      <c r="C27" t="s">
+        <v>0</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="E27" t="s">
+        <v>10</v>
+      </c>
+      <c r="F27" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="G27" s="3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="1">
         <v>41641</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B28" t="s">
         <v>68</v>
       </c>
-      <c r="C24" t="s">
-        <v>0</v>
-      </c>
-      <c r="D24" s="2" t="s">
+      <c r="C28" t="s">
+        <v>0</v>
+      </c>
+      <c r="D28" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="E24" t="s">
+      <c r="E28" t="s">
         <v>1</v>
       </c>
-      <c r="F24" s="3" t="s">
+      <c r="F28" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="G24" s="3" t="s">
+      <c r="G28" s="3" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="1"/>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="1"/>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="1"/>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="1"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" s="1"/>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" s="1"/>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" s="1"/>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Actualizando campos en la base de datos
</commit_message>
<xml_diff>
--- a/backup/cuenta_2200555126.xlsx
+++ b/backup/cuenta_2200555126.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="113">
   <si>
     <t>D</t>
   </si>
@@ -342,6 +342,27 @@
   </si>
   <si>
     <t>0000952785</t>
+  </si>
+  <si>
+    <t>13118145-MASTERCARD-RA-518114000072</t>
+  </si>
+  <si>
+    <t>0007629440</t>
+  </si>
+  <si>
+    <t>718.86  </t>
+  </si>
+  <si>
+    <t>0007829636</t>
+  </si>
+  <si>
+    <t>115.00  </t>
+  </si>
+  <si>
+    <t>2612.81</t>
+  </si>
+  <si>
+    <t>1893.95</t>
   </si>
 </sst>
 </file>
@@ -664,10 +685,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H33"/>
+  <dimension ref="A1:H35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -679,34 +700,34 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1">
-        <v>41680</v>
+        <v>41682</v>
       </c>
       <c r="B1" t="s">
-        <v>3</v>
+        <v>106</v>
       </c>
       <c r="C1" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="E1" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>6</v>
+        <v>108</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>98</v>
+        <v>112</v>
       </c>
       <c r="H1" t="str">
-        <f ca="1">CONCATENATE("array('mo_fecha' =&gt; new \DateTime('",TEXT(A1,"yyyy-mm-dd"),"'), 'mo_concepto' =&gt; '",B1,"', 'mo_tipo' =&gt; '",C1,"', 'mo_documento' =&gt; '",D1,"', 'mo_oficina' =&gt; '",E1,"', 'mo_monto' =&gt; ",TRIM(F1),", 'mo_saldo' =&gt; ",G1,", 'mo_fecha_crea' =&gt; new \DateTime('",TEXT(NOW(),"yyyy-mm-dd H:m:s"),"'), 'mo_quien_crea' =&gt; 1, 'mo_fecha_modifica' =&gt; NULL, 'mo_quien_modifica' =&gt; NULL),")</f>
-        <v>array('mo_fecha' =&gt; new \DateTime('2014-02-10'), 'mo_concepto' =&gt; '  TRANSFERENCIA INTERNET', 'mo_tipo' =&gt; 'D', 'mo_documento' =&gt; '0000952785', 'mo_oficina' =&gt; 'AG. NORTE', 'mo_monto' =&gt; 100.00  , 'mo_saldo' =&gt; 2497.81, 'mo_fecha_crea' =&gt; new \DateTime('2014-02-08 10:42:33'), 'mo_quien_crea' =&gt; 1, 'mo_fecha_modifica' =&gt; NULL, 'mo_quien_modifica' =&gt; NULL),</v>
+        <f ca="1">CONCATENATE("array('mo_fecha' =&gt; new \DateTime('",TEXT(A1,"yyyy-mm-dd"),"'), 'mo_concepto' =&gt; '",B1,"', 'mo_tipo' =&gt; '",C1,"', 'mo_documento' =&gt; '",D1,"', 'mo_oficina' =&gt; '",E1,"', 'mo_monto' =&gt; ",TRIM(F1),", 'mo_saldo' =&gt; ",G1,", 'mo_fecha_crea' =&gt; new \DateTime('",TEXT(NOW(),"yyyy-mm-dd H:m:s"),"'), 'mo_quien_crea' =&gt; 1, 'mo_fecha_modifica' =&gt; NULL, 'mo_quien_modifica' =&gt; NULL 'mo_borrado_logico' =&gt; false),")</f>
+        <v>array('mo_fecha' =&gt; new \DateTime('2014-02-12'), 'mo_concepto' =&gt; '13118145-MASTERCARD-RA-518114000072', 'mo_tipo' =&gt; 'D', 'mo_documento' =&gt; '0007629440', 'mo_oficina' =&gt; 'SERVICIOS CENTRALES', 'mo_monto' =&gt; 718.86  , 'mo_saldo' =&gt; 1893.95, 'mo_fecha_crea' =&gt; new \DateTime('2014-02-12 22:34:34'), 'mo_quien_crea' =&gt; 1, 'mo_fecha_modifica' =&gt; NULL, 'mo_quien_modifica' =&gt; NULL 'mo_borrado_logico' =&gt; false),</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>41677</v>
+        <v>41680</v>
       </c>
       <c r="B2" t="s">
         <v>32</v>
@@ -715,36 +736,36 @@
         <v>4</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>99</v>
+        <v>109</v>
       </c>
       <c r="E2" t="s">
         <v>10</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>6</v>
+        <v>110</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>104</v>
+        <v>111</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>41677</v>
+        <v>41680</v>
       </c>
       <c r="B3" t="s">
-        <v>59</v>
+        <v>3</v>
       </c>
       <c r="C3" t="s">
         <v>0</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="E3" t="s">
         <v>5</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>101</v>
+        <v>6</v>
       </c>
       <c r="G3" s="3" t="s">
         <v>98</v>
@@ -752,45 +773,45 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
-        <v>41676</v>
+        <v>41677</v>
       </c>
       <c r="B4" t="s">
-        <v>3</v>
+        <v>32</v>
       </c>
       <c r="C4" t="s">
         <v>4</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="E4" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>101</v>
+        <v>6</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
-        <v>41674</v>
+        <v>41677</v>
       </c>
       <c r="B5" t="s">
-        <v>95</v>
+        <v>59</v>
       </c>
       <c r="C5" t="s">
         <v>0</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="E5" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="G5" s="3" t="s">
         <v>98</v>
@@ -798,71 +819,71 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
-        <v>41670</v>
+        <v>41676</v>
       </c>
       <c r="B6" t="s">
-        <v>17</v>
+        <v>3</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>18</v>
+        <v>102</v>
       </c>
       <c r="E6" t="s">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>20</v>
+        <v>101</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>94</v>
+        <v>103</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
-        <v>41666</v>
+        <v>41674</v>
       </c>
       <c r="B7" t="s">
-        <v>3</v>
+        <v>95</v>
       </c>
       <c r="C7" t="s">
         <v>0</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>21</v>
+        <v>96</v>
       </c>
       <c r="E7" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>71</v>
+        <v>97</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
-        <v>41666</v>
+        <v>41670</v>
       </c>
       <c r="B8" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="C8" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="E8" t="s">
-        <v>1</v>
+        <v>19</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -870,22 +891,22 @@
         <v>41666</v>
       </c>
       <c r="B9" t="s">
-        <v>24</v>
+        <v>3</v>
       </c>
       <c r="C9" t="s">
         <v>0</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="E9" t="s">
-        <v>26</v>
+        <v>5</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>27</v>
+        <v>71</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -893,68 +914,68 @@
         <v>41666</v>
       </c>
       <c r="B10" t="s">
-        <v>28</v>
+        <v>2</v>
       </c>
       <c r="C10" t="s">
         <v>0</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="E10" t="s">
         <v>1</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
-        <v>41660</v>
+        <v>41666</v>
       </c>
       <c r="B11" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="C11" t="s">
         <v>0</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="E11" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>9</v>
+        <v>27</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
-        <v>41660</v>
+        <v>41666</v>
       </c>
       <c r="B12" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C12" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="E12" t="s">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>6</v>
+        <v>30</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -962,188 +983,188 @@
         <v>41660</v>
       </c>
       <c r="B13" t="s">
-        <v>34</v>
+        <v>11</v>
       </c>
       <c r="C13" t="s">
         <v>0</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="E13" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>36</v>
+        <v>9</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
-        <v>41659</v>
+        <v>41660</v>
       </c>
       <c r="B14" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="C14" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="E14" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>39</v>
+        <v>6</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
-        <v>41655</v>
+        <v>41660</v>
       </c>
       <c r="B15" t="s">
-        <v>2</v>
+        <v>34</v>
       </c>
       <c r="C15" t="s">
         <v>0</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="E15" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
-        <v>41655</v>
+        <v>41659</v>
       </c>
       <c r="B16" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="C16" t="s">
         <v>0</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="E16" t="s">
-        <v>44</v>
+        <v>1</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>6</v>
+        <v>39</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
-        <v>41652</v>
+        <v>41655</v>
       </c>
       <c r="B17" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C17" t="s">
         <v>0</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="E17" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
-        <v>41649</v>
+        <v>41655</v>
       </c>
       <c r="B18" t="s">
-        <v>3</v>
+        <v>42</v>
       </c>
       <c r="C18" t="s">
         <v>0</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>16</v>
+        <v>43</v>
       </c>
       <c r="E18" t="s">
-        <v>5</v>
+        <v>44</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
-        <v>41648</v>
+        <v>41652</v>
       </c>
       <c r="B19" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C19" t="s">
         <v>0</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E19" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
-        <v>41648</v>
+        <v>41649</v>
       </c>
       <c r="B20" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C20" t="s">
         <v>0</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>49</v>
+        <v>16</v>
       </c>
       <c r="E20" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
-        <v>41647</v>
+        <v>41648</v>
       </c>
       <c r="B21" t="s">
         <v>2</v>
@@ -1152,62 +1173,62 @@
         <v>0</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="E21" t="s">
         <v>1</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
-        <v>41646</v>
+        <v>41648</v>
       </c>
       <c r="B22" t="s">
-        <v>52</v>
+        <v>7</v>
       </c>
       <c r="C22" t="s">
         <v>0</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="E22" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
-        <v>41646</v>
+        <v>41647</v>
       </c>
       <c r="B23" t="s">
-        <v>54</v>
+        <v>2</v>
       </c>
       <c r="C23" t="s">
         <v>0</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="E23" t="s">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>14</v>
+        <v>51</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
@@ -1215,22 +1236,22 @@
         <v>41646</v>
       </c>
       <c r="B24" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C24" t="s">
         <v>0</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="E24" t="s">
         <v>12</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>58</v>
+        <v>13</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
@@ -1238,98 +1259,138 @@
         <v>41646</v>
       </c>
       <c r="B25" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="C25" t="s">
         <v>0</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="E25" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>61</v>
+        <v>14</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
-        <v>41645</v>
+        <v>41646</v>
       </c>
       <c r="B26" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="C26" t="s">
         <v>0</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="E26" t="s">
-        <v>64</v>
+        <v>12</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>9</v>
+        <v>58</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
-        <v>41642</v>
+        <v>41646</v>
       </c>
       <c r="B27" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="C27" t="s">
         <v>0</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="E27" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
+        <v>41645</v>
+      </c>
+      <c r="B28" t="s">
+        <v>62</v>
+      </c>
+      <c r="C28" t="s">
+        <v>0</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="E28" t="s">
+        <v>64</v>
+      </c>
+      <c r="F28" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G28" s="3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" s="1">
+        <v>41642</v>
+      </c>
+      <c r="B29" t="s">
+        <v>65</v>
+      </c>
+      <c r="C29" t="s">
+        <v>0</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="E29" t="s">
+        <v>10</v>
+      </c>
+      <c r="F29" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="G29" s="3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" s="1">
         <v>41641</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B30" t="s">
         <v>68</v>
       </c>
-      <c r="C28" t="s">
-        <v>0</v>
-      </c>
-      <c r="D28" s="2" t="s">
+      <c r="C30" t="s">
+        <v>0</v>
+      </c>
+      <c r="D30" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="E28" t="s">
+      <c r="E30" t="s">
         <v>1</v>
       </c>
-      <c r="F28" s="3" t="s">
+      <c r="F30" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="G28" s="3" t="s">
+      <c r="G30" s="3" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="1"/>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="1"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
@@ -1339,6 +1400,12 @@
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" s="1"/>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" s="1"/>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Ajustando el paginador en la vista de movimientos
</commit_message>
<xml_diff>
--- a/backup/cuenta_2200555126.xlsx
+++ b/backup/cuenta_2200555126.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="117">
   <si>
     <t>D</t>
   </si>
@@ -363,6 +363,18 @@
   </si>
   <si>
     <t>1893.95</t>
+  </si>
+  <si>
+    <t>0003049433</t>
+  </si>
+  <si>
+    <t>67.76  </t>
+  </si>
+  <si>
+    <t>0002989186</t>
+  </si>
+  <si>
+    <t>1961.71</t>
   </si>
 </sst>
 </file>
@@ -685,10 +697,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H35"/>
+  <dimension ref="A1:H37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -700,80 +712,84 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1">
-        <v>41682</v>
+        <v>41690</v>
       </c>
       <c r="B1" t="s">
-        <v>106</v>
+        <v>3</v>
       </c>
       <c r="C1" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>107</v>
+        <v>113</v>
       </c>
       <c r="E1" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>108</v>
+        <v>114</v>
       </c>
       <c r="G1" s="3" t="s">
         <v>112</v>
       </c>
       <c r="H1" t="str">
-        <f ca="1">CONCATENATE("array('mo_fecha' =&gt; new \DateTime('",TEXT(A1,"yyyy-mm-dd"),"'), 'mo_concepto' =&gt; '",B1,"', 'mo_tipo' =&gt; '",C1,"', 'mo_documento' =&gt; '",D1,"', 'mo_oficina' =&gt; '",E1,"', 'mo_monto' =&gt; ",TRIM(F1),", 'mo_saldo' =&gt; ",G1,", 'mo_fecha_crea' =&gt; new \DateTime('",TEXT(NOW(),"yyyy-mm-dd H:m:s"),"'), 'mo_quien_crea' =&gt; 1, 'mo_fecha_modifica' =&gt; NULL, 'mo_quien_modifica' =&gt; NULL 'mo_borrado_logico' =&gt; false),")</f>
-        <v>array('mo_fecha' =&gt; new \DateTime('2014-02-12'), 'mo_concepto' =&gt; '13118145-MASTERCARD-RA-518114000072', 'mo_tipo' =&gt; 'D', 'mo_documento' =&gt; '0007629440', 'mo_oficina' =&gt; 'SERVICIOS CENTRALES', 'mo_monto' =&gt; 718.86  , 'mo_saldo' =&gt; 1893.95, 'mo_fecha_crea' =&gt; new \DateTime('2014-02-12 22:34:34'), 'mo_quien_crea' =&gt; 1, 'mo_fecha_modifica' =&gt; NULL, 'mo_quien_modifica' =&gt; NULL 'mo_borrado_logico' =&gt; false),</v>
+        <f ca="1">CONCATENATE("array('mo_fecha' =&gt; new \DateTime('",TEXT(A1,"yyyy-mm-dd"),"'), 'mo_concepto' =&gt; '",B1,"', 'mo_tipo' =&gt; '",C1,"', 'mo_documento' =&gt; '",D1,"', 'mo_oficina' =&gt; '",E1,"', 'mo_monto' =&gt; ",TRIM(F1),", 'mo_saldo' =&gt; ",G1,", 'mo_fecha_crea' =&gt; new \DateTime('",TEXT(NOW(),"yyyy-mm-dd H:m:s"),"'), 'mo_quien_crea' =&gt; 1, 'mo_fecha_modifica' =&gt; NULL, 'mo_quien_modifica' =&gt; NULL, 'mo_borrado_logico' =&gt; false),")</f>
+        <v>array('mo_fecha' =&gt; new \DateTime('2014-02-20'), 'mo_concepto' =&gt; '  TRANSFERENCIA INTERNET', 'mo_tipo' =&gt; 'D', 'mo_documento' =&gt; '0003049433', 'mo_oficina' =&gt; 'AG. NORTE', 'mo_monto' =&gt; 67.76  , 'mo_saldo' =&gt; 1893.95, 'mo_fecha_crea' =&gt; new \DateTime('2014-02-20 13:34:52'), 'mo_quien_crea' =&gt; 1, 'mo_fecha_modifica' =&gt; NULL, 'mo_quien_modifica' =&gt; NULL, 'mo_borrado_logico' =&gt; false),</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>41680</v>
+        <v>41690</v>
       </c>
       <c r="B2" t="s">
-        <v>32</v>
+        <v>3</v>
       </c>
       <c r="C2" t="s">
         <v>4</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>109</v>
+        <v>115</v>
       </c>
       <c r="E2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>111</v>
+        <v>116</v>
+      </c>
+      <c r="H2" t="str">
+        <f ca="1">CONCATENATE("array('mo_fecha' =&gt; new \DateTime('",TEXT(A2,"yyyy-mm-dd"),"'), 'mo_concepto' =&gt; '",B2,"', 'mo_tipo' =&gt; '",C2,"', 'mo_documento' =&gt; '",D2,"', 'mo_oficina' =&gt; '",E2,"', 'mo_monto' =&gt; ",TRIM(F2),", 'mo_saldo' =&gt; ",G2,", 'mo_fecha_crea' =&gt; new \DateTime('",TEXT(NOW(),"yyyy-mm-dd H:m:s"),"'), 'mo_quien_crea' =&gt; 1, 'mo_fecha_modifica' =&gt; NULL, 'mo_quien_modifica' =&gt; NULL, 'mo_borrado_logico' =&gt; false),")</f>
+        <v>array('mo_fecha' =&gt; new \DateTime('2014-02-20'), 'mo_concepto' =&gt; '  TRANSFERENCIA INTERNET', 'mo_tipo' =&gt; 'C', 'mo_documento' =&gt; '0002989186', 'mo_oficina' =&gt; 'AG. NORTE', 'mo_monto' =&gt; 67.76  , 'mo_saldo' =&gt; 1961.71, 'mo_fecha_crea' =&gt; new \DateTime('2014-02-20 13:34:52'), 'mo_quien_crea' =&gt; 1, 'mo_fecha_modifica' =&gt; NULL, 'mo_quien_modifica' =&gt; NULL, 'mo_borrado_logico' =&gt; false),</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>41680</v>
+        <v>41682</v>
       </c>
       <c r="B3" t="s">
-        <v>3</v>
+        <v>106</v>
       </c>
       <c r="C3" t="s">
         <v>0</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="E3" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>6</v>
+        <v>108</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>98</v>
+        <v>112</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
-        <v>41677</v>
+        <v>41680</v>
       </c>
       <c r="B4" t="s">
         <v>32</v>
@@ -782,36 +798,36 @@
         <v>4</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>99</v>
+        <v>109</v>
       </c>
       <c r="E4" t="s">
         <v>10</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>6</v>
+        <v>110</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>104</v>
+        <v>111</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
-        <v>41677</v>
+        <v>41680</v>
       </c>
       <c r="B5" t="s">
-        <v>59</v>
+        <v>3</v>
       </c>
       <c r="C5" t="s">
         <v>0</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="E5" t="s">
         <v>5</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>101</v>
+        <v>6</v>
       </c>
       <c r="G5" s="3" t="s">
         <v>98</v>
@@ -819,45 +835,45 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
-        <v>41676</v>
+        <v>41677</v>
       </c>
       <c r="B6" t="s">
-        <v>3</v>
+        <v>32</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="E6" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>101</v>
+        <v>6</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
-        <v>41674</v>
+        <v>41677</v>
       </c>
       <c r="B7" t="s">
-        <v>95</v>
+        <v>59</v>
       </c>
       <c r="C7" t="s">
         <v>0</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="E7" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="G7" s="3" t="s">
         <v>98</v>
@@ -865,71 +881,71 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
-        <v>41670</v>
+        <v>41676</v>
       </c>
       <c r="B8" t="s">
-        <v>17</v>
+        <v>3</v>
       </c>
       <c r="C8" t="s">
         <v>4</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>18</v>
+        <v>102</v>
       </c>
       <c r="E8" t="s">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>20</v>
+        <v>101</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>94</v>
+        <v>103</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
-        <v>41666</v>
+        <v>41674</v>
       </c>
       <c r="B9" t="s">
-        <v>3</v>
+        <v>95</v>
       </c>
       <c r="C9" t="s">
         <v>0</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>21</v>
+        <v>96</v>
       </c>
       <c r="E9" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>71</v>
+        <v>97</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
-        <v>41666</v>
+        <v>41670</v>
       </c>
       <c r="B10" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="C10" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="E10" t="s">
-        <v>1</v>
+        <v>19</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -937,22 +953,22 @@
         <v>41666</v>
       </c>
       <c r="B11" t="s">
-        <v>24</v>
+        <v>3</v>
       </c>
       <c r="C11" t="s">
         <v>0</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="E11" t="s">
-        <v>26</v>
+        <v>5</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>27</v>
+        <v>71</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -960,68 +976,68 @@
         <v>41666</v>
       </c>
       <c r="B12" t="s">
-        <v>28</v>
+        <v>2</v>
       </c>
       <c r="C12" t="s">
         <v>0</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="E12" t="s">
         <v>1</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
-        <v>41660</v>
+        <v>41666</v>
       </c>
       <c r="B13" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="C13" t="s">
         <v>0</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="E13" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>9</v>
+        <v>27</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
-        <v>41660</v>
+        <v>41666</v>
       </c>
       <c r="B14" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C14" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="E14" t="s">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>6</v>
+        <v>30</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -1029,188 +1045,188 @@
         <v>41660</v>
       </c>
       <c r="B15" t="s">
-        <v>34</v>
+        <v>11</v>
       </c>
       <c r="C15" t="s">
         <v>0</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="E15" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>36</v>
+        <v>9</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
-        <v>41659</v>
+        <v>41660</v>
       </c>
       <c r="B16" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="C16" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="E16" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>39</v>
+        <v>6</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
-        <v>41655</v>
+        <v>41660</v>
       </c>
       <c r="B17" t="s">
-        <v>2</v>
+        <v>34</v>
       </c>
       <c r="C17" t="s">
         <v>0</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="E17" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
-        <v>41655</v>
+        <v>41659</v>
       </c>
       <c r="B18" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="C18" t="s">
         <v>0</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="E18" t="s">
-        <v>44</v>
+        <v>1</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>6</v>
+        <v>39</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
-        <v>41652</v>
+        <v>41655</v>
       </c>
       <c r="B19" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C19" t="s">
         <v>0</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="E19" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
-        <v>41649</v>
+        <v>41655</v>
       </c>
       <c r="B20" t="s">
-        <v>3</v>
+        <v>42</v>
       </c>
       <c r="C20" t="s">
         <v>0</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>16</v>
+        <v>43</v>
       </c>
       <c r="E20" t="s">
-        <v>5</v>
+        <v>44</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
-        <v>41648</v>
+        <v>41652</v>
       </c>
       <c r="B21" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C21" t="s">
         <v>0</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E21" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
-        <v>41648</v>
+        <v>41649</v>
       </c>
       <c r="B22" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C22" t="s">
         <v>0</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>49</v>
+        <v>16</v>
       </c>
       <c r="E22" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
-        <v>41647</v>
+        <v>41648</v>
       </c>
       <c r="B23" t="s">
         <v>2</v>
@@ -1219,62 +1235,62 @@
         <v>0</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="E23" t="s">
         <v>1</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
-        <v>41646</v>
+        <v>41648</v>
       </c>
       <c r="B24" t="s">
-        <v>52</v>
+        <v>7</v>
       </c>
       <c r="C24" t="s">
         <v>0</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="E24" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
-        <v>41646</v>
+        <v>41647</v>
       </c>
       <c r="B25" t="s">
-        <v>54</v>
+        <v>2</v>
       </c>
       <c r="C25" t="s">
         <v>0</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="E25" t="s">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>14</v>
+        <v>51</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
@@ -1282,22 +1298,22 @@
         <v>41646</v>
       </c>
       <c r="B26" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C26" t="s">
         <v>0</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="E26" t="s">
         <v>12</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>58</v>
+        <v>13</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
@@ -1305,98 +1321,138 @@
         <v>41646</v>
       </c>
       <c r="B27" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="C27" t="s">
         <v>0</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="E27" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>61</v>
+        <v>14</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
-        <v>41645</v>
+        <v>41646</v>
       </c>
       <c r="B28" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="C28" t="s">
         <v>0</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="E28" t="s">
-        <v>64</v>
+        <v>12</v>
       </c>
       <c r="F28" s="3" t="s">
-        <v>9</v>
+        <v>58</v>
       </c>
       <c r="G28" s="3" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
-        <v>41642</v>
+        <v>41646</v>
       </c>
       <c r="B29" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="C29" t="s">
         <v>0</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="E29" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="G29" s="3" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
+        <v>41645</v>
+      </c>
+      <c r="B30" t="s">
+        <v>62</v>
+      </c>
+      <c r="C30" t="s">
+        <v>0</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="E30" t="s">
+        <v>64</v>
+      </c>
+      <c r="F30" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G30" s="3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" s="1">
+        <v>41642</v>
+      </c>
+      <c r="B31" t="s">
+        <v>65</v>
+      </c>
+      <c r="C31" t="s">
+        <v>0</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="E31" t="s">
+        <v>10</v>
+      </c>
+      <c r="F31" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="G31" s="3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" s="1">
         <v>41641</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B32" t="s">
         <v>68</v>
       </c>
-      <c r="C30" t="s">
-        <v>0</v>
-      </c>
-      <c r="D30" s="2" t="s">
+      <c r="C32" t="s">
+        <v>0</v>
+      </c>
+      <c r="D32" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="E30" t="s">
+      <c r="E32" t="s">
         <v>1</v>
       </c>
-      <c r="F30" s="3" t="s">
+      <c r="F32" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="G30" s="3" t="s">
+      <c r="G32" s="3" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" s="1"/>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="1"/>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" s="1"/>
@@ -1406,6 +1462,12 @@
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" s="1"/>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Actualizando datos modelo MOVIMIENTOS
</commit_message>
<xml_diff>
--- a/backup/cuenta_2200555126.xlsx
+++ b/backup/cuenta_2200555126.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="132">
   <si>
     <t>D</t>
   </si>
@@ -375,6 +375,51 @@
   </si>
   <si>
     <t>1961.71</t>
+  </si>
+  <si>
+    <t>CONSUMO VISA NA KFC K104</t>
+  </si>
+  <si>
+    <t>0004085602</t>
+  </si>
+  <si>
+    <t>10.60  </t>
+  </si>
+  <si>
+    <t>0004018676</t>
+  </si>
+  <si>
+    <t>83.32  </t>
+  </si>
+  <si>
+    <t>0000948985</t>
+  </si>
+  <si>
+    <t>1.53  </t>
+  </si>
+  <si>
+    <t>DEP CNB-1501119901001</t>
+  </si>
+  <si>
+    <t>0004766633</t>
+  </si>
+  <si>
+    <t>0004751756</t>
+  </si>
+  <si>
+    <t>1943.95</t>
+  </si>
+  <si>
+    <t>1993.95</t>
+  </si>
+  <si>
+    <t>1995.48</t>
+  </si>
+  <si>
+    <t>1912.16</t>
+  </si>
+  <si>
+    <t>1901.56</t>
   </si>
 </sst>
 </file>
@@ -697,10 +742,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H37"/>
+  <dimension ref="A1:H42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H1" sqref="H1:H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -712,762 +757,889 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1">
-        <v>41690</v>
+        <v>41703</v>
       </c>
       <c r="B1" t="s">
-        <v>3</v>
+        <v>117</v>
       </c>
       <c r="C1" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="E1" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>112</v>
+        <v>131</v>
       </c>
       <c r="H1" t="str">
-        <f ca="1">CONCATENATE("array('mo_fecha' =&gt; new \DateTime('",TEXT(A1,"yyyy-mm-dd"),"'), 'mo_concepto' =&gt; '",B1,"', 'mo_tipo' =&gt; '",C1,"', 'mo_documento' =&gt; '",D1,"', 'mo_oficina' =&gt; '",E1,"', 'mo_monto' =&gt; ",TRIM(F1),", 'mo_saldo' =&gt; ",G1,", 'mo_fecha_crea' =&gt; new \DateTime('",TEXT(NOW(),"yyyy-mm-dd H:m:s"),"'), 'mo_quien_crea' =&gt; 1, 'mo_fecha_modifica' =&gt; NULL, 'mo_quien_modifica' =&gt; NULL, 'mo_borrado_logico' =&gt; false),")</f>
-        <v>array('mo_fecha' =&gt; new \DateTime('2014-02-20'), 'mo_concepto' =&gt; '  TRANSFERENCIA INTERNET', 'mo_tipo' =&gt; 'D', 'mo_documento' =&gt; '0003049433', 'mo_oficina' =&gt; 'AG. NORTE', 'mo_monto' =&gt; 67.76  , 'mo_saldo' =&gt; 1893.95, 'mo_fecha_crea' =&gt; new \DateTime('2014-02-20 13:34:52'), 'mo_quien_crea' =&gt; 1, 'mo_fecha_modifica' =&gt; NULL, 'mo_quien_modifica' =&gt; NULL, 'mo_borrado_logico' =&gt; false),</v>
+        <f t="shared" ref="H1:H5" ca="1" si="0">CONCATENATE("array('mo_fecha' =&gt; new \DateTime('",TEXT(A1,"yyyy-mm-dd"),"'), 'mo_concepto' =&gt; '",B1,"', 'mo_tipo' =&gt; '",C1,"', 'mo_documento' =&gt; '",D1,"', 'mo_oficina' =&gt; '",E1,"', 'mo_monto' =&gt; ",TRIM(F1),", 'mo_saldo' =&gt; ",G1,", 'mo_fecha_crea' =&gt; new \DateTime('",TEXT(NOW(),"yyyy-mm-dd H:m:s"),"'), 'mo_quien_crea' =&gt; 1, 'mo_fecha_modifica' =&gt; NULL, 'mo_quien_modifica' =&gt; NULL, 'mo_borrado_logico' =&gt; false),")</f>
+        <v>array('mo_fecha' =&gt; new \DateTime('2014-03-05'), 'mo_concepto' =&gt; 'CONSUMO VISA NA KFC K104', 'mo_tipo' =&gt; 'D', 'mo_documento' =&gt; '0004085602', 'mo_oficina' =&gt; 'INSTITUCIONAL SS.CC.', 'mo_monto' =&gt; 10.60  , 'mo_saldo' =&gt; 1901.56, 'mo_fecha_crea' =&gt; new \DateTime('2014-03-01 21:38:22'), 'mo_quien_crea' =&gt; 1, 'mo_fecha_modifica' =&gt; NULL, 'mo_quien_modifica' =&gt; NULL, 'mo_borrado_logico' =&gt; false),</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>41690</v>
+        <v>41703</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>115</v>
+        <v>120</v>
       </c>
       <c r="E2" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>114</v>
+        <v>121</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>116</v>
+        <v>130</v>
       </c>
       <c r="H2" t="str">
-        <f ca="1">CONCATENATE("array('mo_fecha' =&gt; new \DateTime('",TEXT(A2,"yyyy-mm-dd"),"'), 'mo_concepto' =&gt; '",B2,"', 'mo_tipo' =&gt; '",C2,"', 'mo_documento' =&gt; '",D2,"', 'mo_oficina' =&gt; '",E2,"', 'mo_monto' =&gt; ",TRIM(F2),", 'mo_saldo' =&gt; ",G2,", 'mo_fecha_crea' =&gt; new \DateTime('",TEXT(NOW(),"yyyy-mm-dd H:m:s"),"'), 'mo_quien_crea' =&gt; 1, 'mo_fecha_modifica' =&gt; NULL, 'mo_quien_modifica' =&gt; NULL, 'mo_borrado_logico' =&gt; false),")</f>
-        <v>array('mo_fecha' =&gt; new \DateTime('2014-02-20'), 'mo_concepto' =&gt; '  TRANSFERENCIA INTERNET', 'mo_tipo' =&gt; 'C', 'mo_documento' =&gt; '0002989186', 'mo_oficina' =&gt; 'AG. NORTE', 'mo_monto' =&gt; 67.76  , 'mo_saldo' =&gt; 1961.71, 'mo_fecha_crea' =&gt; new \DateTime('2014-02-20 13:34:52'), 'mo_quien_crea' =&gt; 1, 'mo_fecha_modifica' =&gt; NULL, 'mo_quien_modifica' =&gt; NULL, 'mo_borrado_logico' =&gt; false),</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>array('mo_fecha' =&gt; new \DateTime('2014-03-05'), 'mo_concepto' =&gt; 'CONSUMO DATA AKI MOLINEROS 161', 'mo_tipo' =&gt; 'D', 'mo_documento' =&gt; '0004018676', 'mo_oficina' =&gt; 'INSTITUCIONAL SS.CC.', 'mo_monto' =&gt; 83.32  , 'mo_saldo' =&gt; 1912.16, 'mo_fecha_crea' =&gt; new \DateTime('2014-03-01 21:38:22'), 'mo_quien_crea' =&gt; 1, 'mo_fecha_modifica' =&gt; NULL, 'mo_quien_modifica' =&gt; NULL, 'mo_borrado_logico' =&gt; false),</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>41682</v>
+        <v>41698</v>
       </c>
       <c r="B3" t="s">
-        <v>106</v>
+        <v>17</v>
       </c>
       <c r="C3" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>107</v>
+        <v>122</v>
       </c>
       <c r="E3" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>108</v>
+        <v>123</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>112</v>
+        <v>129</v>
+      </c>
+      <c r="H3" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>array('mo_fecha' =&gt; new \DateTime('2014-02-28'), 'mo_concepto' =&gt; 'INTERES A SU FAVOR', 'mo_tipo' =&gt; 'C', 'mo_documento' =&gt; '0000948985', 'mo_oficina' =&gt; 'AGENCIA PARA PROCESOS BATCH', 'mo_monto' =&gt; 1.53  , 'mo_saldo' =&gt; 1995.48, 'mo_fecha_crea' =&gt; new \DateTime('2014-03-01 21:38:22'), 'mo_quien_crea' =&gt; 1, 'mo_fecha_modifica' =&gt; NULL, 'mo_quien_modifica' =&gt; NULL, 'mo_borrado_logico' =&gt; false),</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
-        <v>41680</v>
+        <v>41691</v>
       </c>
       <c r="B4" t="s">
-        <v>32</v>
+        <v>124</v>
       </c>
       <c r="C4" t="s">
         <v>4</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>109</v>
+        <v>125</v>
       </c>
       <c r="E4" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>110</v>
+        <v>67</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>111</v>
+        <v>128</v>
+      </c>
+      <c r="H4" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>array('mo_fecha' =&gt; new \DateTime('2014-02-21'), 'mo_concepto' =&gt; 'DEP CNB-1501119901001', 'mo_tipo' =&gt; 'C', 'mo_documento' =&gt; '0004766633', 'mo_oficina' =&gt; 'AG. NORTE', 'mo_monto' =&gt; 50.00  , 'mo_saldo' =&gt; 1993.95, 'mo_fecha_crea' =&gt; new \DateTime('2014-03-01 21:38:22'), 'mo_quien_crea' =&gt; 1, 'mo_fecha_modifica' =&gt; NULL, 'mo_quien_modifica' =&gt; NULL, 'mo_borrado_logico' =&gt; false),</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
-        <v>41680</v>
+        <v>41691</v>
       </c>
       <c r="B5" t="s">
-        <v>3</v>
+        <v>124</v>
       </c>
       <c r="C5" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>105</v>
+        <v>126</v>
       </c>
       <c r="E5" t="s">
         <v>5</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>6</v>
+        <v>67</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>98</v>
+        <v>127</v>
+      </c>
+      <c r="H5" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>array('mo_fecha' =&gt; new \DateTime('2014-02-21'), 'mo_concepto' =&gt; 'DEP CNB-1501119901001', 'mo_tipo' =&gt; 'C', 'mo_documento' =&gt; '0004751756', 'mo_oficina' =&gt; 'AG. NORTE', 'mo_monto' =&gt; 50.00  , 'mo_saldo' =&gt; 1943.95, 'mo_fecha_crea' =&gt; new \DateTime('2014-03-01 21:38:22'), 'mo_quien_crea' =&gt; 1, 'mo_fecha_modifica' =&gt; NULL, 'mo_quien_modifica' =&gt; NULL, 'mo_borrado_logico' =&gt; false),</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
-        <v>41677</v>
+        <v>41690</v>
       </c>
       <c r="B6" t="s">
-        <v>32</v>
+        <v>3</v>
       </c>
       <c r="C6" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>99</v>
+        <v>113</v>
       </c>
       <c r="E6" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>6</v>
+        <v>114</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>104</v>
+        <v>112</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
-        <v>41677</v>
+        <v>41690</v>
       </c>
       <c r="B7" t="s">
-        <v>59</v>
+        <v>3</v>
       </c>
       <c r="C7" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>100</v>
+        <v>115</v>
       </c>
       <c r="E7" t="s">
         <v>5</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>98</v>
+        <v>116</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
-        <v>41676</v>
+        <v>41682</v>
       </c>
       <c r="B8" t="s">
-        <v>3</v>
+        <v>106</v>
       </c>
       <c r="C8" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>102</v>
+        <v>107</v>
       </c>
       <c r="E8" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>101</v>
+        <v>108</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>103</v>
+        <v>112</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
-        <v>41674</v>
+        <v>41680</v>
       </c>
       <c r="B9" t="s">
-        <v>95</v>
+        <v>32</v>
       </c>
       <c r="C9" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>96</v>
+        <v>109</v>
       </c>
       <c r="E9" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>97</v>
+        <v>110</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>98</v>
+        <v>111</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
-        <v>41670</v>
+        <v>41680</v>
       </c>
       <c r="B10" t="s">
-        <v>17</v>
+        <v>3</v>
       </c>
       <c r="C10" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>18</v>
+        <v>105</v>
       </c>
       <c r="E10" t="s">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
-        <v>41666</v>
+        <v>41677</v>
       </c>
       <c r="B11" t="s">
-        <v>3</v>
+        <v>32</v>
       </c>
       <c r="C11" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>21</v>
+        <v>99</v>
       </c>
       <c r="E11" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>71</v>
+        <v>6</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
-        <v>41666</v>
+        <v>41677</v>
       </c>
       <c r="B12" t="s">
-        <v>2</v>
+        <v>59</v>
       </c>
       <c r="C12" t="s">
         <v>0</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>22</v>
+        <v>100</v>
       </c>
       <c r="E12" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>23</v>
+        <v>101</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
-        <v>41666</v>
+        <v>41676</v>
       </c>
       <c r="B13" t="s">
-        <v>24</v>
+        <v>3</v>
       </c>
       <c r="C13" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>25</v>
+        <v>102</v>
       </c>
       <c r="E13" t="s">
-        <v>26</v>
+        <v>5</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>27</v>
+        <v>101</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>91</v>
+        <v>103</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
-        <v>41666</v>
+        <v>41674</v>
       </c>
       <c r="B14" t="s">
-        <v>28</v>
+        <v>95</v>
       </c>
       <c r="C14" t="s">
         <v>0</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>29</v>
+        <v>96</v>
       </c>
       <c r="E14" t="s">
         <v>1</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>30</v>
+        <v>97</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>90</v>
+        <v>98</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
-        <v>41660</v>
+        <v>41670</v>
       </c>
       <c r="B15" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="C15" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>31</v>
+        <v>18</v>
       </c>
       <c r="E15" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
-        <v>41660</v>
+        <v>41666</v>
       </c>
       <c r="B16" t="s">
-        <v>32</v>
+        <v>3</v>
       </c>
       <c r="C16" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>33</v>
+        <v>21</v>
       </c>
       <c r="E16" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>6</v>
+        <v>71</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
-        <v>41660</v>
+        <v>41666</v>
       </c>
       <c r="B17" t="s">
-        <v>34</v>
+        <v>2</v>
       </c>
       <c r="C17" t="s">
         <v>0</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>35</v>
+        <v>22</v>
       </c>
       <c r="E17" t="s">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>36</v>
+        <v>23</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
-        <v>41659</v>
+        <v>41666</v>
       </c>
       <c r="B18" t="s">
-        <v>37</v>
+        <v>24</v>
       </c>
       <c r="C18" t="s">
         <v>0</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
       <c r="E18" t="s">
-        <v>1</v>
+        <v>26</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
-        <v>41655</v>
+        <v>41666</v>
       </c>
       <c r="B19" t="s">
-        <v>2</v>
+        <v>28</v>
       </c>
       <c r="C19" t="s">
         <v>0</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>40</v>
+        <v>29</v>
       </c>
       <c r="E19" t="s">
         <v>1</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
-        <v>41655</v>
+        <v>41660</v>
       </c>
       <c r="B20" t="s">
-        <v>42</v>
+        <v>11</v>
       </c>
       <c r="C20" t="s">
         <v>0</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="E20" t="s">
-        <v>44</v>
+        <v>8</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
-        <v>41652</v>
+        <v>41660</v>
       </c>
       <c r="B21" t="s">
-        <v>3</v>
+        <v>32</v>
       </c>
       <c r="C21" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="E21" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>46</v>
+        <v>6</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
-        <v>41649</v>
+        <v>41660</v>
       </c>
       <c r="B22" t="s">
-        <v>3</v>
+        <v>34</v>
       </c>
       <c r="C22" t="s">
         <v>0</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>16</v>
+        <v>35</v>
       </c>
       <c r="E22" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>15</v>
+        <v>36</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
-        <v>41648</v>
+        <v>41659</v>
       </c>
       <c r="B23" t="s">
-        <v>2</v>
+        <v>37</v>
       </c>
       <c r="C23" t="s">
         <v>0</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="E23" t="s">
         <v>1</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
-        <v>41648</v>
+        <v>41655</v>
       </c>
       <c r="B24" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="C24" t="s">
         <v>0</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="E24" t="s">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>9</v>
+        <v>41</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
-        <v>41647</v>
+        <v>41655</v>
       </c>
       <c r="B25" t="s">
-        <v>2</v>
+        <v>42</v>
       </c>
       <c r="C25" t="s">
         <v>0</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="E25" t="s">
-        <v>1</v>
+        <v>44</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>51</v>
+        <v>6</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
-        <v>41646</v>
+        <v>41652</v>
       </c>
       <c r="B26" t="s">
-        <v>52</v>
+        <v>3</v>
       </c>
       <c r="C26" t="s">
         <v>0</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="E26" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>13</v>
+        <v>46</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
-        <v>41646</v>
+        <v>41649</v>
       </c>
       <c r="B27" t="s">
-        <v>54</v>
+        <v>3</v>
       </c>
       <c r="C27" t="s">
         <v>0</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>55</v>
+        <v>16</v>
       </c>
       <c r="E27" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
-        <v>41646</v>
+        <v>41648</v>
       </c>
       <c r="B28" t="s">
-        <v>56</v>
+        <v>2</v>
       </c>
       <c r="C28" t="s">
         <v>0</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="E28" t="s">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="F28" s="3" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="G28" s="3" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
-        <v>41646</v>
+        <v>41648</v>
       </c>
       <c r="B29" t="s">
-        <v>59</v>
+        <v>7</v>
       </c>
       <c r="C29" t="s">
         <v>0</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>60</v>
+        <v>49</v>
       </c>
       <c r="E29" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>61</v>
+        <v>9</v>
       </c>
       <c r="G29" s="3" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
-        <v>41645</v>
+        <v>41647</v>
       </c>
       <c r="B30" t="s">
-        <v>62</v>
+        <v>2</v>
       </c>
       <c r="C30" t="s">
         <v>0</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>63</v>
+        <v>50</v>
       </c>
       <c r="E30" t="s">
-        <v>64</v>
+        <v>1</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>9</v>
+        <v>51</v>
       </c>
       <c r="G30" s="3" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
-        <v>41642</v>
+        <v>41646</v>
       </c>
       <c r="B31" t="s">
-        <v>65</v>
+        <v>52</v>
       </c>
       <c r="C31" t="s">
         <v>0</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>66</v>
+        <v>53</v>
       </c>
       <c r="E31" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>67</v>
+        <v>13</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
+        <v>41646</v>
+      </c>
+      <c r="B32" t="s">
+        <v>54</v>
+      </c>
+      <c r="C32" t="s">
+        <v>0</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="E32" t="s">
+        <v>12</v>
+      </c>
+      <c r="F32" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G32" s="3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" s="1">
+        <v>41646</v>
+      </c>
+      <c r="B33" t="s">
+        <v>56</v>
+      </c>
+      <c r="C33" t="s">
+        <v>0</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="E33" t="s">
+        <v>12</v>
+      </c>
+      <c r="F33" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="G33" s="3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" s="1">
+        <v>41646</v>
+      </c>
+      <c r="B34" t="s">
+        <v>59</v>
+      </c>
+      <c r="C34" t="s">
+        <v>0</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="E34" t="s">
+        <v>5</v>
+      </c>
+      <c r="F34" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="G34" s="3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" s="1">
+        <v>41645</v>
+      </c>
+      <c r="B35" t="s">
+        <v>62</v>
+      </c>
+      <c r="C35" t="s">
+        <v>0</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="E35" t="s">
+        <v>64</v>
+      </c>
+      <c r="F35" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G35" s="3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36" s="1">
+        <v>41642</v>
+      </c>
+      <c r="B36" t="s">
+        <v>65</v>
+      </c>
+      <c r="C36" t="s">
+        <v>0</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="E36" t="s">
+        <v>10</v>
+      </c>
+      <c r="F36" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="G36" s="3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" s="1">
         <v>41641</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B37" t="s">
         <v>68</v>
       </c>
-      <c r="C32" t="s">
-        <v>0</v>
-      </c>
-      <c r="D32" s="2" t="s">
+      <c r="C37" t="s">
+        <v>0</v>
+      </c>
+      <c r="D37" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="E32" t="s">
+      <c r="E37" t="s">
         <v>1</v>
       </c>
-      <c r="F32" s="3" t="s">
+      <c r="F37" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="G32" s="3" t="s">
+      <c r="G37" s="3" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A33" s="1"/>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A34" s="1"/>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A35" s="1"/>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A36" s="1"/>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A37" s="1"/>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38" s="1"/>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39" s="1"/>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A40" s="1"/>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A41" s="1"/>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A42" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Personalizando clase individual para paginador
</commit_message>
<xml_diff>
--- a/backup/cuenta_2200555126.xlsx
+++ b/backup/cuenta_2200555126.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="135">
   <si>
     <t>D</t>
   </si>
@@ -420,6 +420,15 @@
   </si>
   <si>
     <t>1901.56</t>
+  </si>
+  <si>
+    <t>0016349162</t>
+  </si>
+  <si>
+    <t>280.95  </t>
+  </si>
+  <si>
+    <t>2182.51</t>
   </si>
 </sst>
 </file>
@@ -742,10 +751,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H42"/>
+  <dimension ref="A1:H43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1:H5"/>
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -760,26 +769,26 @@
         <v>41703</v>
       </c>
       <c r="B1" t="s">
-        <v>117</v>
+        <v>3</v>
       </c>
       <c r="C1" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>118</v>
+        <v>132</v>
       </c>
       <c r="E1" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>119</v>
+        <v>133</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="H1" t="str">
-        <f t="shared" ref="H1:H5" ca="1" si="0">CONCATENATE("array('mo_fecha' =&gt; new \DateTime('",TEXT(A1,"yyyy-mm-dd"),"'), 'mo_concepto' =&gt; '",B1,"', 'mo_tipo' =&gt; '",C1,"', 'mo_documento' =&gt; '",D1,"', 'mo_oficina' =&gt; '",E1,"', 'mo_monto' =&gt; ",TRIM(F1),", 'mo_saldo' =&gt; ",G1,", 'mo_fecha_crea' =&gt; new \DateTime('",TEXT(NOW(),"yyyy-mm-dd H:m:s"),"'), 'mo_quien_crea' =&gt; 1, 'mo_fecha_modifica' =&gt; NULL, 'mo_quien_modifica' =&gt; NULL, 'mo_borrado_logico' =&gt; false),")</f>
-        <v>array('mo_fecha' =&gt; new \DateTime('2014-03-05'), 'mo_concepto' =&gt; 'CONSUMO VISA NA KFC K104', 'mo_tipo' =&gt; 'D', 'mo_documento' =&gt; '0004085602', 'mo_oficina' =&gt; 'INSTITUCIONAL SS.CC.', 'mo_monto' =&gt; 10.60  , 'mo_saldo' =&gt; 1901.56, 'mo_fecha_crea' =&gt; new \DateTime('2014-03-01 21:38:22'), 'mo_quien_crea' =&gt; 1, 'mo_fecha_modifica' =&gt; NULL, 'mo_quien_modifica' =&gt; NULL, 'mo_borrado_logico' =&gt; false),</v>
+        <f t="shared" ref="H1" ca="1" si="0">CONCATENATE("array('mo_fecha' =&gt; new \DateTime('",TEXT(A1,"yyyy-mm-dd"),"'), 'mo_concepto' =&gt; '",B1,"', 'mo_tipo' =&gt; '",C1,"', 'mo_documento' =&gt; '",D1,"', 'mo_oficina' =&gt; '",E1,"', 'mo_monto' =&gt; ",TRIM(F1),", 'mo_saldo' =&gt; ",G1,", 'mo_fecha_crea' =&gt; new \DateTime('",TEXT(NOW(),"yyyy-mm-dd H:m:s"),"'), 'mo_quien_crea' =&gt; 1, 'mo_fecha_modifica' =&gt; NULL, 'mo_quien_modifica' =&gt; NULL, 'mo_borrado_logico' =&gt; false),")</f>
+        <v>array('mo_fecha' =&gt; new \DateTime('2014-03-05'), 'mo_concepto' =&gt; '  TRANSFERENCIA INTERNET', 'mo_tipo' =&gt; 'C', 'mo_documento' =&gt; '0016349162', 'mo_oficina' =&gt; 'AG. NORTE', 'mo_monto' =&gt; 280.95  , 'mo_saldo' =&gt; 2182.51, 'mo_fecha_crea' =&gt; new \DateTime('2014-03-05 20:16:55'), 'mo_quien_crea' =&gt; 1, 'mo_fecha_modifica' =&gt; NULL, 'mo_quien_modifica' =&gt; NULL, 'mo_borrado_logico' =&gt; false),</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -787,80 +796,68 @@
         <v>41703</v>
       </c>
       <c r="B2" t="s">
-        <v>2</v>
+        <v>117</v>
       </c>
       <c r="C2" t="s">
         <v>0</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="E2" t="s">
         <v>1</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="H2" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>array('mo_fecha' =&gt; new \DateTime('2014-03-05'), 'mo_concepto' =&gt; 'CONSUMO DATA AKI MOLINEROS 161', 'mo_tipo' =&gt; 'D', 'mo_documento' =&gt; '0004018676', 'mo_oficina' =&gt; 'INSTITUCIONAL SS.CC.', 'mo_monto' =&gt; 83.32  , 'mo_saldo' =&gt; 1912.16, 'mo_fecha_crea' =&gt; new \DateTime('2014-03-01 21:38:22'), 'mo_quien_crea' =&gt; 1, 'mo_fecha_modifica' =&gt; NULL, 'mo_quien_modifica' =&gt; NULL, 'mo_borrado_logico' =&gt; false),</v>
+        <v>131</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>41698</v>
+        <v>41703</v>
       </c>
       <c r="B3" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="E3" t="s">
-        <v>19</v>
+        <v>1</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>129</v>
-      </c>
-      <c r="H3" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>array('mo_fecha' =&gt; new \DateTime('2014-02-28'), 'mo_concepto' =&gt; 'INTERES A SU FAVOR', 'mo_tipo' =&gt; 'C', 'mo_documento' =&gt; '0000948985', 'mo_oficina' =&gt; 'AGENCIA PARA PROCESOS BATCH', 'mo_monto' =&gt; 1.53  , 'mo_saldo' =&gt; 1995.48, 'mo_fecha_crea' =&gt; new \DateTime('2014-03-01 21:38:22'), 'mo_quien_crea' =&gt; 1, 'mo_fecha_modifica' =&gt; NULL, 'mo_quien_modifica' =&gt; NULL, 'mo_borrado_logico' =&gt; false),</v>
+        <v>130</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
-        <v>41691</v>
+        <v>41698</v>
       </c>
       <c r="B4" t="s">
-        <v>124</v>
+        <v>17</v>
       </c>
       <c r="C4" t="s">
         <v>4</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="E4" t="s">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>67</v>
+        <v>123</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="H4" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>array('mo_fecha' =&gt; new \DateTime('2014-02-21'), 'mo_concepto' =&gt; 'DEP CNB-1501119901001', 'mo_tipo' =&gt; 'C', 'mo_documento' =&gt; '0004766633', 'mo_oficina' =&gt; 'AG. NORTE', 'mo_monto' =&gt; 50.00  , 'mo_saldo' =&gt; 1993.95, 'mo_fecha_crea' =&gt; new \DateTime('2014-03-01 21:38:22'), 'mo_quien_crea' =&gt; 1, 'mo_fecha_modifica' =&gt; NULL, 'mo_quien_modifica' =&gt; NULL, 'mo_borrado_logico' =&gt; false),</v>
+        <v>129</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -874,7 +871,7 @@
         <v>4</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E5" t="s">
         <v>5</v>
@@ -883,34 +880,30 @@
         <v>67</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>127</v>
-      </c>
-      <c r="H5" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>array('mo_fecha' =&gt; new \DateTime('2014-02-21'), 'mo_concepto' =&gt; 'DEP CNB-1501119901001', 'mo_tipo' =&gt; 'C', 'mo_documento' =&gt; '0004751756', 'mo_oficina' =&gt; 'AG. NORTE', 'mo_monto' =&gt; 50.00  , 'mo_saldo' =&gt; 1943.95, 'mo_fecha_crea' =&gt; new \DateTime('2014-03-01 21:38:22'), 'mo_quien_crea' =&gt; 1, 'mo_fecha_modifica' =&gt; NULL, 'mo_quien_modifica' =&gt; NULL, 'mo_borrado_logico' =&gt; false),</v>
+        <v>128</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
-        <v>41690</v>
+        <v>41691</v>
       </c>
       <c r="B6" t="s">
-        <v>3</v>
+        <v>124</v>
       </c>
       <c r="C6" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>113</v>
+        <v>126</v>
       </c>
       <c r="E6" t="s">
         <v>5</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>114</v>
+        <v>67</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>112</v>
+        <v>127</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -921,10 +914,10 @@
         <v>3</v>
       </c>
       <c r="C7" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="E7" t="s">
         <v>5</v>
@@ -933,53 +926,53 @@
         <v>114</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
-        <v>41682</v>
+        <v>41690</v>
       </c>
       <c r="B8" t="s">
-        <v>106</v>
+        <v>3</v>
       </c>
       <c r="C8" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>107</v>
+        <v>115</v>
       </c>
       <c r="E8" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>108</v>
+        <v>114</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
-        <v>41680</v>
+        <v>41682</v>
       </c>
       <c r="B9" t="s">
-        <v>32</v>
+        <v>106</v>
       </c>
       <c r="C9" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="E9" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -987,45 +980,45 @@
         <v>41680</v>
       </c>
       <c r="B10" t="s">
-        <v>3</v>
+        <v>32</v>
       </c>
       <c r="C10" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="E10" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>6</v>
+        <v>110</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>98</v>
+        <v>111</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
-        <v>41677</v>
+        <v>41680</v>
       </c>
       <c r="B11" t="s">
-        <v>32</v>
+        <v>3</v>
       </c>
       <c r="C11" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>99</v>
+        <v>105</v>
       </c>
       <c r="E11" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="F11" s="3" t="s">
         <v>6</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -1033,36 +1026,36 @@
         <v>41677</v>
       </c>
       <c r="B12" t="s">
-        <v>59</v>
+        <v>32</v>
       </c>
       <c r="C12" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E12" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>101</v>
+        <v>6</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>98</v>
+        <v>104</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
-        <v>41676</v>
+        <v>41677</v>
       </c>
       <c r="B13" t="s">
-        <v>3</v>
+        <v>59</v>
       </c>
       <c r="C13" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="E13" t="s">
         <v>5</v>
@@ -1071,76 +1064,76 @@
         <v>101</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
-        <v>41674</v>
+        <v>41676</v>
       </c>
       <c r="B14" t="s">
-        <v>95</v>
+        <v>3</v>
       </c>
       <c r="C14" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>96</v>
+        <v>102</v>
       </c>
       <c r="E14" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
-        <v>41670</v>
+        <v>41674</v>
       </c>
       <c r="B15" t="s">
-        <v>17</v>
+        <v>95</v>
       </c>
       <c r="C15" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>18</v>
+        <v>96</v>
       </c>
       <c r="E15" t="s">
-        <v>19</v>
+        <v>1</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>20</v>
+        <v>97</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
-        <v>41666</v>
+        <v>41670</v>
       </c>
       <c r="B16" t="s">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="C16" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="E16" t="s">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>71</v>
+        <v>20</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
@@ -1148,22 +1141,22 @@
         <v>41666</v>
       </c>
       <c r="B17" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C17" t="s">
         <v>0</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E17" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>23</v>
+        <v>71</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
@@ -1171,22 +1164,22 @@
         <v>41666</v>
       </c>
       <c r="B18" t="s">
-        <v>24</v>
+        <v>2</v>
       </c>
       <c r="C18" t="s">
         <v>0</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E18" t="s">
-        <v>26</v>
+        <v>1</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
@@ -1194,45 +1187,45 @@
         <v>41666</v>
       </c>
       <c r="B19" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C19" t="s">
         <v>0</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="E19" t="s">
-        <v>1</v>
+        <v>26</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
-        <v>41660</v>
+        <v>41666</v>
       </c>
       <c r="B20" t="s">
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="C20" t="s">
         <v>0</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E20" t="s">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>9</v>
+        <v>30</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
@@ -1240,22 +1233,22 @@
         <v>41660</v>
       </c>
       <c r="B21" t="s">
-        <v>32</v>
+        <v>11</v>
       </c>
       <c r="C21" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E21" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
@@ -1263,68 +1256,68 @@
         <v>41660</v>
       </c>
       <c r="B22" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C22" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E22" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>36</v>
+        <v>6</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
-        <v>41659</v>
+        <v>41660</v>
       </c>
       <c r="B23" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C23" t="s">
         <v>0</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="E23" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
-        <v>41655</v>
+        <v>41659</v>
       </c>
       <c r="B24" t="s">
-        <v>2</v>
+        <v>37</v>
       </c>
       <c r="C24" t="s">
         <v>0</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E24" t="s">
         <v>1</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
@@ -1332,50 +1325,50 @@
         <v>41655</v>
       </c>
       <c r="B25" t="s">
-        <v>42</v>
+        <v>2</v>
       </c>
       <c r="C25" t="s">
         <v>0</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="E25" t="s">
-        <v>44</v>
+        <v>1</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>6</v>
+        <v>41</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
-        <v>41652</v>
+        <v>41655</v>
       </c>
       <c r="B26" t="s">
-        <v>3</v>
+        <v>42</v>
       </c>
       <c r="C26" t="s">
         <v>0</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E26" t="s">
-        <v>5</v>
+        <v>44</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>46</v>
+        <v>6</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
-        <v>41649</v>
+        <v>41652</v>
       </c>
       <c r="B27" t="s">
         <v>3</v>
@@ -1384,39 +1377,39 @@
         <v>0</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>16</v>
+        <v>45</v>
       </c>
       <c r="E27" t="s">
         <v>5</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>15</v>
+        <v>46</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
-        <v>41648</v>
+        <v>41649</v>
       </c>
       <c r="B28" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C28" t="s">
         <v>0</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>47</v>
+        <v>16</v>
       </c>
       <c r="E28" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F28" s="3" t="s">
-        <v>48</v>
+        <v>15</v>
       </c>
       <c r="G28" s="3" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
@@ -1424,68 +1417,68 @@
         <v>41648</v>
       </c>
       <c r="B29" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="C29" t="s">
         <v>0</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E29" t="s">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>9</v>
+        <v>48</v>
       </c>
       <c r="G29" s="3" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
-        <v>41647</v>
+        <v>41648</v>
       </c>
       <c r="B30" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="C30" t="s">
         <v>0</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E30" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>51</v>
+        <v>9</v>
       </c>
       <c r="G30" s="3" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
-        <v>41646</v>
+        <v>41647</v>
       </c>
       <c r="B31" t="s">
-        <v>52</v>
+        <v>2</v>
       </c>
       <c r="C31" t="s">
         <v>0</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="E31" t="s">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>13</v>
+        <v>51</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
@@ -1493,22 +1486,22 @@
         <v>41646</v>
       </c>
       <c r="B32" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C32" t="s">
         <v>0</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E32" t="s">
         <v>12</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G32" s="3" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
@@ -1516,22 +1509,22 @@
         <v>41646</v>
       </c>
       <c r="B33" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C33" t="s">
         <v>0</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E33" t="s">
         <v>12</v>
       </c>
       <c r="F33" s="3" t="s">
-        <v>58</v>
+        <v>14</v>
       </c>
       <c r="G33" s="3" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
@@ -1539,95 +1532,115 @@
         <v>41646</v>
       </c>
       <c r="B34" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C34" t="s">
         <v>0</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E34" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="G34" s="3" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
-        <v>41645</v>
+        <v>41646</v>
       </c>
       <c r="B35" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C35" t="s">
         <v>0</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="E35" t="s">
-        <v>64</v>
+        <v>5</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>9</v>
+        <v>61</v>
       </c>
       <c r="G35" s="3" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
-        <v>41642</v>
+        <v>41645</v>
       </c>
       <c r="B36" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C36" t="s">
         <v>0</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="E36" t="s">
-        <v>10</v>
+        <v>64</v>
       </c>
       <c r="F36" s="3" t="s">
-        <v>67</v>
+        <v>9</v>
       </c>
       <c r="G36" s="3" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
+        <v>41642</v>
+      </c>
+      <c r="B37" t="s">
+        <v>65</v>
+      </c>
+      <c r="C37" t="s">
+        <v>0</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="E37" t="s">
+        <v>10</v>
+      </c>
+      <c r="F37" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="G37" s="3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38" s="1">
         <v>41641</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B38" t="s">
         <v>68</v>
       </c>
-      <c r="C37" t="s">
-        <v>0</v>
-      </c>
-      <c r="D37" s="2" t="s">
+      <c r="C38" t="s">
+        <v>0</v>
+      </c>
+      <c r="D38" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="E37" t="s">
+      <c r="E38" t="s">
         <v>1</v>
       </c>
-      <c r="F37" s="3" t="s">
+      <c r="F38" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="G37" s="3" t="s">
+      <c r="G38" s="3" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A38" s="1"/>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="1"/>
@@ -1640,6 +1653,9 @@
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="1"/>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A43" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Paginador de Symfony1 a Symfony2 implementado y funcionando
</commit_message>
<xml_diff>
--- a/backup/cuenta_2200555126.xlsx
+++ b/backup/cuenta_2200555126.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\php-projects\dml2\backup\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\xampp\htdocs\dml2\backup\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="143">
   <si>
     <t>D</t>
   </si>
@@ -441,6 +441,18 @@
   </si>
   <si>
     <t>2001.56</t>
+  </si>
+  <si>
+    <t>2200555126/0995935959</t>
+  </si>
+  <si>
+    <t>0007745172</t>
+  </si>
+  <si>
+    <t>6.00  </t>
+  </si>
+  <si>
+    <t>1995.56</t>
   </si>
 </sst>
 </file>
@@ -763,10 +775,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H45"/>
+  <dimension ref="A1:H46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1:H2"/>
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -778,70 +790,66 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1">
-        <v>41708</v>
+        <v>41712</v>
       </c>
       <c r="B1" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="C1" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="E1" t="s">
         <v>5</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>6</v>
+        <v>141</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
       <c r="H1" t="str">
-        <f t="shared" ref="H1:H2" ca="1" si="0">CONCATENATE("array('mo_fecha' =&gt; new \DateTime('",TEXT(A1,"yyyy-mm-dd"),"'), 'mo_concepto' =&gt; '",B1,"', 'mo_tipo' =&gt; '",C1,"', 'mo_documento' =&gt; '",D1,"', 'mo_oficina' =&gt; '",E1,"', 'mo_monto' =&gt; ",TRIM(F1),", 'mo_saldo' =&gt; ",G1,", 'mo_fecha_crea' =&gt; new \DateTime('",TEXT(NOW(),"yyyy-mm-dd H:m:s"),"'), 'mo_quien_crea' =&gt; 1, 'mo_fecha_modifica' =&gt; NULL, 'mo_quien_modifica' =&gt; NULL, 'mo_borrado_logico' =&gt; false),")</f>
-        <v>array('mo_fecha' =&gt; new \DateTime('2014-03-10'), 'mo_concepto' =&gt; 'DEP CNB-1500415029001', 'mo_tipo' =&gt; 'C', 'mo_documento' =&gt; '0002243295', 'mo_oficina' =&gt; 'AG. NORTE', 'mo_monto' =&gt; 100.00  , 'mo_saldo' =&gt; 2001.56, 'mo_fecha_crea' =&gt; new \DateTime('2014-03-12 20:56:42'), 'mo_quien_crea' =&gt; 1, 'mo_fecha_modifica' =&gt; NULL, 'mo_quien_modifica' =&gt; NULL, 'mo_borrado_logico' =&gt; false),</v>
+        <f t="shared" ref="H1:H3" ca="1" si="0">CONCATENATE("array('mo_fecha' =&gt; new \DateTime('",TEXT(A1,"yyyy-mm-dd"),"'), 'mo_concepto' =&gt; '",B1,"', 'mo_tipo' =&gt; '",C1,"', 'mo_documento' =&gt; '",D1,"', 'mo_oficina' =&gt; '",E1,"', 'mo_monto' =&gt; ",TRIM(F1),", 'mo_saldo' =&gt; ",G1,", 'mo_fecha_crea' =&gt; new \DateTime('",TEXT(NOW(),"yyyy-mm-dd H:m:s"),"'), 'mo_quien_crea' =&gt; 1, 'mo_fecha_modifica' =&gt; NULL, 'mo_quien_modifica' =&gt; NULL, 'mo_borrado_logico' =&gt; false),")</f>
+        <v>array('mo_fecha' =&gt; new \DateTime('2014-03-14'), 'mo_concepto' =&gt; '2200555126/0995935959', 'mo_tipo' =&gt; 'D', 'mo_documento' =&gt; '0007745172', 'mo_oficina' =&gt; 'AG. NORTE', 'mo_monto' =&gt; 6.00  , 'mo_saldo' =&gt; 1995.56, 'mo_fecha_crea' =&gt; new \DateTime('2014-03-15 10:9:14'), 'mo_quien_crea' =&gt; 1, 'mo_fecha_modifica' =&gt; NULL, 'mo_quien_modifica' =&gt; NULL, 'mo_borrado_logico' =&gt; false),</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>41705</v>
+        <v>41708</v>
       </c>
       <c r="B2" t="s">
-        <v>59</v>
+        <v>135</v>
       </c>
       <c r="C2" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E2" t="s">
         <v>5</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>133</v>
+        <v>6</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="H2" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>array('mo_fecha' =&gt; new \DateTime('2014-03-07'), 'mo_concepto' =&gt; 'PAGO PRESTAMO', 'mo_tipo' =&gt; 'D', 'mo_documento' =&gt; '0000762454', 'mo_oficina' =&gt; 'AG. NORTE', 'mo_monto' =&gt; 280.95  , 'mo_saldo' =&gt; 1901.56, 'mo_fecha_crea' =&gt; new \DateTime('2014-03-12 20:56:42'), 'mo_quien_crea' =&gt; 1, 'mo_fecha_modifica' =&gt; NULL, 'mo_quien_modifica' =&gt; NULL, 'mo_borrado_logico' =&gt; false),</v>
+        <v>138</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>41703</v>
+        <v>41705</v>
       </c>
       <c r="B3" t="s">
-        <v>3</v>
+        <v>59</v>
       </c>
       <c r="C3" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>132</v>
+        <v>137</v>
       </c>
       <c r="E3" t="s">
         <v>5</v>
@@ -850,7 +858,7 @@
         <v>133</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -858,22 +866,22 @@
         <v>41703</v>
       </c>
       <c r="B4" t="s">
-        <v>117</v>
+        <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>118</v>
+        <v>132</v>
       </c>
       <c r="E4" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>119</v>
+        <v>133</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -881,68 +889,68 @@
         <v>41703</v>
       </c>
       <c r="B5" t="s">
-        <v>2</v>
+        <v>117</v>
       </c>
       <c r="C5" t="s">
         <v>0</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="E5" t="s">
         <v>1</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
-        <v>41698</v>
+        <v>41703</v>
       </c>
       <c r="B6" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="C6" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="E6" t="s">
-        <v>19</v>
+        <v>1</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
-        <v>41691</v>
+        <v>41698</v>
       </c>
       <c r="B7" t="s">
-        <v>124</v>
+        <v>17</v>
       </c>
       <c r="C7" t="s">
         <v>4</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="E7" t="s">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>67</v>
+        <v>123</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -956,7 +964,7 @@
         <v>4</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E8" t="s">
         <v>5</v>
@@ -965,30 +973,30 @@
         <v>67</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
-        <v>41690</v>
+        <v>41691</v>
       </c>
       <c r="B9" t="s">
-        <v>3</v>
+        <v>124</v>
       </c>
       <c r="C9" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>113</v>
+        <v>126</v>
       </c>
       <c r="E9" t="s">
         <v>5</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>114</v>
+        <v>67</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>112</v>
+        <v>127</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -999,10 +1007,10 @@
         <v>3</v>
       </c>
       <c r="C10" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="E10" t="s">
         <v>5</v>
@@ -1011,53 +1019,53 @@
         <v>114</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
-        <v>41682</v>
+        <v>41690</v>
       </c>
       <c r="B11" t="s">
-        <v>106</v>
+        <v>3</v>
       </c>
       <c r="C11" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>107</v>
+        <v>115</v>
       </c>
       <c r="E11" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>108</v>
+        <v>114</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
-        <v>41680</v>
+        <v>41682</v>
       </c>
       <c r="B12" t="s">
-        <v>32</v>
+        <v>106</v>
       </c>
       <c r="C12" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="E12" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -1065,45 +1073,45 @@
         <v>41680</v>
       </c>
       <c r="B13" t="s">
-        <v>3</v>
+        <v>32</v>
       </c>
       <c r="C13" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="E13" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>6</v>
+        <v>110</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>98</v>
+        <v>111</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
-        <v>41677</v>
+        <v>41680</v>
       </c>
       <c r="B14" t="s">
-        <v>32</v>
+        <v>3</v>
       </c>
       <c r="C14" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>99</v>
+        <v>105</v>
       </c>
       <c r="E14" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="F14" s="3" t="s">
         <v>6</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -1111,36 +1119,36 @@
         <v>41677</v>
       </c>
       <c r="B15" t="s">
-        <v>59</v>
+        <v>32</v>
       </c>
       <c r="C15" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E15" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>101</v>
+        <v>6</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>98</v>
+        <v>104</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
-        <v>41676</v>
+        <v>41677</v>
       </c>
       <c r="B16" t="s">
-        <v>3</v>
+        <v>59</v>
       </c>
       <c r="C16" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="E16" t="s">
         <v>5</v>
@@ -1149,76 +1157,76 @@
         <v>101</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
-        <v>41674</v>
+        <v>41676</v>
       </c>
       <c r="B17" t="s">
-        <v>95</v>
+        <v>3</v>
       </c>
       <c r="C17" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>96</v>
+        <v>102</v>
       </c>
       <c r="E17" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
-        <v>41670</v>
+        <v>41674</v>
       </c>
       <c r="B18" t="s">
-        <v>17</v>
+        <v>95</v>
       </c>
       <c r="C18" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>18</v>
+        <v>96</v>
       </c>
       <c r="E18" t="s">
-        <v>19</v>
+        <v>1</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>20</v>
+        <v>97</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
-        <v>41666</v>
+        <v>41670</v>
       </c>
       <c r="B19" t="s">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="C19" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="E19" t="s">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>71</v>
+        <v>20</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
@@ -1226,22 +1234,22 @@
         <v>41666</v>
       </c>
       <c r="B20" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C20" t="s">
         <v>0</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E20" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>23</v>
+        <v>71</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
@@ -1249,22 +1257,22 @@
         <v>41666</v>
       </c>
       <c r="B21" t="s">
-        <v>24</v>
+        <v>2</v>
       </c>
       <c r="C21" t="s">
         <v>0</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E21" t="s">
-        <v>26</v>
+        <v>1</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
@@ -1272,45 +1280,45 @@
         <v>41666</v>
       </c>
       <c r="B22" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C22" t="s">
         <v>0</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="E22" t="s">
-        <v>1</v>
+        <v>26</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
-        <v>41660</v>
+        <v>41666</v>
       </c>
       <c r="B23" t="s">
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="C23" t="s">
         <v>0</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E23" t="s">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>9</v>
+        <v>30</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
@@ -1318,22 +1326,22 @@
         <v>41660</v>
       </c>
       <c r="B24" t="s">
-        <v>32</v>
+        <v>11</v>
       </c>
       <c r="C24" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E24" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
@@ -1341,68 +1349,68 @@
         <v>41660</v>
       </c>
       <c r="B25" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C25" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E25" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>36</v>
+        <v>6</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
-        <v>41659</v>
+        <v>41660</v>
       </c>
       <c r="B26" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C26" t="s">
         <v>0</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="E26" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
-        <v>41655</v>
+        <v>41659</v>
       </c>
       <c r="B27" t="s">
-        <v>2</v>
+        <v>37</v>
       </c>
       <c r="C27" t="s">
         <v>0</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E27" t="s">
         <v>1</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
@@ -1410,50 +1418,50 @@
         <v>41655</v>
       </c>
       <c r="B28" t="s">
-        <v>42</v>
+        <v>2</v>
       </c>
       <c r="C28" t="s">
         <v>0</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="E28" t="s">
-        <v>44</v>
+        <v>1</v>
       </c>
       <c r="F28" s="3" t="s">
-        <v>6</v>
+        <v>41</v>
       </c>
       <c r="G28" s="3" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
-        <v>41652</v>
+        <v>41655</v>
       </c>
       <c r="B29" t="s">
-        <v>3</v>
+        <v>42</v>
       </c>
       <c r="C29" t="s">
         <v>0</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E29" t="s">
-        <v>5</v>
+        <v>44</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>46</v>
+        <v>6</v>
       </c>
       <c r="G29" s="3" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
-        <v>41649</v>
+        <v>41652</v>
       </c>
       <c r="B30" t="s">
         <v>3</v>
@@ -1462,39 +1470,39 @@
         <v>0</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>16</v>
+        <v>45</v>
       </c>
       <c r="E30" t="s">
         <v>5</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>15</v>
+        <v>46</v>
       </c>
       <c r="G30" s="3" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
-        <v>41648</v>
+        <v>41649</v>
       </c>
       <c r="B31" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C31" t="s">
         <v>0</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>47</v>
+        <v>16</v>
       </c>
       <c r="E31" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>48</v>
+        <v>15</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
@@ -1502,68 +1510,68 @@
         <v>41648</v>
       </c>
       <c r="B32" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="C32" t="s">
         <v>0</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E32" t="s">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>9</v>
+        <v>48</v>
       </c>
       <c r="G32" s="3" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
-        <v>41647</v>
+        <v>41648</v>
       </c>
       <c r="B33" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="C33" t="s">
         <v>0</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E33" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="F33" s="3" t="s">
-        <v>51</v>
+        <v>9</v>
       </c>
       <c r="G33" s="3" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
-        <v>41646</v>
+        <v>41647</v>
       </c>
       <c r="B34" t="s">
-        <v>52</v>
+        <v>2</v>
       </c>
       <c r="C34" t="s">
         <v>0</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="E34" t="s">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>13</v>
+        <v>51</v>
       </c>
       <c r="G34" s="3" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
@@ -1571,22 +1579,22 @@
         <v>41646</v>
       </c>
       <c r="B35" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C35" t="s">
         <v>0</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E35" t="s">
         <v>12</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G35" s="3" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
@@ -1594,22 +1602,22 @@
         <v>41646</v>
       </c>
       <c r="B36" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C36" t="s">
         <v>0</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E36" t="s">
         <v>12</v>
       </c>
       <c r="F36" s="3" t="s">
-        <v>58</v>
+        <v>14</v>
       </c>
       <c r="G36" s="3" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
@@ -1617,95 +1625,115 @@
         <v>41646</v>
       </c>
       <c r="B37" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C37" t="s">
         <v>0</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E37" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="F37" s="3" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="G37" s="3" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
-        <v>41645</v>
+        <v>41646</v>
       </c>
       <c r="B38" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C38" t="s">
         <v>0</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="E38" t="s">
-        <v>64</v>
+        <v>5</v>
       </c>
       <c r="F38" s="3" t="s">
-        <v>9</v>
+        <v>61</v>
       </c>
       <c r="G38" s="3" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
-        <v>41642</v>
+        <v>41645</v>
       </c>
       <c r="B39" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C39" t="s">
         <v>0</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="E39" t="s">
-        <v>10</v>
+        <v>64</v>
       </c>
       <c r="F39" s="3" t="s">
-        <v>67</v>
+        <v>9</v>
       </c>
       <c r="G39" s="3" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
+        <v>41642</v>
+      </c>
+      <c r="B40" t="s">
+        <v>65</v>
+      </c>
+      <c r="C40" t="s">
+        <v>0</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="E40" t="s">
+        <v>10</v>
+      </c>
+      <c r="F40" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="G40" s="3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A41" s="1">
         <v>41641</v>
       </c>
-      <c r="B40" t="s">
+      <c r="B41" t="s">
         <v>68</v>
       </c>
-      <c r="C40" t="s">
-        <v>0</v>
-      </c>
-      <c r="D40" s="2" t="s">
+      <c r="C41" t="s">
+        <v>0</v>
+      </c>
+      <c r="D41" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="E40" t="s">
+      <c r="E41" t="s">
         <v>1</v>
       </c>
-      <c r="F40" s="3" t="s">
+      <c r="F41" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="G40" s="3" t="s">
+      <c r="G41" s="3" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A41" s="1"/>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="1"/>
@@ -1718,6 +1746,9 @@
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="1"/>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A46" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Ajax en el paginador y combo box
</commit_message>
<xml_diff>
--- a/backup/cuenta_2200555126.xlsx
+++ b/backup/cuenta_2200555126.xlsx
@@ -811,8 +811,8 @@
         <v>142</v>
       </c>
       <c r="H1" t="str">
-        <f t="shared" ref="H1:H3" ca="1" si="0">CONCATENATE("array('mo_fecha' =&gt; new \DateTime('",TEXT(A1,"yyyy-mm-dd"),"'), 'mo_concepto' =&gt; '",B1,"', 'mo_tipo' =&gt; '",C1,"', 'mo_documento' =&gt; '",D1,"', 'mo_oficina' =&gt; '",E1,"', 'mo_monto' =&gt; ",TRIM(F1),", 'mo_saldo' =&gt; ",G1,", 'mo_fecha_crea' =&gt; new \DateTime('",TEXT(NOW(),"yyyy-mm-dd H:m:s"),"'), 'mo_quien_crea' =&gt; 1, 'mo_fecha_modifica' =&gt; NULL, 'mo_quien_modifica' =&gt; NULL, 'mo_borrado_logico' =&gt; false),")</f>
-        <v>array('mo_fecha' =&gt; new \DateTime('2014-03-14'), 'mo_concepto' =&gt; '2200555126/0995935959', 'mo_tipo' =&gt; 'D', 'mo_documento' =&gt; '0007745172', 'mo_oficina' =&gt; 'AG. NORTE', 'mo_monto' =&gt; 6.00  , 'mo_saldo' =&gt; 1995.56, 'mo_fecha_crea' =&gt; new \DateTime('2014-03-15 10:9:14'), 'mo_quien_crea' =&gt; 1, 'mo_fecha_modifica' =&gt; NULL, 'mo_quien_modifica' =&gt; NULL, 'mo_borrado_logico' =&gt; false),</v>
+        <f t="shared" ref="H1" ca="1" si="0">CONCATENATE("array('mo_fecha' =&gt; new \DateTime('",TEXT(A1,"yyyy-mm-dd"),"'), 'mo_concepto' =&gt; '",B1,"', 'mo_tipo' =&gt; '",C1,"', 'mo_documento' =&gt; '",D1,"', 'mo_oficina' =&gt; '",E1,"', 'mo_monto' =&gt; ",TRIM(F1),", 'mo_saldo' =&gt; ",G1,", 'mo_fecha_crea' =&gt; new \DateTime('",TEXT(NOW(),"yyyy-mm-dd H:m:s"),"'), 'mo_quien_crea' =&gt; 1, 'mo_fecha_modifica' =&gt; NULL, 'mo_quien_modifica' =&gt; NULL, 'mo_borrado_logico' =&gt; false),")</f>
+        <v>array('mo_fecha' =&gt; new \DateTime('2014-03-14'), 'mo_concepto' =&gt; '2200555126/0995935959', 'mo_tipo' =&gt; 'D', 'mo_documento' =&gt; '0007745172', 'mo_oficina' =&gt; 'AG. NORTE', 'mo_monto' =&gt; 6.00  , 'mo_saldo' =&gt; 1995.56, 'mo_fecha_crea' =&gt; new \DateTime('2014-03-20 11:4:2'), 'mo_quien_crea' =&gt; 1, 'mo_fecha_modifica' =&gt; NULL, 'mo_quien_modifica' =&gt; NULL, 'mo_borrado_logico' =&gt; false),</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Agregando componentes adicionales al módulo Movimientos
</commit_message>
<xml_diff>
--- a/backup/cuenta_2200555126.xlsx
+++ b/backup/cuenta_2200555126.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\xampp\htdocs\dml2\backup\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\php-projects\dml2\backup\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="151">
   <si>
     <t>D</t>
   </si>
@@ -453,6 +453,30 @@
   </si>
   <si>
     <t>1995.56</t>
+  </si>
+  <si>
+    <t>0002254424</t>
+  </si>
+  <si>
+    <t>RETIRO ATM BP D/KENNEDY 3</t>
+  </si>
+  <si>
+    <t>0000653181</t>
+  </si>
+  <si>
+    <t>KENNEDY</t>
+  </si>
+  <si>
+    <t>0006095191</t>
+  </si>
+  <si>
+    <t>2095.56</t>
+  </si>
+  <si>
+    <t>2055.56</t>
+  </si>
+  <si>
+    <t>2035.56</t>
   </si>
 </sst>
 </file>
@@ -775,10 +799,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H46"/>
+  <dimension ref="A1:H49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -790,512 +814,520 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1">
-        <v>41712</v>
+        <v>41722</v>
       </c>
       <c r="B1" t="s">
-        <v>139</v>
+        <v>3</v>
       </c>
       <c r="C1" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="E1" t="s">
         <v>5</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>141</v>
+        <v>9</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>142</v>
+        <v>150</v>
       </c>
       <c r="H1" t="str">
-        <f t="shared" ref="H1" ca="1" si="0">CONCATENATE("array('mo_fecha' =&gt; new \DateTime('",TEXT(A1,"yyyy-mm-dd"),"'), 'mo_concepto' =&gt; '",B1,"', 'mo_tipo' =&gt; '",C1,"', 'mo_documento' =&gt; '",D1,"', 'mo_oficina' =&gt; '",E1,"', 'mo_monto' =&gt; ",TRIM(F1),", 'mo_saldo' =&gt; ",G1,", 'mo_fecha_crea' =&gt; new \DateTime('",TEXT(NOW(),"yyyy-mm-dd H:m:s"),"'), 'mo_quien_crea' =&gt; 1, 'mo_fecha_modifica' =&gt; NULL, 'mo_quien_modifica' =&gt; NULL, 'mo_borrado_logico' =&gt; false),")</f>
-        <v>array('mo_fecha' =&gt; new \DateTime('2014-03-14'), 'mo_concepto' =&gt; '2200555126/0995935959', 'mo_tipo' =&gt; 'D', 'mo_documento' =&gt; '0007745172', 'mo_oficina' =&gt; 'AG. NORTE', 'mo_monto' =&gt; 6.00  , 'mo_saldo' =&gt; 1995.56, 'mo_fecha_crea' =&gt; new \DateTime('2014-03-20 11:4:2'), 'mo_quien_crea' =&gt; 1, 'mo_fecha_modifica' =&gt; NULL, 'mo_quien_modifica' =&gt; NULL, 'mo_borrado_logico' =&gt; false),</v>
+        <f t="shared" ref="H1:H3" ca="1" si="0">CONCATENATE("array('mo_fecha' =&gt; new \DateTime('",TEXT(A1,"yyyy-mm-dd"),"'), 'mo_concepto' =&gt; '",B1,"', 'mo_tipo' =&gt; '",C1,"', 'mo_documento' =&gt; '",D1,"', 'mo_oficina' =&gt; '",E1,"', 'mo_monto' =&gt; ",TRIM(F1),", 'mo_saldo' =&gt; ",G1,", 'mo_fecha_crea' =&gt; new \DateTime('",TEXT(NOW(),"yyyy-mm-dd H:m:s"),"'), 'mo_quien_crea' =&gt; 1, 'mo_fecha_modifica' =&gt; NULL, 'mo_quien_modifica' =&gt; NULL, 'mo_borrado_logico' =&gt; false),")</f>
+        <v>array('mo_fecha' =&gt; new \DateTime('2014-03-24'), 'mo_concepto' =&gt; '  TRANSFERENCIA INTERNET', 'mo_tipo' =&gt; 'D', 'mo_documento' =&gt; '0002254424', 'mo_oficina' =&gt; 'AG. NORTE', 'mo_monto' =&gt; 20.00  , 'mo_saldo' =&gt; 2035.56, 'mo_fecha_crea' =&gt; new \DateTime('2014-03-22 14:12:58'), 'mo_quien_crea' =&gt; 1, 'mo_fecha_modifica' =&gt; NULL, 'mo_quien_modifica' =&gt; NULL, 'mo_borrado_logico' =&gt; false),</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>41708</v>
+        <v>41722</v>
       </c>
       <c r="B2" t="s">
-        <v>135</v>
+        <v>144</v>
       </c>
       <c r="C2" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>136</v>
+        <v>145</v>
       </c>
       <c r="E2" t="s">
-        <v>5</v>
+        <v>146</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>6</v>
+        <v>27</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>138</v>
+        <v>149</v>
+      </c>
+      <c r="H2" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>array('mo_fecha' =&gt; new \DateTime('2014-03-24'), 'mo_concepto' =&gt; 'RETIRO ATM BP D/KENNEDY 3', 'mo_tipo' =&gt; 'D', 'mo_documento' =&gt; '0000653181', 'mo_oficina' =&gt; 'KENNEDY', 'mo_monto' =&gt; 40.00  , 'mo_saldo' =&gt; 2055.56, 'mo_fecha_crea' =&gt; new \DateTime('2014-03-22 14:12:58'), 'mo_quien_crea' =&gt; 1, 'mo_fecha_modifica' =&gt; NULL, 'mo_quien_modifica' =&gt; NULL, 'mo_borrado_logico' =&gt; false),</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>41705</v>
+        <v>41719</v>
       </c>
       <c r="B3" t="s">
-        <v>59</v>
+        <v>32</v>
       </c>
       <c r="C3" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>137</v>
+        <v>147</v>
       </c>
       <c r="E3" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>133</v>
+        <v>6</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>131</v>
+        <v>148</v>
+      </c>
+      <c r="H3" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>array('mo_fecha' =&gt; new \DateTime('2014-03-21'), 'mo_concepto' =&gt; 'DEPOSITO', 'mo_tipo' =&gt; 'C', 'mo_documento' =&gt; '0006095191', 'mo_oficina' =&gt; 'TENA', 'mo_monto' =&gt; 100.00  , 'mo_saldo' =&gt; 2095.56, 'mo_fecha_crea' =&gt; new \DateTime('2014-03-22 14:12:58'), 'mo_quien_crea' =&gt; 1, 'mo_fecha_modifica' =&gt; NULL, 'mo_quien_modifica' =&gt; NULL, 'mo_borrado_logico' =&gt; false),</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
-        <v>41703</v>
+        <v>41712</v>
       </c>
       <c r="B4" t="s">
-        <v>3</v>
+        <v>139</v>
       </c>
       <c r="C4" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>132</v>
+        <v>140</v>
       </c>
       <c r="E4" t="s">
         <v>5</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>133</v>
+        <v>141</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>134</v>
+        <v>142</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
-        <v>41703</v>
+        <v>41708</v>
       </c>
       <c r="B5" t="s">
-        <v>117</v>
+        <v>135</v>
       </c>
       <c r="C5" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>118</v>
+        <v>136</v>
       </c>
       <c r="E5" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>119</v>
+        <v>6</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>131</v>
+        <v>138</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
-        <v>41703</v>
+        <v>41705</v>
       </c>
       <c r="B6" t="s">
-        <v>2</v>
+        <v>59</v>
       </c>
       <c r="C6" t="s">
         <v>0</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>120</v>
+        <v>137</v>
       </c>
       <c r="E6" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>121</v>
+        <v>133</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
-        <v>41698</v>
+        <v>41703</v>
       </c>
       <c r="B7" t="s">
-        <v>17</v>
+        <v>3</v>
       </c>
       <c r="C7" t="s">
         <v>4</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>122</v>
+        <v>132</v>
       </c>
       <c r="E7" t="s">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>123</v>
+        <v>133</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>129</v>
+        <v>134</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
-        <v>41691</v>
+        <v>41703</v>
       </c>
       <c r="B8" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="C8" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="E8" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>67</v>
+        <v>119</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
-        <v>41691</v>
+        <v>41703</v>
       </c>
       <c r="B9" t="s">
-        <v>124</v>
+        <v>2</v>
       </c>
       <c r="C9" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="E9" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>67</v>
+        <v>121</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
-        <v>41690</v>
+        <v>41698</v>
       </c>
       <c r="B10" t="s">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="C10" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>113</v>
+        <v>122</v>
       </c>
       <c r="E10" t="s">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>114</v>
+        <v>123</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>112</v>
+        <v>129</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
-        <v>41690</v>
+        <v>41691</v>
       </c>
       <c r="B11" t="s">
-        <v>3</v>
+        <v>124</v>
       </c>
       <c r="C11" t="s">
         <v>4</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>115</v>
+        <v>125</v>
       </c>
       <c r="E11" t="s">
         <v>5</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>114</v>
+        <v>67</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>116</v>
+        <v>128</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
-        <v>41682</v>
+        <v>41691</v>
       </c>
       <c r="B12" t="s">
-        <v>106</v>
+        <v>124</v>
       </c>
       <c r="C12" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>107</v>
+        <v>126</v>
       </c>
       <c r="E12" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>108</v>
+        <v>67</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>112</v>
+        <v>127</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
-        <v>41680</v>
+        <v>41690</v>
       </c>
       <c r="B13" t="s">
-        <v>32</v>
+        <v>3</v>
       </c>
       <c r="C13" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="E13" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
-        <v>41680</v>
+        <v>41690</v>
       </c>
       <c r="B14" t="s">
         <v>3</v>
       </c>
       <c r="C14" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>105</v>
+        <v>115</v>
       </c>
       <c r="E14" t="s">
         <v>5</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>6</v>
+        <v>114</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>98</v>
+        <v>116</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
-        <v>41677</v>
+        <v>41682</v>
       </c>
       <c r="B15" t="s">
-        <v>32</v>
+        <v>106</v>
       </c>
       <c r="C15" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>99</v>
+        <v>107</v>
       </c>
       <c r="E15" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>6</v>
+        <v>108</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>104</v>
+        <v>112</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
-        <v>41677</v>
+        <v>41680</v>
       </c>
       <c r="B16" t="s">
-        <v>59</v>
+        <v>32</v>
       </c>
       <c r="C16" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>100</v>
+        <v>109</v>
       </c>
       <c r="E16" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>101</v>
+        <v>110</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>98</v>
+        <v>111</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
-        <v>41676</v>
+        <v>41680</v>
       </c>
       <c r="B17" t="s">
         <v>3</v>
       </c>
       <c r="C17" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="E17" t="s">
         <v>5</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>101</v>
+        <v>6</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
-        <v>41674</v>
+        <v>41677</v>
       </c>
       <c r="B18" t="s">
-        <v>95</v>
+        <v>32</v>
       </c>
       <c r="C18" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="E18" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>97</v>
+        <v>6</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>98</v>
+        <v>104</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
-        <v>41670</v>
+        <v>41677</v>
       </c>
       <c r="B19" t="s">
-        <v>17</v>
+        <v>59</v>
       </c>
       <c r="C19" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>18</v>
+        <v>100</v>
       </c>
       <c r="E19" t="s">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>20</v>
+        <v>101</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
-        <v>41666</v>
+        <v>41676</v>
       </c>
       <c r="B20" t="s">
         <v>3</v>
       </c>
       <c r="C20" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>21</v>
+        <v>102</v>
       </c>
       <c r="E20" t="s">
         <v>5</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>71</v>
+        <v>101</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>93</v>
+        <v>103</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
-        <v>41666</v>
+        <v>41674</v>
       </c>
       <c r="B21" t="s">
-        <v>2</v>
+        <v>95</v>
       </c>
       <c r="C21" t="s">
         <v>0</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>22</v>
+        <v>96</v>
       </c>
       <c r="E21" t="s">
         <v>1</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>23</v>
+        <v>97</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
-        <v>41666</v>
+        <v>41670</v>
       </c>
       <c r="B22" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="C22" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="E22" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
@@ -1303,344 +1335,344 @@
         <v>41666</v>
       </c>
       <c r="B23" t="s">
-        <v>28</v>
+        <v>3</v>
       </c>
       <c r="C23" t="s">
         <v>0</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="E23" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>30</v>
+        <v>71</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
-        <v>41660</v>
+        <v>41666</v>
       </c>
       <c r="B24" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="C24" t="s">
         <v>0</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="E24" t="s">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>9</v>
+        <v>23</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
-        <v>41660</v>
+        <v>41666</v>
       </c>
       <c r="B25" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="C25" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="E25" t="s">
-        <v>10</v>
+        <v>26</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>6</v>
+        <v>27</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
-        <v>41660</v>
+        <v>41666</v>
       </c>
       <c r="B26" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="C26" t="s">
         <v>0</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="E26" t="s">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
-        <v>41659</v>
+        <v>41660</v>
       </c>
       <c r="B27" t="s">
-        <v>37</v>
+        <v>11</v>
       </c>
       <c r="C27" t="s">
         <v>0</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="E27" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>39</v>
+        <v>9</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
-        <v>41655</v>
+        <v>41660</v>
       </c>
       <c r="B28" t="s">
-        <v>2</v>
+        <v>32</v>
       </c>
       <c r="C28" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="E28" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F28" s="3" t="s">
-        <v>41</v>
+        <v>6</v>
       </c>
       <c r="G28" s="3" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
-        <v>41655</v>
+        <v>41660</v>
       </c>
       <c r="B29" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="C29" t="s">
         <v>0</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="E29" t="s">
-        <v>44</v>
+        <v>12</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>6</v>
+        <v>36</v>
       </c>
       <c r="G29" s="3" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
-        <v>41652</v>
+        <v>41659</v>
       </c>
       <c r="B30" t="s">
-        <v>3</v>
+        <v>37</v>
       </c>
       <c r="C30" t="s">
         <v>0</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="E30" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="G30" s="3" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
-        <v>41649</v>
+        <v>41655</v>
       </c>
       <c r="B31" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C31" t="s">
         <v>0</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>16</v>
+        <v>40</v>
       </c>
       <c r="E31" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>15</v>
+        <v>41</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
-        <v>41648</v>
+        <v>41655</v>
       </c>
       <c r="B32" t="s">
-        <v>2</v>
+        <v>42</v>
       </c>
       <c r="C32" t="s">
         <v>0</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="E32" t="s">
-        <v>1</v>
+        <v>44</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>48</v>
+        <v>6</v>
       </c>
       <c r="G32" s="3" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
-        <v>41648</v>
+        <v>41652</v>
       </c>
       <c r="B33" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C33" t="s">
         <v>0</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="E33" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F33" s="3" t="s">
-        <v>9</v>
+        <v>46</v>
       </c>
       <c r="G33" s="3" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
-        <v>41647</v>
+        <v>41649</v>
       </c>
       <c r="B34" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C34" t="s">
         <v>0</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>50</v>
+        <v>16</v>
       </c>
       <c r="E34" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>51</v>
+        <v>15</v>
       </c>
       <c r="G34" s="3" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
-        <v>41646</v>
+        <v>41648</v>
       </c>
       <c r="B35" t="s">
-        <v>52</v>
+        <v>2</v>
       </c>
       <c r="C35" t="s">
         <v>0</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="E35" t="s">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>13</v>
+        <v>48</v>
       </c>
       <c r="G35" s="3" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
-        <v>41646</v>
+        <v>41648</v>
       </c>
       <c r="B36" t="s">
-        <v>54</v>
+        <v>7</v>
       </c>
       <c r="C36" t="s">
         <v>0</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="E36" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F36" s="3" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="G36" s="3" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
-        <v>41646</v>
+        <v>41647</v>
       </c>
       <c r="B37" t="s">
-        <v>56</v>
+        <v>2</v>
       </c>
       <c r="C37" t="s">
         <v>0</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="E37" t="s">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="F37" s="3" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="G37" s="3" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
@@ -1648,107 +1680,176 @@
         <v>41646</v>
       </c>
       <c r="B38" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="C38" t="s">
         <v>0</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="E38" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="F38" s="3" t="s">
-        <v>61</v>
+        <v>13</v>
       </c>
       <c r="G38" s="3" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
-        <v>41645</v>
+        <v>41646</v>
       </c>
       <c r="B39" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="C39" t="s">
         <v>0</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="E39" t="s">
-        <v>64</v>
+        <v>12</v>
       </c>
       <c r="F39" s="3" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="G39" s="3" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
-        <v>41642</v>
+        <v>41646</v>
       </c>
       <c r="B40" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="C40" t="s">
         <v>0</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="E40" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F40" s="3" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
       <c r="G40" s="3" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
+        <v>41646</v>
+      </c>
+      <c r="B41" t="s">
+        <v>59</v>
+      </c>
+      <c r="C41" t="s">
+        <v>0</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="E41" t="s">
+        <v>5</v>
+      </c>
+      <c r="F41" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="G41" s="3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A42" s="1">
+        <v>41645</v>
+      </c>
+      <c r="B42" t="s">
+        <v>62</v>
+      </c>
+      <c r="C42" t="s">
+        <v>0</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="E42" t="s">
+        <v>64</v>
+      </c>
+      <c r="F42" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G42" s="3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A43" s="1">
+        <v>41642</v>
+      </c>
+      <c r="B43" t="s">
+        <v>65</v>
+      </c>
+      <c r="C43" t="s">
+        <v>0</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="E43" t="s">
+        <v>10</v>
+      </c>
+      <c r="F43" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="G43" s="3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A44" s="1">
         <v>41641</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B44" t="s">
         <v>68</v>
       </c>
-      <c r="C41" t="s">
-        <v>0</v>
-      </c>
-      <c r="D41" s="2" t="s">
+      <c r="C44" t="s">
+        <v>0</v>
+      </c>
+      <c r="D44" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="E41" t="s">
+      <c r="E44" t="s">
         <v>1</v>
       </c>
-      <c r="F41" s="3" t="s">
+      <c r="F44" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="G41" s="3" t="s">
+      <c r="G44" s="3" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A42" s="1"/>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A43" s="1"/>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A44" s="1"/>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="1"/>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="1"/>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A47" s="1"/>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A48" s="1"/>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A49" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Agregando mas funcionalidades de consulta con Ajax
</commit_message>
<xml_diff>
--- a/backup/cuenta_2200555126.xlsx
+++ b/backup/cuenta_2200555126.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\php-projects\dml2\backup\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\xampp\htdocs\dml2\backup\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -802,7 +802,7 @@
   <dimension ref="A1:H49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="H1" sqref="H1:H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -836,7 +836,7 @@
       </c>
       <c r="H1" t="str">
         <f t="shared" ref="H1:H3" ca="1" si="0">CONCATENATE("array('mo_fecha' =&gt; new \DateTime('",TEXT(A1,"yyyy-mm-dd"),"'), 'mo_concepto' =&gt; '",B1,"', 'mo_tipo' =&gt; '",C1,"', 'mo_documento' =&gt; '",D1,"', 'mo_oficina' =&gt; '",E1,"', 'mo_monto' =&gt; ",TRIM(F1),", 'mo_saldo' =&gt; ",G1,", 'mo_fecha_crea' =&gt; new \DateTime('",TEXT(NOW(),"yyyy-mm-dd H:m:s"),"'), 'mo_quien_crea' =&gt; 1, 'mo_fecha_modifica' =&gt; NULL, 'mo_quien_modifica' =&gt; NULL, 'mo_borrado_logico' =&gt; false),")</f>
-        <v>array('mo_fecha' =&gt; new \DateTime('2014-03-24'), 'mo_concepto' =&gt; '  TRANSFERENCIA INTERNET', 'mo_tipo' =&gt; 'D', 'mo_documento' =&gt; '0002254424', 'mo_oficina' =&gt; 'AG. NORTE', 'mo_monto' =&gt; 20.00  , 'mo_saldo' =&gt; 2035.56, 'mo_fecha_crea' =&gt; new \DateTime('2014-03-22 14:12:58'), 'mo_quien_crea' =&gt; 1, 'mo_fecha_modifica' =&gt; NULL, 'mo_quien_modifica' =&gt; NULL, 'mo_borrado_logico' =&gt; false),</v>
+        <v>array('mo_fecha' =&gt; new \DateTime('2014-03-24'), 'mo_concepto' =&gt; '  TRANSFERENCIA INTERNET', 'mo_tipo' =&gt; 'D', 'mo_documento' =&gt; '0002254424', 'mo_oficina' =&gt; 'AG. NORTE', 'mo_monto' =&gt; 20.00  , 'mo_saldo' =&gt; 2035.56, 'mo_fecha_crea' =&gt; new \DateTime('2014-03-24 16:57:10'), 'mo_quien_crea' =&gt; 1, 'mo_fecha_modifica' =&gt; NULL, 'mo_quien_modifica' =&gt; NULL, 'mo_borrado_logico' =&gt; false),</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -863,7 +863,7 @@
       </c>
       <c r="H2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>array('mo_fecha' =&gt; new \DateTime('2014-03-24'), 'mo_concepto' =&gt; 'RETIRO ATM BP D/KENNEDY 3', 'mo_tipo' =&gt; 'D', 'mo_documento' =&gt; '0000653181', 'mo_oficina' =&gt; 'KENNEDY', 'mo_monto' =&gt; 40.00  , 'mo_saldo' =&gt; 2055.56, 'mo_fecha_crea' =&gt; new \DateTime('2014-03-22 14:12:58'), 'mo_quien_crea' =&gt; 1, 'mo_fecha_modifica' =&gt; NULL, 'mo_quien_modifica' =&gt; NULL, 'mo_borrado_logico' =&gt; false),</v>
+        <v>array('mo_fecha' =&gt; new \DateTime('2014-03-24'), 'mo_concepto' =&gt; 'RETIRO ATM BP D/KENNEDY 3', 'mo_tipo' =&gt; 'D', 'mo_documento' =&gt; '0000653181', 'mo_oficina' =&gt; 'KENNEDY', 'mo_monto' =&gt; 40.00  , 'mo_saldo' =&gt; 2055.56, 'mo_fecha_crea' =&gt; new \DateTime('2014-03-24 16:57:10'), 'mo_quien_crea' =&gt; 1, 'mo_fecha_modifica' =&gt; NULL, 'mo_quien_modifica' =&gt; NULL, 'mo_borrado_logico' =&gt; false),</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -890,7 +890,7 @@
       </c>
       <c r="H3" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>array('mo_fecha' =&gt; new \DateTime('2014-03-21'), 'mo_concepto' =&gt; 'DEPOSITO', 'mo_tipo' =&gt; 'C', 'mo_documento' =&gt; '0006095191', 'mo_oficina' =&gt; 'TENA', 'mo_monto' =&gt; 100.00  , 'mo_saldo' =&gt; 2095.56, 'mo_fecha_crea' =&gt; new \DateTime('2014-03-22 14:12:58'), 'mo_quien_crea' =&gt; 1, 'mo_fecha_modifica' =&gt; NULL, 'mo_quien_modifica' =&gt; NULL, 'mo_borrado_logico' =&gt; false),</v>
+        <v>array('mo_fecha' =&gt; new \DateTime('2014-03-21'), 'mo_concepto' =&gt; 'DEPOSITO', 'mo_tipo' =&gt; 'C', 'mo_documento' =&gt; '0006095191', 'mo_oficina' =&gt; 'TENA', 'mo_monto' =&gt; 100.00  , 'mo_saldo' =&gt; 2095.56, 'mo_fecha_crea' =&gt; new \DateTime('2014-03-24 16:57:10'), 'mo_quien_crea' =&gt; 1, 'mo_fecha_modifica' =&gt; NULL, 'mo_quien_modifica' =&gt; NULL, 'mo_borrado_logico' =&gt; false),</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Añadiendo nuevo plugin jquery zclip
</commit_message>
<xml_diff>
--- a/backup/cuenta_2200555126.xlsx
+++ b/backup/cuenta_2200555126.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="159">
   <si>
     <t>D</t>
   </si>
@@ -477,6 +477,30 @@
   </si>
   <si>
     <t>2035.56</t>
+  </si>
+  <si>
+    <t>CONSUMO DATA SUPERMAXI (AV. 6 DE DI</t>
+  </si>
+  <si>
+    <t>0015391688</t>
+  </si>
+  <si>
+    <t>28.02  </t>
+  </si>
+  <si>
+    <t>RETIRO ATM BP D/MEGA MAXI 1</t>
+  </si>
+  <si>
+    <t>0015258475</t>
+  </si>
+  <si>
+    <t>CENTRO DE ACOPIO NORTE</t>
+  </si>
+  <si>
+    <t>1935.56</t>
+  </si>
+  <si>
+    <t>1907.54</t>
   </si>
 </sst>
 </file>
@@ -799,10 +823,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H49"/>
+  <dimension ref="A1:H51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1:H3"/>
+      <selection activeCell="H1" sqref="H1:H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -817,26 +841,26 @@
         <v>41722</v>
       </c>
       <c r="B1" t="s">
-        <v>3</v>
+        <v>151</v>
       </c>
       <c r="C1" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>143</v>
+        <v>152</v>
       </c>
       <c r="E1" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>9</v>
+        <v>153</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>150</v>
+        <v>158</v>
       </c>
       <c r="H1" t="str">
-        <f t="shared" ref="H1:H3" ca="1" si="0">CONCATENATE("array('mo_fecha' =&gt; new \DateTime('",TEXT(A1,"yyyy-mm-dd"),"'), 'mo_concepto' =&gt; '",B1,"', 'mo_tipo' =&gt; '",C1,"', 'mo_documento' =&gt; '",D1,"', 'mo_oficina' =&gt; '",E1,"', 'mo_monto' =&gt; ",TRIM(F1),", 'mo_saldo' =&gt; ",G1,", 'mo_fecha_crea' =&gt; new \DateTime('",TEXT(NOW(),"yyyy-mm-dd H:m:s"),"'), 'mo_quien_crea' =&gt; 1, 'mo_fecha_modifica' =&gt; NULL, 'mo_quien_modifica' =&gt; NULL, 'mo_borrado_logico' =&gt; false),")</f>
-        <v>array('mo_fecha' =&gt; new \DateTime('2014-03-24'), 'mo_concepto' =&gt; '  TRANSFERENCIA INTERNET', 'mo_tipo' =&gt; 'D', 'mo_documento' =&gt; '0002254424', 'mo_oficina' =&gt; 'AG. NORTE', 'mo_monto' =&gt; 20.00  , 'mo_saldo' =&gt; 2035.56, 'mo_fecha_crea' =&gt; new \DateTime('2014-03-24 16:57:10'), 'mo_quien_crea' =&gt; 1, 'mo_fecha_modifica' =&gt; NULL, 'mo_quien_modifica' =&gt; NULL, 'mo_borrado_logico' =&gt; false),</v>
+        <f t="shared" ref="H1:H5" ca="1" si="0">CONCATENATE("array('mo_fecha' =&gt; new \DateTime('",TEXT(A1,"yyyy-mm-dd"),"'), 'mo_concepto' =&gt; '",B1,"', 'mo_tipo' =&gt; '",C1,"', 'mo_documento' =&gt; '",D1,"', 'mo_oficina' =&gt; '",E1,"', 'mo_monto' =&gt; ",TRIM(F1),", 'mo_saldo' =&gt; ",G1,", 'mo_fecha_crea' =&gt; new \DateTime('",TEXT(NOW(),"yyyy-mm-dd H:m:s"),"'), 'mo_quien_crea' =&gt; 1, 'mo_fecha_modifica' =&gt; NULL, 'mo_quien_modifica' =&gt; NULL, 'mo_borrado_logico' =&gt; false),")</f>
+        <v>array('mo_fecha' =&gt; new \DateTime('2014-03-24'), 'mo_concepto' =&gt; 'CONSUMO DATA SUPERMAXI (AV. 6 DE DI', 'mo_tipo' =&gt; 'D', 'mo_documento' =&gt; '0015391688', 'mo_oficina' =&gt; 'INSTITUCIONAL SS.CC.', 'mo_monto' =&gt; 28.02  , 'mo_saldo' =&gt; 1907.54, 'mo_fecha_crea' =&gt; new \DateTime('2014-03-25 16:15:14'), 'mo_quien_crea' =&gt; 1, 'mo_fecha_modifica' =&gt; NULL, 'mo_quien_modifica' =&gt; NULL, 'mo_borrado_logico' =&gt; false),</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -844,165 +868,161 @@
         <v>41722</v>
       </c>
       <c r="B2" t="s">
-        <v>144</v>
+        <v>154</v>
       </c>
       <c r="C2" t="s">
         <v>0</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>145</v>
+        <v>155</v>
       </c>
       <c r="E2" t="s">
-        <v>146</v>
+        <v>156</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>27</v>
+        <v>6</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>149</v>
+        <v>157</v>
       </c>
       <c r="H2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>array('mo_fecha' =&gt; new \DateTime('2014-03-24'), 'mo_concepto' =&gt; 'RETIRO ATM BP D/KENNEDY 3', 'mo_tipo' =&gt; 'D', 'mo_documento' =&gt; '0000653181', 'mo_oficina' =&gt; 'KENNEDY', 'mo_monto' =&gt; 40.00  , 'mo_saldo' =&gt; 2055.56, 'mo_fecha_crea' =&gt; new \DateTime('2014-03-24 16:57:10'), 'mo_quien_crea' =&gt; 1, 'mo_fecha_modifica' =&gt; NULL, 'mo_quien_modifica' =&gt; NULL, 'mo_borrado_logico' =&gt; false),</v>
+        <v>array('mo_fecha' =&gt; new \DateTime('2014-03-24'), 'mo_concepto' =&gt; 'RETIRO ATM BP D/MEGA MAXI 1', 'mo_tipo' =&gt; 'D', 'mo_documento' =&gt; '0015258475', 'mo_oficina' =&gt; 'CENTRO DE ACOPIO NORTE', 'mo_monto' =&gt; 100.00  , 'mo_saldo' =&gt; 1935.56, 'mo_fecha_crea' =&gt; new \DateTime('2014-03-25 16:15:14'), 'mo_quien_crea' =&gt; 1, 'mo_fecha_modifica' =&gt; NULL, 'mo_quien_modifica' =&gt; NULL, 'mo_borrado_logico' =&gt; false),</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>41719</v>
+        <v>41722</v>
       </c>
       <c r="B3" t="s">
-        <v>32</v>
+        <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="E3" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>148</v>
-      </c>
-      <c r="H3" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>array('mo_fecha' =&gt; new \DateTime('2014-03-21'), 'mo_concepto' =&gt; 'DEPOSITO', 'mo_tipo' =&gt; 'C', 'mo_documento' =&gt; '0006095191', 'mo_oficina' =&gt; 'TENA', 'mo_monto' =&gt; 100.00  , 'mo_saldo' =&gt; 2095.56, 'mo_fecha_crea' =&gt; new \DateTime('2014-03-24 16:57:10'), 'mo_quien_crea' =&gt; 1, 'mo_fecha_modifica' =&gt; NULL, 'mo_quien_modifica' =&gt; NULL, 'mo_borrado_logico' =&gt; false),</v>
+        <v>150</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
-        <v>41712</v>
+        <v>41722</v>
       </c>
       <c r="B4" t="s">
-        <v>139</v>
+        <v>144</v>
       </c>
       <c r="C4" t="s">
         <v>0</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>140</v>
+        <v>145</v>
       </c>
       <c r="E4" t="s">
-        <v>5</v>
+        <v>146</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>141</v>
+        <v>27</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>142</v>
+        <v>149</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
-        <v>41708</v>
+        <v>41719</v>
       </c>
       <c r="B5" t="s">
-        <v>135</v>
+        <v>32</v>
       </c>
       <c r="C5" t="s">
         <v>4</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>136</v>
+        <v>147</v>
       </c>
       <c r="E5" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="F5" s="3" t="s">
         <v>6</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>138</v>
+        <v>148</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
-        <v>41705</v>
+        <v>41712</v>
       </c>
       <c r="B6" t="s">
-        <v>59</v>
+        <v>139</v>
       </c>
       <c r="C6" t="s">
         <v>0</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="E6" t="s">
         <v>5</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>133</v>
+        <v>141</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>131</v>
+        <v>142</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
-        <v>41703</v>
+        <v>41708</v>
       </c>
       <c r="B7" t="s">
-        <v>3</v>
+        <v>135</v>
       </c>
       <c r="C7" t="s">
         <v>4</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
       <c r="E7" t="s">
         <v>5</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>133</v>
+        <v>6</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
-        <v>41703</v>
+        <v>41705</v>
       </c>
       <c r="B8" t="s">
-        <v>117</v>
+        <v>59</v>
       </c>
       <c r="C8" t="s">
         <v>0</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>118</v>
+        <v>137</v>
       </c>
       <c r="E8" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>119</v>
+        <v>133</v>
       </c>
       <c r="G8" s="3" t="s">
         <v>131</v>
@@ -1013,157 +1033,157 @@
         <v>41703</v>
       </c>
       <c r="B9" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C9" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>120</v>
+        <v>132</v>
       </c>
       <c r="E9" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>121</v>
+        <v>133</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
-        <v>41698</v>
+        <v>41703</v>
       </c>
       <c r="B10" t="s">
-        <v>17</v>
+        <v>117</v>
       </c>
       <c r="C10" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="E10" t="s">
-        <v>19</v>
+        <v>1</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
-        <v>41691</v>
+        <v>41703</v>
       </c>
       <c r="B11" t="s">
-        <v>124</v>
+        <v>2</v>
       </c>
       <c r="C11" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="E11" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>67</v>
+        <v>121</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
-        <v>41691</v>
+        <v>41698</v>
       </c>
       <c r="B12" t="s">
-        <v>124</v>
+        <v>17</v>
       </c>
       <c r="C12" t="s">
         <v>4</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="E12" t="s">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>67</v>
+        <v>123</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
-        <v>41690</v>
+        <v>41691</v>
       </c>
       <c r="B13" t="s">
-        <v>3</v>
+        <v>124</v>
       </c>
       <c r="C13" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>113</v>
+        <v>125</v>
       </c>
       <c r="E13" t="s">
         <v>5</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>114</v>
+        <v>67</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>112</v>
+        <v>128</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
-        <v>41690</v>
+        <v>41691</v>
       </c>
       <c r="B14" t="s">
-        <v>3</v>
+        <v>124</v>
       </c>
       <c r="C14" t="s">
         <v>4</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>115</v>
+        <v>126</v>
       </c>
       <c r="E14" t="s">
         <v>5</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>114</v>
+        <v>67</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>116</v>
+        <v>127</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
-        <v>41682</v>
+        <v>41690</v>
       </c>
       <c r="B15" t="s">
-        <v>106</v>
+        <v>3</v>
       </c>
       <c r="C15" t="s">
         <v>0</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>107</v>
+        <v>113</v>
       </c>
       <c r="E15" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>108</v>
+        <v>114</v>
       </c>
       <c r="G15" s="3" t="s">
         <v>112</v>
@@ -1171,53 +1191,53 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
-        <v>41680</v>
+        <v>41690</v>
       </c>
       <c r="B16" t="s">
-        <v>32</v>
+        <v>3</v>
       </c>
       <c r="C16" t="s">
         <v>4</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>109</v>
+        <v>115</v>
       </c>
       <c r="E16" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
-        <v>41680</v>
+        <v>41682</v>
       </c>
       <c r="B17" t="s">
-        <v>3</v>
+        <v>106</v>
       </c>
       <c r="C17" t="s">
         <v>0</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="E17" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>6</v>
+        <v>108</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>98</v>
+        <v>112</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
-        <v>41677</v>
+        <v>41680</v>
       </c>
       <c r="B18" t="s">
         <v>32</v>
@@ -1226,36 +1246,36 @@
         <v>4</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>99</v>
+        <v>109</v>
       </c>
       <c r="E18" t="s">
         <v>10</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>6</v>
+        <v>110</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>104</v>
+        <v>111</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
-        <v>41677</v>
+        <v>41680</v>
       </c>
       <c r="B19" t="s">
-        <v>59</v>
+        <v>3</v>
       </c>
       <c r="C19" t="s">
         <v>0</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="E19" t="s">
         <v>5</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>101</v>
+        <v>6</v>
       </c>
       <c r="G19" s="3" t="s">
         <v>98</v>
@@ -1263,45 +1283,45 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
-        <v>41676</v>
+        <v>41677</v>
       </c>
       <c r="B20" t="s">
-        <v>3</v>
+        <v>32</v>
       </c>
       <c r="C20" t="s">
         <v>4</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="E20" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>101</v>
+        <v>6</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
-        <v>41674</v>
+        <v>41677</v>
       </c>
       <c r="B21" t="s">
-        <v>95</v>
+        <v>59</v>
       </c>
       <c r="C21" t="s">
         <v>0</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="E21" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="G21" s="3" t="s">
         <v>98</v>
@@ -1309,71 +1329,71 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
-        <v>41670</v>
+        <v>41676</v>
       </c>
       <c r="B22" t="s">
-        <v>17</v>
+        <v>3</v>
       </c>
       <c r="C22" t="s">
         <v>4</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>18</v>
+        <v>102</v>
       </c>
       <c r="E22" t="s">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>20</v>
+        <v>101</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>94</v>
+        <v>103</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
-        <v>41666</v>
+        <v>41674</v>
       </c>
       <c r="B23" t="s">
-        <v>3</v>
+        <v>95</v>
       </c>
       <c r="C23" t="s">
         <v>0</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>21</v>
+        <v>96</v>
       </c>
       <c r="E23" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>71</v>
+        <v>97</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
-        <v>41666</v>
+        <v>41670</v>
       </c>
       <c r="B24" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="C24" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="E24" t="s">
-        <v>1</v>
+        <v>19</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
@@ -1381,22 +1401,22 @@
         <v>41666</v>
       </c>
       <c r="B25" t="s">
-        <v>24</v>
+        <v>3</v>
       </c>
       <c r="C25" t="s">
         <v>0</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="E25" t="s">
-        <v>26</v>
+        <v>5</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>27</v>
+        <v>71</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
@@ -1404,68 +1424,68 @@
         <v>41666</v>
       </c>
       <c r="B26" t="s">
-        <v>28</v>
+        <v>2</v>
       </c>
       <c r="C26" t="s">
         <v>0</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="E26" t="s">
         <v>1</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
-        <v>41660</v>
+        <v>41666</v>
       </c>
       <c r="B27" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="C27" t="s">
         <v>0</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="E27" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>9</v>
+        <v>27</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
-        <v>41660</v>
+        <v>41666</v>
       </c>
       <c r="B28" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C28" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="E28" t="s">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="F28" s="3" t="s">
-        <v>6</v>
+        <v>30</v>
       </c>
       <c r="G28" s="3" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
@@ -1473,188 +1493,188 @@
         <v>41660</v>
       </c>
       <c r="B29" t="s">
-        <v>34</v>
+        <v>11</v>
       </c>
       <c r="C29" t="s">
         <v>0</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="E29" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>36</v>
+        <v>9</v>
       </c>
       <c r="G29" s="3" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
-        <v>41659</v>
+        <v>41660</v>
       </c>
       <c r="B30" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="C30" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="E30" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>39</v>
+        <v>6</v>
       </c>
       <c r="G30" s="3" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
-        <v>41655</v>
+        <v>41660</v>
       </c>
       <c r="B31" t="s">
-        <v>2</v>
+        <v>34</v>
       </c>
       <c r="C31" t="s">
         <v>0</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="E31" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
-        <v>41655</v>
+        <v>41659</v>
       </c>
       <c r="B32" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="C32" t="s">
         <v>0</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="E32" t="s">
-        <v>44</v>
+        <v>1</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>6</v>
+        <v>39</v>
       </c>
       <c r="G32" s="3" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
-        <v>41652</v>
+        <v>41655</v>
       </c>
       <c r="B33" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C33" t="s">
         <v>0</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="E33" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F33" s="3" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="G33" s="3" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
-        <v>41649</v>
+        <v>41655</v>
       </c>
       <c r="B34" t="s">
-        <v>3</v>
+        <v>42</v>
       </c>
       <c r="C34" t="s">
         <v>0</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>16</v>
+        <v>43</v>
       </c>
       <c r="E34" t="s">
-        <v>5</v>
+        <v>44</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="G34" s="3" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
-        <v>41648</v>
+        <v>41652</v>
       </c>
       <c r="B35" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C35" t="s">
         <v>0</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E35" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="G35" s="3" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
-        <v>41648</v>
+        <v>41649</v>
       </c>
       <c r="B36" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C36" t="s">
         <v>0</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>49</v>
+        <v>16</v>
       </c>
       <c r="E36" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F36" s="3" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="G36" s="3" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
-        <v>41647</v>
+        <v>41648</v>
       </c>
       <c r="B37" t="s">
         <v>2</v>
@@ -1663,62 +1683,62 @@
         <v>0</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="E37" t="s">
         <v>1</v>
       </c>
       <c r="F37" s="3" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="G37" s="3" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
-        <v>41646</v>
+        <v>41648</v>
       </c>
       <c r="B38" t="s">
-        <v>52</v>
+        <v>7</v>
       </c>
       <c r="C38" t="s">
         <v>0</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="E38" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F38" s="3" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="G38" s="3" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
-        <v>41646</v>
+        <v>41647</v>
       </c>
       <c r="B39" t="s">
-        <v>54</v>
+        <v>2</v>
       </c>
       <c r="C39" t="s">
         <v>0</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="E39" t="s">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="F39" s="3" t="s">
-        <v>14</v>
+        <v>51</v>
       </c>
       <c r="G39" s="3" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
@@ -1726,22 +1746,22 @@
         <v>41646</v>
       </c>
       <c r="B40" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C40" t="s">
         <v>0</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="E40" t="s">
         <v>12</v>
       </c>
       <c r="F40" s="3" t="s">
-        <v>58</v>
+        <v>13</v>
       </c>
       <c r="G40" s="3" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
@@ -1749,98 +1769,138 @@
         <v>41646</v>
       </c>
       <c r="B41" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="C41" t="s">
         <v>0</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="E41" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="F41" s="3" t="s">
-        <v>61</v>
+        <v>14</v>
       </c>
       <c r="G41" s="3" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
-        <v>41645</v>
+        <v>41646</v>
       </c>
       <c r="B42" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="C42" t="s">
         <v>0</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="E42" t="s">
-        <v>64</v>
+        <v>12</v>
       </c>
       <c r="F42" s="3" t="s">
-        <v>9</v>
+        <v>58</v>
       </c>
       <c r="G42" s="3" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
-        <v>41642</v>
+        <v>41646</v>
       </c>
       <c r="B43" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="C43" t="s">
         <v>0</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="E43" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="F43" s="3" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="G43" s="3" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
+        <v>41645</v>
+      </c>
+      <c r="B44" t="s">
+        <v>62</v>
+      </c>
+      <c r="C44" t="s">
+        <v>0</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="E44" t="s">
+        <v>64</v>
+      </c>
+      <c r="F44" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G44" s="3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A45" s="1">
+        <v>41642</v>
+      </c>
+      <c r="B45" t="s">
+        <v>65</v>
+      </c>
+      <c r="C45" t="s">
+        <v>0</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="E45" t="s">
+        <v>10</v>
+      </c>
+      <c r="F45" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="G45" s="3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A46" s="1">
         <v>41641</v>
       </c>
-      <c r="B44" t="s">
+      <c r="B46" t="s">
         <v>68</v>
       </c>
-      <c r="C44" t="s">
-        <v>0</v>
-      </c>
-      <c r="D44" s="2" t="s">
+      <c r="C46" t="s">
+        <v>0</v>
+      </c>
+      <c r="D46" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="E44" t="s">
+      <c r="E46" t="s">
         <v>1</v>
       </c>
-      <c r="F44" s="3" t="s">
+      <c r="F46" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="G44" s="3" t="s">
+      <c r="G46" s="3" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A45" s="1"/>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A46" s="1"/>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="1"/>
@@ -1850,6 +1910,12 @@
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" s="1"/>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A50" s="1"/>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A51" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Agregando nuevas búsquedas ajax
</commit_message>
<xml_diff>
--- a/backup/cuenta_2200555126.xlsx
+++ b/backup/cuenta_2200555126.xlsx
@@ -859,8 +859,8 @@
         <v>158</v>
       </c>
       <c r="H1" t="str">
-        <f t="shared" ref="H1:H5" ca="1" si="0">CONCATENATE("array('mo_fecha' =&gt; new \DateTime('",TEXT(A1,"yyyy-mm-dd"),"'), 'mo_concepto' =&gt; '",B1,"', 'mo_tipo' =&gt; '",C1,"', 'mo_documento' =&gt; '",D1,"', 'mo_oficina' =&gt; '",E1,"', 'mo_monto' =&gt; ",TRIM(F1),", 'mo_saldo' =&gt; ",G1,", 'mo_fecha_crea' =&gt; new \DateTime('",TEXT(NOW(),"yyyy-mm-dd H:m:s"),"'), 'mo_quien_crea' =&gt; 1, 'mo_fecha_modifica' =&gt; NULL, 'mo_quien_modifica' =&gt; NULL, 'mo_borrado_logico' =&gt; false),")</f>
-        <v>array('mo_fecha' =&gt; new \DateTime('2014-03-24'), 'mo_concepto' =&gt; 'CONSUMO DATA SUPERMAXI (AV. 6 DE DI', 'mo_tipo' =&gt; 'D', 'mo_documento' =&gt; '0015391688', 'mo_oficina' =&gt; 'INSTITUCIONAL SS.CC.', 'mo_monto' =&gt; 28.02  , 'mo_saldo' =&gt; 1907.54, 'mo_fecha_crea' =&gt; new \DateTime('2014-03-25 16:15:14'), 'mo_quien_crea' =&gt; 1, 'mo_fecha_modifica' =&gt; NULL, 'mo_quien_modifica' =&gt; NULL, 'mo_borrado_logico' =&gt; false),</v>
+        <f t="shared" ref="H1:H2" ca="1" si="0">CONCATENATE("array('mo_fecha' =&gt; new \DateTime('",TEXT(A1,"yyyy-mm-dd"),"'), 'mo_concepto' =&gt; '",B1,"', 'mo_tipo' =&gt; '",C1,"', 'mo_documento' =&gt; '",D1,"', 'mo_oficina' =&gt; '",E1,"', 'mo_monto' =&gt; ",TRIM(F1),", 'mo_saldo' =&gt; ",G1,", 'mo_fecha_crea' =&gt; new \DateTime('",TEXT(NOW(),"yyyy-mm-dd H:m:s"),"'), 'mo_quien_crea' =&gt; 1, 'mo_fecha_modifica' =&gt; NULL, 'mo_quien_modifica' =&gt; NULL, 'mo_borrado_logico' =&gt; false),")</f>
+        <v>array('mo_fecha' =&gt; new \DateTime('2014-03-24'), 'mo_concepto' =&gt; 'CONSUMO DATA SUPERMAXI (AV. 6 DE DI', 'mo_tipo' =&gt; 'D', 'mo_documento' =&gt; '0015391688', 'mo_oficina' =&gt; 'INSTITUCIONAL SS.CC.', 'mo_monto' =&gt; 28.02  , 'mo_saldo' =&gt; 1907.54, 'mo_fecha_crea' =&gt; new \DateTime('2014-03-26 15:37:38'), 'mo_quien_crea' =&gt; 1, 'mo_fecha_modifica' =&gt; NULL, 'mo_quien_modifica' =&gt; NULL, 'mo_borrado_logico' =&gt; false),</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -887,7 +887,7 @@
       </c>
       <c r="H2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>array('mo_fecha' =&gt; new \DateTime('2014-03-24'), 'mo_concepto' =&gt; 'RETIRO ATM BP D/MEGA MAXI 1', 'mo_tipo' =&gt; 'D', 'mo_documento' =&gt; '0015258475', 'mo_oficina' =&gt; 'CENTRO DE ACOPIO NORTE', 'mo_monto' =&gt; 100.00  , 'mo_saldo' =&gt; 1935.56, 'mo_fecha_crea' =&gt; new \DateTime('2014-03-25 16:15:14'), 'mo_quien_crea' =&gt; 1, 'mo_fecha_modifica' =&gt; NULL, 'mo_quien_modifica' =&gt; NULL, 'mo_borrado_logico' =&gt; false),</v>
+        <v>array('mo_fecha' =&gt; new \DateTime('2014-03-24'), 'mo_concepto' =&gt; 'RETIRO ATM BP D/MEGA MAXI 1', 'mo_tipo' =&gt; 'D', 'mo_documento' =&gt; '0015258475', 'mo_oficina' =&gt; 'CENTRO DE ACOPIO NORTE', 'mo_monto' =&gt; 100.00  , 'mo_saldo' =&gt; 1935.56, 'mo_fecha_crea' =&gt; new \DateTime('2014-03-26 15:37:38'), 'mo_quien_crea' =&gt; 1, 'mo_fecha_modifica' =&gt; NULL, 'mo_quien_modifica' =&gt; NULL, 'mo_borrado_logico' =&gt; false),</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Actualizando info en el Fixtures
</commit_message>
<xml_diff>
--- a/backup/cuenta_2200555126.xlsx
+++ b/backup/cuenta_2200555126.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="164">
   <si>
     <t>D</t>
   </si>
@@ -501,6 +501,21 @@
   </si>
   <si>
     <t>1907.54</t>
+  </si>
+  <si>
+    <t>0000776328</t>
+  </si>
+  <si>
+    <t>380.88  </t>
+  </si>
+  <si>
+    <t>0000464551</t>
+  </si>
+  <si>
+    <t>1807.54</t>
+  </si>
+  <si>
+    <t>2188.42</t>
   </si>
 </sst>
 </file>
@@ -823,7 +838,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H51"/>
+  <dimension ref="A1:H53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="H1" sqref="H1:H2"/>
@@ -838,56 +853,56 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1">
-        <v>41722</v>
+        <v>41725</v>
       </c>
       <c r="B1" t="s">
-        <v>151</v>
+        <v>3</v>
       </c>
       <c r="C1" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>152</v>
+        <v>159</v>
       </c>
       <c r="E1" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>153</v>
+        <v>160</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>158</v>
+        <v>163</v>
       </c>
       <c r="H1" t="str">
-        <f t="shared" ref="H1:H2" ca="1" si="0">CONCATENATE("array('mo_fecha' =&gt; new \DateTime('",TEXT(A1,"yyyy-mm-dd"),"'), 'mo_concepto' =&gt; '",B1,"', 'mo_tipo' =&gt; '",C1,"', 'mo_documento' =&gt; '",D1,"', 'mo_oficina' =&gt; '",E1,"', 'mo_monto' =&gt; ",TRIM(F1),", 'mo_saldo' =&gt; ",G1,", 'mo_fecha_crea' =&gt; new \DateTime('",TEXT(NOW(),"yyyy-mm-dd H:m:s"),"'), 'mo_quien_crea' =&gt; 1, 'mo_fecha_modifica' =&gt; NULL, 'mo_quien_modifica' =&gt; NULL, 'mo_borrado_logico' =&gt; false),")</f>
-        <v>array('mo_fecha' =&gt; new \DateTime('2014-03-24'), 'mo_concepto' =&gt; 'CONSUMO DATA SUPERMAXI (AV. 6 DE DI', 'mo_tipo' =&gt; 'D', 'mo_documento' =&gt; '0015391688', 'mo_oficina' =&gt; 'INSTITUCIONAL SS.CC.', 'mo_monto' =&gt; 28.02  , 'mo_saldo' =&gt; 1907.54, 'mo_fecha_crea' =&gt; new \DateTime('2014-03-26 15:37:38'), 'mo_quien_crea' =&gt; 1, 'mo_fecha_modifica' =&gt; NULL, 'mo_quien_modifica' =&gt; NULL, 'mo_borrado_logico' =&gt; false),</v>
+        <f t="shared" ref="H1:H4" ca="1" si="0">CONCATENATE("array('mo_fecha' =&gt; new \DateTime('",TEXT(A1,"yyyy-mm-dd"),"'), 'mo_concepto' =&gt; '",B1,"', 'mo_tipo' =&gt; '",C1,"', 'mo_documento' =&gt; '",D1,"', 'mo_oficina' =&gt; '",E1,"', 'mo_monto' =&gt; ",TRIM(F1),", 'mo_saldo' =&gt; ",G1,", 'mo_fecha_crea' =&gt; new \DateTime('",TEXT(NOW(),"yyyy-mm-dd H:m:s"),"'), 'mo_quien_crea' =&gt; 1, 'mo_fecha_modifica' =&gt; NULL, 'mo_quien_modifica' =&gt; NULL, 'mo_borrado_logico' =&gt; false),")</f>
+        <v>array('mo_fecha' =&gt; new \DateTime('2014-03-27'), 'mo_concepto' =&gt; '  TRANSFERENCIA INTERNET', 'mo_tipo' =&gt; 'C', 'mo_documento' =&gt; '0000776328', 'mo_oficina' =&gt; 'AG. NORTE', 'mo_monto' =&gt; 380.88  , 'mo_saldo' =&gt; 2188.42, 'mo_fecha_crea' =&gt; new \DateTime('2014-03-27 8:47:9'), 'mo_quien_crea' =&gt; 1, 'mo_fecha_modifica' =&gt; NULL, 'mo_quien_modifica' =&gt; NULL, 'mo_borrado_logico' =&gt; false),</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>41722</v>
+        <v>41725</v>
       </c>
       <c r="B2" t="s">
-        <v>154</v>
+        <v>144</v>
       </c>
       <c r="C2" t="s">
         <v>0</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>155</v>
+        <v>161</v>
       </c>
       <c r="E2" t="s">
-        <v>156</v>
+        <v>146</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>6</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>157</v>
+        <v>162</v>
       </c>
       <c r="H2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>array('mo_fecha' =&gt; new \DateTime('2014-03-24'), 'mo_concepto' =&gt; 'RETIRO ATM BP D/MEGA MAXI 1', 'mo_tipo' =&gt; 'D', 'mo_documento' =&gt; '0015258475', 'mo_oficina' =&gt; 'CENTRO DE ACOPIO NORTE', 'mo_monto' =&gt; 100.00  , 'mo_saldo' =&gt; 1935.56, 'mo_fecha_crea' =&gt; new \DateTime('2014-03-26 15:37:38'), 'mo_quien_crea' =&gt; 1, 'mo_fecha_modifica' =&gt; NULL, 'mo_quien_modifica' =&gt; NULL, 'mo_borrado_logico' =&gt; false),</v>
+        <v>array('mo_fecha' =&gt; new \DateTime('2014-03-27'), 'mo_concepto' =&gt; 'RETIRO ATM BP D/KENNEDY 3', 'mo_tipo' =&gt; 'D', 'mo_documento' =&gt; '0000464551', 'mo_oficina' =&gt; 'KENNEDY', 'mo_monto' =&gt; 100.00  , 'mo_saldo' =&gt; 1807.54, 'mo_fecha_crea' =&gt; new \DateTime('2014-03-27 8:47:9'), 'mo_quien_crea' =&gt; 1, 'mo_fecha_modifica' =&gt; NULL, 'mo_quien_modifica' =&gt; NULL, 'mo_borrado_logico' =&gt; false),</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -895,22 +910,22 @@
         <v>41722</v>
       </c>
       <c r="B3" t="s">
-        <v>3</v>
+        <v>151</v>
       </c>
       <c r="C3" t="s">
         <v>0</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>143</v>
+        <v>152</v>
       </c>
       <c r="E3" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>9</v>
+        <v>153</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>150</v>
+        <v>158</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -918,157 +933,157 @@
         <v>41722</v>
       </c>
       <c r="B4" t="s">
-        <v>144</v>
+        <v>154</v>
       </c>
       <c r="C4" t="s">
         <v>0</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>145</v>
+        <v>155</v>
       </c>
       <c r="E4" t="s">
-        <v>146</v>
+        <v>156</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>27</v>
+        <v>6</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>149</v>
+        <v>157</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
-        <v>41719</v>
+        <v>41722</v>
       </c>
       <c r="B5" t="s">
-        <v>32</v>
+        <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="E5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
-        <v>41712</v>
+        <v>41722</v>
       </c>
       <c r="B6" t="s">
-        <v>139</v>
+        <v>144</v>
       </c>
       <c r="C6" t="s">
         <v>0</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>140</v>
+        <v>145</v>
       </c>
       <c r="E6" t="s">
-        <v>5</v>
+        <v>146</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>141</v>
+        <v>27</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>142</v>
+        <v>149</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
-        <v>41708</v>
+        <v>41719</v>
       </c>
       <c r="B7" t="s">
-        <v>135</v>
+        <v>32</v>
       </c>
       <c r="C7" t="s">
         <v>4</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>136</v>
+        <v>147</v>
       </c>
       <c r="E7" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="F7" s="3" t="s">
         <v>6</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>138</v>
+        <v>148</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
-        <v>41705</v>
+        <v>41712</v>
       </c>
       <c r="B8" t="s">
-        <v>59</v>
+        <v>139</v>
       </c>
       <c r="C8" t="s">
         <v>0</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="E8" t="s">
         <v>5</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>133</v>
+        <v>141</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>131</v>
+        <v>142</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
-        <v>41703</v>
+        <v>41708</v>
       </c>
       <c r="B9" t="s">
-        <v>3</v>
+        <v>135</v>
       </c>
       <c r="C9" t="s">
         <v>4</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
       <c r="E9" t="s">
         <v>5</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>133</v>
+        <v>6</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
-        <v>41703</v>
+        <v>41705</v>
       </c>
       <c r="B10" t="s">
-        <v>117</v>
+        <v>59</v>
       </c>
       <c r="C10" t="s">
         <v>0</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>118</v>
+        <v>137</v>
       </c>
       <c r="E10" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>119</v>
+        <v>133</v>
       </c>
       <c r="G10" s="3" t="s">
         <v>131</v>
@@ -1079,157 +1094,157 @@
         <v>41703</v>
       </c>
       <c r="B11" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C11" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>120</v>
+        <v>132</v>
       </c>
       <c r="E11" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>121</v>
+        <v>133</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
-        <v>41698</v>
+        <v>41703</v>
       </c>
       <c r="B12" t="s">
-        <v>17</v>
+        <v>117</v>
       </c>
       <c r="C12" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="E12" t="s">
-        <v>19</v>
+        <v>1</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
-        <v>41691</v>
+        <v>41703</v>
       </c>
       <c r="B13" t="s">
-        <v>124</v>
+        <v>2</v>
       </c>
       <c r="C13" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="E13" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>67</v>
+        <v>121</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
-        <v>41691</v>
+        <v>41698</v>
       </c>
       <c r="B14" t="s">
-        <v>124</v>
+        <v>17</v>
       </c>
       <c r="C14" t="s">
         <v>4</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="E14" t="s">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>67</v>
+        <v>123</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
-        <v>41690</v>
+        <v>41691</v>
       </c>
       <c r="B15" t="s">
-        <v>3</v>
+        <v>124</v>
       </c>
       <c r="C15" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>113</v>
+        <v>125</v>
       </c>
       <c r="E15" t="s">
         <v>5</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>114</v>
+        <v>67</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>112</v>
+        <v>128</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
-        <v>41690</v>
+        <v>41691</v>
       </c>
       <c r="B16" t="s">
-        <v>3</v>
+        <v>124</v>
       </c>
       <c r="C16" t="s">
         <v>4</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>115</v>
+        <v>126</v>
       </c>
       <c r="E16" t="s">
         <v>5</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>114</v>
+        <v>67</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>116</v>
+        <v>127</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
-        <v>41682</v>
+        <v>41690</v>
       </c>
       <c r="B17" t="s">
-        <v>106</v>
+        <v>3</v>
       </c>
       <c r="C17" t="s">
         <v>0</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>107</v>
+        <v>113</v>
       </c>
       <c r="E17" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>108</v>
+        <v>114</v>
       </c>
       <c r="G17" s="3" t="s">
         <v>112</v>
@@ -1237,53 +1252,53 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
-        <v>41680</v>
+        <v>41690</v>
       </c>
       <c r="B18" t="s">
-        <v>32</v>
+        <v>3</v>
       </c>
       <c r="C18" t="s">
         <v>4</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>109</v>
+        <v>115</v>
       </c>
       <c r="E18" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
-        <v>41680</v>
+        <v>41682</v>
       </c>
       <c r="B19" t="s">
-        <v>3</v>
+        <v>106</v>
       </c>
       <c r="C19" t="s">
         <v>0</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="E19" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>6</v>
+        <v>108</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>98</v>
+        <v>112</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
-        <v>41677</v>
+        <v>41680</v>
       </c>
       <c r="B20" t="s">
         <v>32</v>
@@ -1292,36 +1307,36 @@
         <v>4</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>99</v>
+        <v>109</v>
       </c>
       <c r="E20" t="s">
         <v>10</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>6</v>
+        <v>110</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>104</v>
+        <v>111</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
-        <v>41677</v>
+        <v>41680</v>
       </c>
       <c r="B21" t="s">
-        <v>59</v>
+        <v>3</v>
       </c>
       <c r="C21" t="s">
         <v>0</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="E21" t="s">
         <v>5</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>101</v>
+        <v>6</v>
       </c>
       <c r="G21" s="3" t="s">
         <v>98</v>
@@ -1329,45 +1344,45 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
-        <v>41676</v>
+        <v>41677</v>
       </c>
       <c r="B22" t="s">
-        <v>3</v>
+        <v>32</v>
       </c>
       <c r="C22" t="s">
         <v>4</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="E22" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>101</v>
+        <v>6</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
-        <v>41674</v>
+        <v>41677</v>
       </c>
       <c r="B23" t="s">
-        <v>95</v>
+        <v>59</v>
       </c>
       <c r="C23" t="s">
         <v>0</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="E23" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="G23" s="3" t="s">
         <v>98</v>
@@ -1375,71 +1390,71 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
-        <v>41670</v>
+        <v>41676</v>
       </c>
       <c r="B24" t="s">
-        <v>17</v>
+        <v>3</v>
       </c>
       <c r="C24" t="s">
         <v>4</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>18</v>
+        <v>102</v>
       </c>
       <c r="E24" t="s">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>20</v>
+        <v>101</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>94</v>
+        <v>103</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
-        <v>41666</v>
+        <v>41674</v>
       </c>
       <c r="B25" t="s">
-        <v>3</v>
+        <v>95</v>
       </c>
       <c r="C25" t="s">
         <v>0</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>21</v>
+        <v>96</v>
       </c>
       <c r="E25" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>71</v>
+        <v>97</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
-        <v>41666</v>
+        <v>41670</v>
       </c>
       <c r="B26" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="C26" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="E26" t="s">
-        <v>1</v>
+        <v>19</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
@@ -1447,22 +1462,22 @@
         <v>41666</v>
       </c>
       <c r="B27" t="s">
-        <v>24</v>
+        <v>3</v>
       </c>
       <c r="C27" t="s">
         <v>0</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="E27" t="s">
-        <v>26</v>
+        <v>5</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>27</v>
+        <v>71</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
@@ -1470,68 +1485,68 @@
         <v>41666</v>
       </c>
       <c r="B28" t="s">
-        <v>28</v>
+        <v>2</v>
       </c>
       <c r="C28" t="s">
         <v>0</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="E28" t="s">
         <v>1</v>
       </c>
       <c r="F28" s="3" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="G28" s="3" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
-        <v>41660</v>
+        <v>41666</v>
       </c>
       <c r="B29" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="C29" t="s">
         <v>0</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="E29" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>9</v>
+        <v>27</v>
       </c>
       <c r="G29" s="3" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
-        <v>41660</v>
+        <v>41666</v>
       </c>
       <c r="B30" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C30" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="E30" t="s">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>6</v>
+        <v>30</v>
       </c>
       <c r="G30" s="3" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
@@ -1539,188 +1554,188 @@
         <v>41660</v>
       </c>
       <c r="B31" t="s">
-        <v>34</v>
+        <v>11</v>
       </c>
       <c r="C31" t="s">
         <v>0</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="E31" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>36</v>
+        <v>9</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
-        <v>41659</v>
+        <v>41660</v>
       </c>
       <c r="B32" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="C32" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="E32" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>39</v>
+        <v>6</v>
       </c>
       <c r="G32" s="3" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
-        <v>41655</v>
+        <v>41660</v>
       </c>
       <c r="B33" t="s">
-        <v>2</v>
+        <v>34</v>
       </c>
       <c r="C33" t="s">
         <v>0</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="E33" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="F33" s="3" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="G33" s="3" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
-        <v>41655</v>
+        <v>41659</v>
       </c>
       <c r="B34" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="C34" t="s">
         <v>0</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="E34" t="s">
-        <v>44</v>
+        <v>1</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>6</v>
+        <v>39</v>
       </c>
       <c r="G34" s="3" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
-        <v>41652</v>
+        <v>41655</v>
       </c>
       <c r="B35" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C35" t="s">
         <v>0</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="E35" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="G35" s="3" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
-        <v>41649</v>
+        <v>41655</v>
       </c>
       <c r="B36" t="s">
-        <v>3</v>
+        <v>42</v>
       </c>
       <c r="C36" t="s">
         <v>0</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>16</v>
+        <v>43</v>
       </c>
       <c r="E36" t="s">
-        <v>5</v>
+        <v>44</v>
       </c>
       <c r="F36" s="3" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="G36" s="3" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
-        <v>41648</v>
+        <v>41652</v>
       </c>
       <c r="B37" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C37" t="s">
         <v>0</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E37" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F37" s="3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="G37" s="3" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
-        <v>41648</v>
+        <v>41649</v>
       </c>
       <c r="B38" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C38" t="s">
         <v>0</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>49</v>
+        <v>16</v>
       </c>
       <c r="E38" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F38" s="3" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="G38" s="3" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
-        <v>41647</v>
+        <v>41648</v>
       </c>
       <c r="B39" t="s">
         <v>2</v>
@@ -1729,62 +1744,62 @@
         <v>0</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="E39" t="s">
         <v>1</v>
       </c>
       <c r="F39" s="3" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="G39" s="3" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
-        <v>41646</v>
+        <v>41648</v>
       </c>
       <c r="B40" t="s">
-        <v>52</v>
+        <v>7</v>
       </c>
       <c r="C40" t="s">
         <v>0</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="E40" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F40" s="3" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="G40" s="3" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
-        <v>41646</v>
+        <v>41647</v>
       </c>
       <c r="B41" t="s">
-        <v>54</v>
+        <v>2</v>
       </c>
       <c r="C41" t="s">
         <v>0</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="E41" t="s">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="F41" s="3" t="s">
-        <v>14</v>
+        <v>51</v>
       </c>
       <c r="G41" s="3" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
@@ -1792,22 +1807,22 @@
         <v>41646</v>
       </c>
       <c r="B42" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C42" t="s">
         <v>0</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="E42" t="s">
         <v>12</v>
       </c>
       <c r="F42" s="3" t="s">
-        <v>58</v>
+        <v>13</v>
       </c>
       <c r="G42" s="3" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
@@ -1815,98 +1830,138 @@
         <v>41646</v>
       </c>
       <c r="B43" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="C43" t="s">
         <v>0</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="E43" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="F43" s="3" t="s">
-        <v>61</v>
+        <v>14</v>
       </c>
       <c r="G43" s="3" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
-        <v>41645</v>
+        <v>41646</v>
       </c>
       <c r="B44" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="C44" t="s">
         <v>0</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="E44" t="s">
-        <v>64</v>
+        <v>12</v>
       </c>
       <c r="F44" s="3" t="s">
-        <v>9</v>
+        <v>58</v>
       </c>
       <c r="G44" s="3" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
-        <v>41642</v>
+        <v>41646</v>
       </c>
       <c r="B45" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="C45" t="s">
         <v>0</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="E45" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="F45" s="3" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="G45" s="3" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
+        <v>41645</v>
+      </c>
+      <c r="B46" t="s">
+        <v>62</v>
+      </c>
+      <c r="C46" t="s">
+        <v>0</v>
+      </c>
+      <c r="D46" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="E46" t="s">
+        <v>64</v>
+      </c>
+      <c r="F46" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G46" s="3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A47" s="1">
+        <v>41642</v>
+      </c>
+      <c r="B47" t="s">
+        <v>65</v>
+      </c>
+      <c r="C47" t="s">
+        <v>0</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="E47" t="s">
+        <v>10</v>
+      </c>
+      <c r="F47" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="G47" s="3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A48" s="1">
         <v>41641</v>
       </c>
-      <c r="B46" t="s">
+      <c r="B48" t="s">
         <v>68</v>
       </c>
-      <c r="C46" t="s">
-        <v>0</v>
-      </c>
-      <c r="D46" s="2" t="s">
+      <c r="C48" t="s">
+        <v>0</v>
+      </c>
+      <c r="D48" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="E46" t="s">
+      <c r="E48" t="s">
         <v>1</v>
       </c>
-      <c r="F46" s="3" t="s">
+      <c r="F48" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="G46" s="3" t="s">
+      <c r="G48" s="3" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A47" s="1"/>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A48" s="1"/>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" s="1"/>
@@ -1916,6 +1971,12 @@
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" s="1"/>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A52" s="1"/>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A53" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Corrigiendo errores en peticiones Ajax
</commit_message>
<xml_diff>
--- a/backup/cuenta_2200555126.xlsx
+++ b/backup/cuenta_2200555126.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\xampp\htdocs\dml2\backup\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\php-projects\dml2\backup\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -874,8 +874,8 @@
         <v>163</v>
       </c>
       <c r="H1" t="str">
-        <f t="shared" ref="H1:H4" ca="1" si="0">CONCATENATE("array('mo_fecha' =&gt; new \DateTime('",TEXT(A1,"yyyy-mm-dd"),"'), 'mo_concepto' =&gt; '",B1,"', 'mo_tipo' =&gt; '",C1,"', 'mo_documento' =&gt; '",D1,"', 'mo_oficina' =&gt; '",E1,"', 'mo_monto' =&gt; ",TRIM(F1),", 'mo_saldo' =&gt; ",G1,", 'mo_fecha_crea' =&gt; new \DateTime('",TEXT(NOW(),"yyyy-mm-dd H:m:s"),"'), 'mo_quien_crea' =&gt; 1, 'mo_fecha_modifica' =&gt; NULL, 'mo_quien_modifica' =&gt; NULL, 'mo_borrado_logico' =&gt; false),")</f>
-        <v>array('mo_fecha' =&gt; new \DateTime('2014-03-27'), 'mo_concepto' =&gt; '  TRANSFERENCIA INTERNET', 'mo_tipo' =&gt; 'C', 'mo_documento' =&gt; '0000776328', 'mo_oficina' =&gt; 'AG. NORTE', 'mo_monto' =&gt; 380.88  , 'mo_saldo' =&gt; 2188.42, 'mo_fecha_crea' =&gt; new \DateTime('2014-03-27 8:47:9'), 'mo_quien_crea' =&gt; 1, 'mo_fecha_modifica' =&gt; NULL, 'mo_quien_modifica' =&gt; NULL, 'mo_borrado_logico' =&gt; false),</v>
+        <f t="shared" ref="H1:H2" ca="1" si="0">CONCATENATE("array('mo_fecha' =&gt; new \DateTime('",TEXT(A1,"yyyy-mm-dd"),"'), 'mo_concepto' =&gt; '",B1,"', 'mo_tipo' =&gt; '",C1,"', 'mo_documento' =&gt; '",D1,"', 'mo_oficina' =&gt; '",E1,"', 'mo_monto' =&gt; ",TRIM(F1),", 'mo_saldo' =&gt; ",G1,", 'mo_fecha_crea' =&gt; new \DateTime('",TEXT(NOW(),"yyyy-mm-dd H:m:s"),"'), 'mo_quien_crea' =&gt; 1, 'mo_fecha_modifica' =&gt; NULL, 'mo_quien_modifica' =&gt; NULL, 'mo_borrado_logico' =&gt; false),")</f>
+        <v>array('mo_fecha' =&gt; new \DateTime('2014-03-27'), 'mo_concepto' =&gt; '  TRANSFERENCIA INTERNET', 'mo_tipo' =&gt; 'C', 'mo_documento' =&gt; '0000776328', 'mo_oficina' =&gt; 'AG. NORTE', 'mo_monto' =&gt; 380.88  , 'mo_saldo' =&gt; 2188.42, 'mo_fecha_crea' =&gt; new \DateTime('2014-03-27 21:16:14'), 'mo_quien_crea' =&gt; 1, 'mo_fecha_modifica' =&gt; NULL, 'mo_quien_modifica' =&gt; NULL, 'mo_borrado_logico' =&gt; false),</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -902,7 +902,7 @@
       </c>
       <c r="H2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>array('mo_fecha' =&gt; new \DateTime('2014-03-27'), 'mo_concepto' =&gt; 'RETIRO ATM BP D/KENNEDY 3', 'mo_tipo' =&gt; 'D', 'mo_documento' =&gt; '0000464551', 'mo_oficina' =&gt; 'KENNEDY', 'mo_monto' =&gt; 100.00  , 'mo_saldo' =&gt; 1807.54, 'mo_fecha_crea' =&gt; new \DateTime('2014-03-27 8:47:9'), 'mo_quien_crea' =&gt; 1, 'mo_fecha_modifica' =&gt; NULL, 'mo_quien_modifica' =&gt; NULL, 'mo_borrado_logico' =&gt; false),</v>
+        <v>array('mo_fecha' =&gt; new \DateTime('2014-03-27'), 'mo_concepto' =&gt; 'RETIRO ATM BP D/KENNEDY 3', 'mo_tipo' =&gt; 'D', 'mo_documento' =&gt; '0000464551', 'mo_oficina' =&gt; 'KENNEDY', 'mo_monto' =&gt; 100.00  , 'mo_saldo' =&gt; 1807.54, 'mo_fecha_crea' =&gt; new \DateTime('2014-03-27 21:16:14'), 'mo_quien_crea' =&gt; 1, 'mo_fecha_modifica' =&gt; NULL, 'mo_quien_modifica' =&gt; NULL, 'mo_borrado_logico' =&gt; false),</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Agregando la inserción de datos con ajax
</commit_message>
<xml_diff>
--- a/backup/cuenta_2200555126.xlsx
+++ b/backup/cuenta_2200555126.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="414" uniqueCount="219">
   <si>
     <t>D</t>
   </si>
@@ -573,6 +573,114 @@
   </si>
   <si>
     <t>2109.09</t>
+  </si>
+  <si>
+    <t>0004566186</t>
+  </si>
+  <si>
+    <t>1509.09</t>
+  </si>
+  <si>
+    <t>CONSUMO DATA FYBECA TORRES MEDICAS</t>
+  </si>
+  <si>
+    <t>0004017189</t>
+  </si>
+  <si>
+    <t>3.37  </t>
+  </si>
+  <si>
+    <t>0002026113</t>
+  </si>
+  <si>
+    <t>CONSUMO DATA FYBECA (PLAZA DE TOROS</t>
+  </si>
+  <si>
+    <t>0008586167</t>
+  </si>
+  <si>
+    <t>26.80  </t>
+  </si>
+  <si>
+    <t>0008502524</t>
+  </si>
+  <si>
+    <t>1459.09</t>
+  </si>
+  <si>
+    <t>1432.29</t>
+  </si>
+  <si>
+    <t>1232.29</t>
+  </si>
+  <si>
+    <t>1228.92</t>
+  </si>
+  <si>
+    <t>RETIRO ATM BP D/REINA VICTORIA</t>
+  </si>
+  <si>
+    <t>0000990490</t>
+  </si>
+  <si>
+    <t>748.22</t>
+  </si>
+  <si>
+    <t>0008775881</t>
+  </si>
+  <si>
+    <t>768.22</t>
+  </si>
+  <si>
+    <t>0004392772</t>
+  </si>
+  <si>
+    <t>41.58  </t>
+  </si>
+  <si>
+    <t>718.22</t>
+  </si>
+  <si>
+    <t>0002223892</t>
+  </si>
+  <si>
+    <t>2.31  </t>
+  </si>
+  <si>
+    <t>759.80</t>
+  </si>
+  <si>
+    <t>0002195122</t>
+  </si>
+  <si>
+    <t>38.19  </t>
+  </si>
+  <si>
+    <t>762.11</t>
+  </si>
+  <si>
+    <t>0007431020</t>
+  </si>
+  <si>
+    <t>800.30</t>
+  </si>
+  <si>
+    <t>0007349236</t>
+  </si>
+  <si>
+    <t>243.19  </t>
+  </si>
+  <si>
+    <t>900.30</t>
+  </si>
+  <si>
+    <t>0002730824</t>
+  </si>
+  <si>
+    <t>85.43  </t>
+  </si>
+  <si>
+    <t>1143.49</t>
   </si>
 </sst>
 </file>
@@ -895,10 +1003,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H61"/>
+  <dimension ref="A1:H74"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1:H4"/>
+      <selection activeCell="H1" sqref="H1:H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -910,299 +1018,315 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1">
-        <v>41737</v>
+        <v>41746</v>
       </c>
       <c r="B1" t="s">
-        <v>3</v>
+        <v>197</v>
       </c>
       <c r="C1" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>173</v>
+        <v>198</v>
       </c>
       <c r="E1" t="s">
-        <v>5</v>
+        <v>156</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>174</v>
+        <v>9</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>181</v>
+        <v>199</v>
       </c>
       <c r="H1" t="str">
-        <f t="shared" ref="H1:H4" ca="1" si="0">CONCATENATE("array('mo_fecha' =&gt; new \DateTime('",TEXT(A1,"yyyy-mm-dd"),"'), 'mo_concepto' =&gt; '",B1,"', 'mo_tipo' =&gt; '",C1,"', 'mo_documento' =&gt; '",D1,"', 'mo_oficina' =&gt; '",E1,"', 'mo_monto' =&gt; ",TRIM(F1),", 'mo_saldo' =&gt; ",G1,", 'mo_fecha_crea' =&gt; new \DateTime('",TEXT(NOW(),"yyyy-mm-dd H:m:s"),"'), 'mo_quien_crea' =&gt; 1, 'mo_fecha_modifica' =&gt; NULL, 'mo_quien_modifica' =&gt; NULL, 'mo_borrado_logico' =&gt; false),")</f>
-        <v>array('mo_fecha' =&gt; new \DateTime('2014-04-08'), 'mo_concepto' =&gt; '  TRANSFERENCIA INTERNET', 'mo_tipo' =&gt; 'C', 'mo_documento' =&gt; '0006550584', 'mo_oficina' =&gt; 'AG. NORTE', 'mo_monto' =&gt; 400.00  , 'mo_saldo' =&gt; 2509.09, 'mo_fecha_crea' =&gt; new \DateTime('2014-04-08 16:14:10'), 'mo_quien_crea' =&gt; 1, 'mo_fecha_modifica' =&gt; NULL, 'mo_quien_modifica' =&gt; NULL, 'mo_borrado_logico' =&gt; false),</v>
+        <f t="shared" ref="H1:H8" ca="1" si="0">CONCATENATE("array('mo_fecha' =&gt; new \DateTime('",TEXT(A1,"yyyy-mm-dd"),"'), 'mo_concepto' =&gt; '",B1,"', 'mo_tipo' =&gt; '",C1,"', 'mo_documento' =&gt; '",D1,"', 'mo_oficina' =&gt; '",E1,"', 'mo_monto' =&gt; ",TRIM(F1),", 'mo_saldo' =&gt; ",G1,", 'mo_fecha_crea' =&gt; new \DateTime('",TEXT(NOW(),"yyyy-mm-dd H:m:s"),"'), 'mo_quien_crea' =&gt; 1, 'mo_fecha_modifica' =&gt; NULL, 'mo_quien_modifica' =&gt; NULL, 'mo_borrado_logico' =&gt; false),")</f>
+        <v>array('mo_fecha' =&gt; new \DateTime('2014-04-17'), 'mo_concepto' =&gt; 'RETIRO ATM BP D/REINA VICTORIA', 'mo_tipo' =&gt; 'D', 'mo_documento' =&gt; '0000990490', 'mo_oficina' =&gt; 'CENTRO DE ACOPIO NORTE', 'mo_monto' =&gt; 20.00  , 'mo_saldo' =&gt; 748.22, 'mo_fecha_crea' =&gt; new \DateTime('2014-04-18 13:44:39'), 'mo_quien_crea' =&gt; 1, 'mo_fecha_modifica' =&gt; NULL, 'mo_quien_modifica' =&gt; NULL, 'mo_borrado_logico' =&gt; false),</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>41736</v>
+        <v>41744</v>
       </c>
       <c r="B2" t="s">
-        <v>175</v>
+        <v>135</v>
       </c>
       <c r="C2" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>176</v>
+        <v>200</v>
       </c>
       <c r="E2" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>174</v>
+        <v>67</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>182</v>
+        <v>201</v>
       </c>
       <c r="H2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>array('mo_fecha' =&gt; new \DateTime('2014-04-07'), 'mo_concepto' =&gt; 'CONSUMO VISA NA UNIVERSIDAD POLITECNIC', 'mo_tipo' =&gt; 'D', 'mo_documento' =&gt; '0008014779', 'mo_oficina' =&gt; 'INSTITUCIONAL SS.CC.', 'mo_monto' =&gt; 400.00  , 'mo_saldo' =&gt; 2109.09, 'mo_fecha_crea' =&gt; new \DateTime('2014-04-08 16:14:10'), 'mo_quien_crea' =&gt; 1, 'mo_fecha_modifica' =&gt; NULL, 'mo_quien_modifica' =&gt; NULL, 'mo_borrado_logico' =&gt; false),</v>
+        <v>array('mo_fecha' =&gt; new \DateTime('2014-04-15'), 'mo_concepto' =&gt; 'DEP CNB-1500415029001', 'mo_tipo' =&gt; 'C', 'mo_documento' =&gt; '0008775881', 'mo_oficina' =&gt; 'AG. NORTE', 'mo_monto' =&gt; 50.00  , 'mo_saldo' =&gt; 768.22, 'mo_fecha_crea' =&gt; new \DateTime('2014-04-18 13:44:39'), 'mo_quien_crea' =&gt; 1, 'mo_fecha_modifica' =&gt; NULL, 'mo_quien_modifica' =&gt; NULL, 'mo_borrado_logico' =&gt; false),</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>41736</v>
+        <v>41744</v>
       </c>
       <c r="B3" t="s">
-        <v>59</v>
+        <v>189</v>
       </c>
       <c r="C3" t="s">
         <v>0</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>177</v>
+        <v>202</v>
       </c>
       <c r="E3" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>178</v>
+        <v>203</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>181</v>
+        <v>204</v>
       </c>
       <c r="H3" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>array('mo_fecha' =&gt; new \DateTime('2014-04-07'), 'mo_concepto' =&gt; 'PAGO PRESTAMO', 'mo_tipo' =&gt; 'D', 'mo_documento' =&gt; '0006767712', 'mo_oficina' =&gt; 'AG. NORTE', 'mo_monto' =&gt; 280.88  , 'mo_saldo' =&gt; 2509.09, 'mo_fecha_crea' =&gt; new \DateTime('2014-04-08 16:14:10'), 'mo_quien_crea' =&gt; 1, 'mo_fecha_modifica' =&gt; NULL, 'mo_quien_modifica' =&gt; NULL, 'mo_borrado_logico' =&gt; false),</v>
+        <v>array('mo_fecha' =&gt; new \DateTime('2014-04-15'), 'mo_concepto' =&gt; 'CONSUMO DATA FYBECA (PLAZA DE TOROS', 'mo_tipo' =&gt; 'D', 'mo_documento' =&gt; '0004392772', 'mo_oficina' =&gt; 'INSTITUCIONAL SS.CC.', 'mo_monto' =&gt; 41.58  , 'mo_saldo' =&gt; 718.22, 'mo_fecha_crea' =&gt; new \DateTime('2014-04-18 13:44:39'), 'mo_quien_crea' =&gt; 1, 'mo_fecha_modifica' =&gt; NULL, 'mo_quien_modifica' =&gt; NULL, 'mo_borrado_logico' =&gt; false),</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
-        <v>41736</v>
+        <v>41744</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>185</v>
       </c>
       <c r="C4" t="s">
         <v>0</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>179</v>
+        <v>205</v>
       </c>
       <c r="E4" t="s">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>174</v>
+        <v>206</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>180</v>
+        <v>207</v>
       </c>
       <c r="H4" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>array('mo_fecha' =&gt; new \DateTime('2014-04-07'), 'mo_concepto' =&gt; 'RETIRO ATM BP N/EL GIRON-3', 'mo_tipo' =&gt; 'D', 'mo_documento' =&gt; '0006696624', 'mo_oficina' =&gt; 'EL GIRON', 'mo_monto' =&gt; 400.00  , 'mo_saldo' =&gt; 2789.97, 'mo_fecha_crea' =&gt; new \DateTime('2014-04-08 16:14:10'), 'mo_quien_crea' =&gt; 1, 'mo_fecha_modifica' =&gt; NULL, 'mo_quien_modifica' =&gt; NULL, 'mo_borrado_logico' =&gt; false),</v>
+        <v>array('mo_fecha' =&gt; new \DateTime('2014-04-15'), 'mo_concepto' =&gt; 'CONSUMO DATA FYBECA TORRES MEDICAS', 'mo_tipo' =&gt; 'D', 'mo_documento' =&gt; '0002223892', 'mo_oficina' =&gt; 'INSTITUCIONAL SS.CC.', 'mo_monto' =&gt; 2.31  , 'mo_saldo' =&gt; 759.80, 'mo_fecha_crea' =&gt; new \DateTime('2014-04-18 13:44:39'), 'mo_quien_crea' =&gt; 1, 'mo_fecha_modifica' =&gt; NULL, 'mo_quien_modifica' =&gt; NULL, 'mo_borrado_logico' =&gt; false),</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
-        <v>41731</v>
+        <v>41744</v>
       </c>
       <c r="B5" t="s">
-        <v>3</v>
+        <v>185</v>
       </c>
       <c r="C5" t="s">
         <v>0</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>167</v>
+        <v>208</v>
       </c>
       <c r="E5" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>15</v>
+        <v>209</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>171</v>
+        <v>210</v>
+      </c>
+      <c r="H5" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>array('mo_fecha' =&gt; new \DateTime('2014-04-15'), 'mo_concepto' =&gt; 'CONSUMO DATA FYBECA TORRES MEDICAS', 'mo_tipo' =&gt; 'D', 'mo_documento' =&gt; '0002195122', 'mo_oficina' =&gt; 'INSTITUCIONAL SS.CC.', 'mo_monto' =&gt; 38.19  , 'mo_saldo' =&gt; 762.11, 'mo_fecha_crea' =&gt; new \DateTime('2014-04-18 13:44:39'), 'mo_quien_crea' =&gt; 1, 'mo_fecha_modifica' =&gt; NULL, 'mo_quien_modifica' =&gt; NULL, 'mo_borrado_logico' =&gt; false),</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
-        <v>41731</v>
+        <v>41743</v>
       </c>
       <c r="B6" t="s">
-        <v>32</v>
+        <v>3</v>
       </c>
       <c r="C6" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>168</v>
+        <v>211</v>
       </c>
       <c r="E6" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>172</v>
+        <v>212</v>
+      </c>
+      <c r="H6" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>array('mo_fecha' =&gt; new \DateTime('2014-04-14'), 'mo_concepto' =&gt; '  TRANSFERENCIA INTERNET', 'mo_tipo' =&gt; 'D', 'mo_documento' =&gt; '0007431020', 'mo_oficina' =&gt; 'AG. NORTE', 'mo_monto' =&gt; 100.00  , 'mo_saldo' =&gt; 800.30, 'mo_fecha_crea' =&gt; new \DateTime('2014-04-18 13:44:39'), 'mo_quien_crea' =&gt; 1, 'mo_fecha_modifica' =&gt; NULL, 'mo_quien_modifica' =&gt; NULL, 'mo_borrado_logico' =&gt; false),</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
-        <v>41729</v>
+        <v>41743</v>
       </c>
       <c r="B7" t="s">
-        <v>17</v>
+        <v>3</v>
       </c>
       <c r="C7" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>169</v>
+        <v>213</v>
       </c>
       <c r="E7" t="s">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>170</v>
+        <v>214</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>171</v>
+        <v>215</v>
+      </c>
+      <c r="H7" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>array('mo_fecha' =&gt; new \DateTime('2014-04-14'), 'mo_concepto' =&gt; '  TRANSFERENCIA INTERNET', 'mo_tipo' =&gt; 'D', 'mo_documento' =&gt; '0007349236', 'mo_oficina' =&gt; 'AG. NORTE', 'mo_monto' =&gt; 243.19  , 'mo_saldo' =&gt; 900.30, 'mo_fecha_crea' =&gt; new \DateTime('2014-04-18 13:44:39'), 'mo_quien_crea' =&gt; 1, 'mo_fecha_modifica' =&gt; NULL, 'mo_quien_modifica' =&gt; NULL, 'mo_borrado_logico' =&gt; false),</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
-        <v>41729</v>
+        <v>41743</v>
       </c>
       <c r="B8" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C8" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>164</v>
+        <v>216</v>
       </c>
       <c r="E8" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>165</v>
+        <v>217</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>166</v>
+        <v>218</v>
+      </c>
+      <c r="H8" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>array('mo_fecha' =&gt; new \DateTime('2014-04-14'), 'mo_concepto' =&gt; 'CONSUMO DATA AKI MOLINEROS 161', 'mo_tipo' =&gt; 'D', 'mo_documento' =&gt; '0002730824', 'mo_oficina' =&gt; 'INSTITUCIONAL SS.CC.', 'mo_monto' =&gt; 85.43  , 'mo_saldo' =&gt; 1143.49, 'mo_fecha_crea' =&gt; new \DateTime('2014-04-18 13:44:39'), 'mo_quien_crea' =&gt; 1, 'mo_fecha_modifica' =&gt; NULL, 'mo_quien_modifica' =&gt; NULL, 'mo_borrado_logico' =&gt; false),</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
-        <v>41725</v>
+        <v>41740</v>
       </c>
       <c r="B9" t="s">
-        <v>3</v>
+        <v>185</v>
       </c>
       <c r="C9" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>159</v>
+        <v>186</v>
       </c>
       <c r="E9" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>160</v>
+        <v>187</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>163</v>
+        <v>196</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
-        <v>41725</v>
+        <v>41740</v>
       </c>
       <c r="B10" t="s">
-        <v>144</v>
+        <v>42</v>
       </c>
       <c r="C10" t="s">
         <v>0</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>161</v>
+        <v>188</v>
       </c>
       <c r="E10" t="s">
-        <v>146</v>
+        <v>44</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>162</v>
+        <v>195</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
-        <v>41722</v>
+        <v>41739</v>
       </c>
       <c r="B11" t="s">
-        <v>151</v>
+        <v>189</v>
       </c>
       <c r="C11" t="s">
         <v>0</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>152</v>
+        <v>190</v>
       </c>
       <c r="E11" t="s">
         <v>1</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>153</v>
+        <v>191</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>158</v>
+        <v>194</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
-        <v>41722</v>
+        <v>41739</v>
       </c>
       <c r="B12" t="s">
-        <v>154</v>
+        <v>42</v>
       </c>
       <c r="C12" t="s">
         <v>0</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>155</v>
+        <v>192</v>
       </c>
       <c r="E12" t="s">
-        <v>156</v>
+        <v>44</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>6</v>
+        <v>67</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>157</v>
+        <v>193</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
-        <v>41722</v>
+        <v>41738</v>
       </c>
       <c r="B13" t="s">
         <v>3</v>
@@ -1211,343 +1335,343 @@
         <v>0</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>143</v>
+        <v>183</v>
       </c>
       <c r="E13" t="s">
         <v>5</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>9</v>
+        <v>165</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>150</v>
+        <v>184</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
-        <v>41722</v>
+        <v>41737</v>
       </c>
       <c r="B14" t="s">
-        <v>144</v>
+        <v>3</v>
       </c>
       <c r="C14" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>145</v>
+        <v>173</v>
       </c>
       <c r="E14" t="s">
-        <v>146</v>
+        <v>5</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>27</v>
+        <v>174</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>149</v>
+        <v>181</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
-        <v>41719</v>
+        <v>41736</v>
       </c>
       <c r="B15" t="s">
-        <v>32</v>
+        <v>175</v>
       </c>
       <c r="C15" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>147</v>
+        <v>176</v>
       </c>
       <c r="E15" t="s">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>6</v>
+        <v>174</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>148</v>
+        <v>182</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
-        <v>41712</v>
+        <v>41736</v>
       </c>
       <c r="B16" t="s">
-        <v>139</v>
+        <v>59</v>
       </c>
       <c r="C16" t="s">
         <v>0</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>140</v>
+        <v>177</v>
       </c>
       <c r="E16" t="s">
         <v>5</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>141</v>
+        <v>178</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>142</v>
+        <v>181</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
-        <v>41708</v>
+        <v>41736</v>
       </c>
       <c r="B17" t="s">
-        <v>135</v>
+        <v>7</v>
       </c>
       <c r="C17" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>136</v>
+        <v>179</v>
       </c>
       <c r="E17" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>6</v>
+        <v>174</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>138</v>
+        <v>180</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
-        <v>41705</v>
+        <v>41731</v>
       </c>
       <c r="B18" t="s">
-        <v>59</v>
+        <v>3</v>
       </c>
       <c r="C18" t="s">
         <v>0</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>137</v>
+        <v>167</v>
       </c>
       <c r="E18" t="s">
         <v>5</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>133</v>
+        <v>15</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>131</v>
+        <v>171</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
-        <v>41703</v>
+        <v>41731</v>
       </c>
       <c r="B19" t="s">
-        <v>3</v>
+        <v>32</v>
       </c>
       <c r="C19" t="s">
         <v>4</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>132</v>
+        <v>168</v>
       </c>
       <c r="E19" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>133</v>
+        <v>15</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>134</v>
+        <v>172</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
-        <v>41703</v>
+        <v>41729</v>
       </c>
       <c r="B20" t="s">
-        <v>117</v>
+        <v>17</v>
       </c>
       <c r="C20" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>118</v>
+        <v>169</v>
       </c>
       <c r="E20" t="s">
-        <v>1</v>
+        <v>19</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>119</v>
+        <v>170</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>131</v>
+        <v>171</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
-        <v>41703</v>
+        <v>41729</v>
       </c>
       <c r="B21" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C21" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>120</v>
+        <v>164</v>
       </c>
       <c r="E21" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>121</v>
+        <v>165</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>130</v>
+        <v>166</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
-        <v>41698</v>
+        <v>41725</v>
       </c>
       <c r="B22" t="s">
-        <v>17</v>
+        <v>3</v>
       </c>
       <c r="C22" t="s">
         <v>4</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>122</v>
+        <v>159</v>
       </c>
       <c r="E22" t="s">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>123</v>
+        <v>160</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>129</v>
+        <v>163</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
-        <v>41691</v>
+        <v>41725</v>
       </c>
       <c r="B23" t="s">
-        <v>124</v>
+        <v>144</v>
       </c>
       <c r="C23" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>125</v>
+        <v>161</v>
       </c>
       <c r="E23" t="s">
-        <v>5</v>
+        <v>146</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>67</v>
+        <v>6</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>128</v>
+        <v>162</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
-        <v>41691</v>
+        <v>41722</v>
       </c>
       <c r="B24" t="s">
-        <v>124</v>
+        <v>151</v>
       </c>
       <c r="C24" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>126</v>
+        <v>152</v>
       </c>
       <c r="E24" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>67</v>
+        <v>153</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>127</v>
+        <v>158</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
-        <v>41690</v>
+        <v>41722</v>
       </c>
       <c r="B25" t="s">
-        <v>3</v>
+        <v>154</v>
       </c>
       <c r="C25" t="s">
         <v>0</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>113</v>
+        <v>155</v>
       </c>
       <c r="E25" t="s">
-        <v>5</v>
+        <v>156</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>114</v>
+        <v>6</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>112</v>
+        <v>157</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
-        <v>41690</v>
+        <v>41722</v>
       </c>
       <c r="B26" t="s">
         <v>3</v>
       </c>
       <c r="C26" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>115</v>
+        <v>143</v>
       </c>
       <c r="E26" t="s">
         <v>5</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>114</v>
+        <v>9</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>116</v>
+        <v>150</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
-        <v>41682</v>
+        <v>41722</v>
       </c>
       <c r="B27" t="s">
-        <v>106</v>
+        <v>144</v>
       </c>
       <c r="C27" t="s">
         <v>0</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>107</v>
+        <v>145</v>
       </c>
       <c r="E27" t="s">
-        <v>12</v>
+        <v>146</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>108</v>
+        <v>27</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>112</v>
+        <v>149</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
-        <v>41680</v>
+        <v>41719</v>
       </c>
       <c r="B28" t="s">
         <v>32</v>
@@ -1556,67 +1680,67 @@
         <v>4</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>109</v>
+        <v>147</v>
       </c>
       <c r="E28" t="s">
         <v>10</v>
       </c>
       <c r="F28" s="3" t="s">
-        <v>110</v>
+        <v>6</v>
       </c>
       <c r="G28" s="3" t="s">
-        <v>111</v>
+        <v>148</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
-        <v>41680</v>
+        <v>41712</v>
       </c>
       <c r="B29" t="s">
-        <v>3</v>
+        <v>139</v>
       </c>
       <c r="C29" t="s">
         <v>0</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>105</v>
+        <v>140</v>
       </c>
       <c r="E29" t="s">
         <v>5</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>6</v>
+        <v>141</v>
       </c>
       <c r="G29" s="3" t="s">
-        <v>98</v>
+        <v>142</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
-        <v>41677</v>
+        <v>41708</v>
       </c>
       <c r="B30" t="s">
-        <v>32</v>
+        <v>135</v>
       </c>
       <c r="C30" t="s">
         <v>4</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>99</v>
+        <v>136</v>
       </c>
       <c r="E30" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="F30" s="3" t="s">
         <v>6</v>
       </c>
       <c r="G30" s="3" t="s">
-        <v>104</v>
+        <v>138</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
-        <v>41677</v>
+        <v>41705</v>
       </c>
       <c r="B31" t="s">
         <v>59</v>
@@ -1625,21 +1749,21 @@
         <v>0</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>100</v>
+        <v>137</v>
       </c>
       <c r="E31" t="s">
         <v>5</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>101</v>
+        <v>133</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>98</v>
+        <v>131</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
-        <v>41676</v>
+        <v>41703</v>
       </c>
       <c r="B32" t="s">
         <v>3</v>
@@ -1648,389 +1772,389 @@
         <v>4</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>102</v>
+        <v>132</v>
       </c>
       <c r="E32" t="s">
         <v>5</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>101</v>
+        <v>133</v>
       </c>
       <c r="G32" s="3" t="s">
-        <v>103</v>
+        <v>134</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
-        <v>41674</v>
+        <v>41703</v>
       </c>
       <c r="B33" t="s">
-        <v>95</v>
+        <v>117</v>
       </c>
       <c r="C33" t="s">
         <v>0</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>96</v>
+        <v>118</v>
       </c>
       <c r="E33" t="s">
         <v>1</v>
       </c>
       <c r="F33" s="3" t="s">
-        <v>97</v>
+        <v>119</v>
       </c>
       <c r="G33" s="3" t="s">
-        <v>98</v>
+        <v>131</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
-        <v>41670</v>
+        <v>41703</v>
       </c>
       <c r="B34" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="C34" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>18</v>
+        <v>120</v>
       </c>
       <c r="E34" t="s">
-        <v>19</v>
+        <v>1</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>20</v>
+        <v>121</v>
       </c>
       <c r="G34" s="3" t="s">
-        <v>94</v>
+        <v>130</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
-        <v>41666</v>
+        <v>41698</v>
       </c>
       <c r="B35" t="s">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="C35" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>21</v>
+        <v>122</v>
       </c>
       <c r="E35" t="s">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>71</v>
+        <v>123</v>
       </c>
       <c r="G35" s="3" t="s">
-        <v>93</v>
+        <v>129</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
-        <v>41666</v>
+        <v>41691</v>
       </c>
       <c r="B36" t="s">
-        <v>2</v>
+        <v>124</v>
       </c>
       <c r="C36" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>22</v>
+        <v>125</v>
       </c>
       <c r="E36" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F36" s="3" t="s">
-        <v>23</v>
+        <v>67</v>
       </c>
       <c r="G36" s="3" t="s">
-        <v>92</v>
+        <v>128</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
-        <v>41666</v>
+        <v>41691</v>
       </c>
       <c r="B37" t="s">
-        <v>24</v>
+        <v>124</v>
       </c>
       <c r="C37" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>25</v>
+        <v>126</v>
       </c>
       <c r="E37" t="s">
-        <v>26</v>
+        <v>5</v>
       </c>
       <c r="F37" s="3" t="s">
-        <v>27</v>
+        <v>67</v>
       </c>
       <c r="G37" s="3" t="s">
-        <v>91</v>
+        <v>127</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
-        <v>41666</v>
+        <v>41690</v>
       </c>
       <c r="B38" t="s">
-        <v>28</v>
+        <v>3</v>
       </c>
       <c r="C38" t="s">
         <v>0</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>29</v>
+        <v>113</v>
       </c>
       <c r="E38" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F38" s="3" t="s">
-        <v>30</v>
+        <v>114</v>
       </c>
       <c r="G38" s="3" t="s">
-        <v>90</v>
+        <v>112</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
-        <v>41660</v>
+        <v>41690</v>
       </c>
       <c r="B39" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="C39" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>31</v>
+        <v>115</v>
       </c>
       <c r="E39" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F39" s="3" t="s">
-        <v>9</v>
+        <v>114</v>
       </c>
       <c r="G39" s="3" t="s">
-        <v>89</v>
+        <v>116</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
-        <v>41660</v>
+        <v>41682</v>
       </c>
       <c r="B40" t="s">
-        <v>32</v>
+        <v>106</v>
       </c>
       <c r="C40" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>33</v>
+        <v>107</v>
       </c>
       <c r="E40" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F40" s="3" t="s">
-        <v>6</v>
+        <v>108</v>
       </c>
       <c r="G40" s="3" t="s">
-        <v>88</v>
+        <v>112</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
-        <v>41660</v>
+        <v>41680</v>
       </c>
       <c r="B41" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C41" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>35</v>
+        <v>109</v>
       </c>
       <c r="E41" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F41" s="3" t="s">
-        <v>36</v>
+        <v>110</v>
       </c>
       <c r="G41" s="3" t="s">
-        <v>87</v>
+        <v>111</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
-        <v>41659</v>
+        <v>41680</v>
       </c>
       <c r="B42" t="s">
-        <v>37</v>
+        <v>3</v>
       </c>
       <c r="C42" t="s">
         <v>0</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>38</v>
+        <v>105</v>
       </c>
       <c r="E42" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F42" s="3" t="s">
-        <v>39</v>
+        <v>6</v>
       </c>
       <c r="G42" s="3" t="s">
-        <v>86</v>
+        <v>98</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
-        <v>41655</v>
+        <v>41677</v>
       </c>
       <c r="B43" t="s">
-        <v>2</v>
+        <v>32</v>
       </c>
       <c r="C43" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>40</v>
+        <v>99</v>
       </c>
       <c r="E43" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F43" s="3" t="s">
-        <v>41</v>
+        <v>6</v>
       </c>
       <c r="G43" s="3" t="s">
-        <v>85</v>
+        <v>104</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
-        <v>41655</v>
+        <v>41677</v>
       </c>
       <c r="B44" t="s">
-        <v>42</v>
+        <v>59</v>
       </c>
       <c r="C44" t="s">
         <v>0</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>43</v>
+        <v>100</v>
       </c>
       <c r="E44" t="s">
-        <v>44</v>
+        <v>5</v>
       </c>
       <c r="F44" s="3" t="s">
-        <v>6</v>
+        <v>101</v>
       </c>
       <c r="G44" s="3" t="s">
-        <v>84</v>
+        <v>98</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
-        <v>41652</v>
+        <v>41676</v>
       </c>
       <c r="B45" t="s">
         <v>3</v>
       </c>
       <c r="C45" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>45</v>
+        <v>102</v>
       </c>
       <c r="E45" t="s">
         <v>5</v>
       </c>
       <c r="F45" s="3" t="s">
-        <v>46</v>
+        <v>101</v>
       </c>
       <c r="G45" s="3" t="s">
-        <v>83</v>
+        <v>103</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
-        <v>41649</v>
+        <v>41674</v>
       </c>
       <c r="B46" t="s">
-        <v>3</v>
+        <v>95</v>
       </c>
       <c r="C46" t="s">
         <v>0</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>16</v>
+        <v>96</v>
       </c>
       <c r="E46" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F46" s="3" t="s">
-        <v>15</v>
+        <v>97</v>
       </c>
       <c r="G46" s="3" t="s">
-        <v>82</v>
+        <v>98</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
-        <v>41648</v>
+        <v>41670</v>
       </c>
       <c r="B47" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="C47" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>47</v>
+        <v>18</v>
       </c>
       <c r="E47" t="s">
-        <v>1</v>
+        <v>19</v>
       </c>
       <c r="F47" s="3" t="s">
-        <v>48</v>
+        <v>20</v>
       </c>
       <c r="G47" s="3" t="s">
-        <v>81</v>
+        <v>94</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
-        <v>41648</v>
+        <v>41666</v>
       </c>
       <c r="B48" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C48" t="s">
         <v>0</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>49</v>
+        <v>21</v>
       </c>
       <c r="E48" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F48" s="3" t="s">
-        <v>9</v>
+        <v>71</v>
       </c>
       <c r="G48" s="3" t="s">
-        <v>80</v>
+        <v>93</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
-        <v>41647</v>
+        <v>41666</v>
       </c>
       <c r="B49" t="s">
         <v>2</v>
@@ -2039,193 +2163,492 @@
         <v>0</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>50</v>
+        <v>22</v>
       </c>
       <c r="E49" t="s">
         <v>1</v>
       </c>
       <c r="F49" s="3" t="s">
-        <v>51</v>
+        <v>23</v>
       </c>
       <c r="G49" s="3" t="s">
-        <v>79</v>
+        <v>92</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
-        <v>41646</v>
+        <v>41666</v>
       </c>
       <c r="B50" t="s">
-        <v>52</v>
+        <v>24</v>
       </c>
       <c r="C50" t="s">
         <v>0</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>53</v>
+        <v>25</v>
       </c>
       <c r="E50" t="s">
-        <v>12</v>
+        <v>26</v>
       </c>
       <c r="F50" s="3" t="s">
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="G50" s="3" t="s">
-        <v>78</v>
+        <v>91</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
-        <v>41646</v>
+        <v>41666</v>
       </c>
       <c r="B51" t="s">
-        <v>54</v>
+        <v>28</v>
       </c>
       <c r="C51" t="s">
         <v>0</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>55</v>
+        <v>29</v>
       </c>
       <c r="E51" t="s">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="F51" s="3" t="s">
-        <v>14</v>
+        <v>30</v>
       </c>
       <c r="G51" s="3" t="s">
-        <v>77</v>
+        <v>90</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
-        <v>41646</v>
+        <v>41660</v>
       </c>
       <c r="B52" t="s">
-        <v>56</v>
+        <v>11</v>
       </c>
       <c r="C52" t="s">
         <v>0</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>57</v>
+        <v>31</v>
       </c>
       <c r="E52" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F52" s="3" t="s">
-        <v>58</v>
+        <v>9</v>
       </c>
       <c r="G52" s="3" t="s">
-        <v>76</v>
+        <v>89</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
-        <v>41646</v>
+        <v>41660</v>
       </c>
       <c r="B53" t="s">
-        <v>59</v>
+        <v>32</v>
       </c>
       <c r="C53" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>60</v>
+        <v>33</v>
       </c>
       <c r="E53" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="F53" s="3" t="s">
-        <v>61</v>
+        <v>6</v>
       </c>
       <c r="G53" s="3" t="s">
-        <v>75</v>
+        <v>88</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
-        <v>41645</v>
+        <v>41660</v>
       </c>
       <c r="B54" t="s">
-        <v>62</v>
+        <v>34</v>
       </c>
       <c r="C54" t="s">
         <v>0</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>63</v>
+        <v>35</v>
       </c>
       <c r="E54" t="s">
-        <v>64</v>
+        <v>12</v>
       </c>
       <c r="F54" s="3" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
       <c r="G54" s="3" t="s">
-        <v>74</v>
+        <v>87</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
-        <v>41642</v>
+        <v>41659</v>
       </c>
       <c r="B55" t="s">
-        <v>65</v>
+        <v>37</v>
       </c>
       <c r="C55" t="s">
         <v>0</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>66</v>
+        <v>38</v>
       </c>
       <c r="E55" t="s">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="F55" s="3" t="s">
-        <v>67</v>
+        <v>39</v>
       </c>
       <c r="G55" s="3" t="s">
-        <v>73</v>
+        <v>86</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
-        <v>41641</v>
+        <v>41655</v>
       </c>
       <c r="B56" t="s">
-        <v>68</v>
+        <v>2</v>
       </c>
       <c r="C56" t="s">
         <v>0</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>69</v>
+        <v>40</v>
       </c>
       <c r="E56" t="s">
         <v>1</v>
       </c>
       <c r="F56" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="G56" s="3" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A57" s="1">
+        <v>41655</v>
+      </c>
+      <c r="B57" t="s">
+        <v>42</v>
+      </c>
+      <c r="C57" t="s">
+        <v>0</v>
+      </c>
+      <c r="D57" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E57" t="s">
+        <v>44</v>
+      </c>
+      <c r="F57" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G57" s="3" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A58" s="1">
+        <v>41652</v>
+      </c>
+      <c r="B58" t="s">
+        <v>3</v>
+      </c>
+      <c r="C58" t="s">
+        <v>0</v>
+      </c>
+      <c r="D58" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="E58" t="s">
+        <v>5</v>
+      </c>
+      <c r="F58" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="G58" s="3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A59" s="1">
+        <v>41649</v>
+      </c>
+      <c r="B59" t="s">
+        <v>3</v>
+      </c>
+      <c r="C59" t="s">
+        <v>0</v>
+      </c>
+      <c r="D59" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E59" t="s">
+        <v>5</v>
+      </c>
+      <c r="F59" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G59" s="3" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A60" s="1">
+        <v>41648</v>
+      </c>
+      <c r="B60" t="s">
+        <v>2</v>
+      </c>
+      <c r="C60" t="s">
+        <v>0</v>
+      </c>
+      <c r="D60" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E60" t="s">
+        <v>1</v>
+      </c>
+      <c r="F60" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="G60" s="3" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A61" s="1">
+        <v>41648</v>
+      </c>
+      <c r="B61" t="s">
+        <v>7</v>
+      </c>
+      <c r="C61" t="s">
+        <v>0</v>
+      </c>
+      <c r="D61" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E61" t="s">
+        <v>8</v>
+      </c>
+      <c r="F61" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G61" s="3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A62" s="1">
+        <v>41647</v>
+      </c>
+      <c r="B62" t="s">
+        <v>2</v>
+      </c>
+      <c r="C62" t="s">
+        <v>0</v>
+      </c>
+      <c r="D62" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E62" t="s">
+        <v>1</v>
+      </c>
+      <c r="F62" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="G62" s="3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A63" s="1">
+        <v>41646</v>
+      </c>
+      <c r="B63" t="s">
+        <v>52</v>
+      </c>
+      <c r="C63" t="s">
+        <v>0</v>
+      </c>
+      <c r="D63" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E63" t="s">
+        <v>12</v>
+      </c>
+      <c r="F63" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G63" s="3" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A64" s="1">
+        <v>41646</v>
+      </c>
+      <c r="B64" t="s">
+        <v>54</v>
+      </c>
+      <c r="C64" t="s">
+        <v>0</v>
+      </c>
+      <c r="D64" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="E64" t="s">
+        <v>12</v>
+      </c>
+      <c r="F64" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G64" s="3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A65" s="1">
+        <v>41646</v>
+      </c>
+      <c r="B65" t="s">
+        <v>56</v>
+      </c>
+      <c r="C65" t="s">
+        <v>0</v>
+      </c>
+      <c r="D65" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="E65" t="s">
+        <v>12</v>
+      </c>
+      <c r="F65" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="G65" s="3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A66" s="1">
+        <v>41646</v>
+      </c>
+      <c r="B66" t="s">
+        <v>59</v>
+      </c>
+      <c r="C66" t="s">
+        <v>0</v>
+      </c>
+      <c r="D66" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="E66" t="s">
+        <v>5</v>
+      </c>
+      <c r="F66" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="G66" s="3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A67" s="1">
+        <v>41645</v>
+      </c>
+      <c r="B67" t="s">
+        <v>62</v>
+      </c>
+      <c r="C67" t="s">
+        <v>0</v>
+      </c>
+      <c r="D67" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="E67" t="s">
+        <v>64</v>
+      </c>
+      <c r="F67" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G67" s="3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A68" s="1">
+        <v>41642</v>
+      </c>
+      <c r="B68" t="s">
+        <v>65</v>
+      </c>
+      <c r="C68" t="s">
+        <v>0</v>
+      </c>
+      <c r="D68" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="E68" t="s">
+        <v>10</v>
+      </c>
+      <c r="F68" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="G68" s="3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A69" s="1">
+        <v>41641</v>
+      </c>
+      <c r="B69" t="s">
+        <v>68</v>
+      </c>
+      <c r="C69" t="s">
+        <v>0</v>
+      </c>
+      <c r="D69" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="E69" t="s">
+        <v>1</v>
+      </c>
+      <c r="F69" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="G56" s="3" t="s">
+      <c r="G69" s="3" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A57" s="1"/>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A58" s="1"/>
-    </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A59" s="1"/>
-    </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A60" s="1"/>
-    </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A61" s="1"/>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A70" s="1"/>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A71" s="1"/>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A72" s="1"/>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A73" s="1"/>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A74" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Actualizando el modelo de bdd
</commit_message>
<xml_diff>
--- a/backup/cuenta_2200555126.xlsx
+++ b/backup/cuenta_2200555126.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="414" uniqueCount="219">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="420" uniqueCount="223">
   <si>
     <t>D</t>
   </si>
@@ -681,6 +681,18 @@
   </si>
   <si>
     <t>1143.49</t>
+  </si>
+  <si>
+    <t>CONSUMO DATA RESCUMBAYA CIA. LTDA.</t>
+  </si>
+  <si>
+    <t>0006803136</t>
+  </si>
+  <si>
+    <t>19.71  </t>
+  </si>
+  <si>
+    <t>728.51</t>
   </si>
 </sst>
 </file>
@@ -1003,10 +1015,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H74"/>
+  <dimension ref="A1:H75"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1:H8"/>
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1018,56 +1030,52 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1">
-        <v>41746</v>
+        <v>41750</v>
       </c>
       <c r="B1" t="s">
-        <v>197</v>
+        <v>219</v>
       </c>
       <c r="C1" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>198</v>
+        <v>220</v>
       </c>
       <c r="E1" t="s">
-        <v>156</v>
+        <v>1</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>9</v>
+        <v>221</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>199</v>
+        <v>222</v>
       </c>
       <c r="H1" t="str">
-        <f t="shared" ref="H1:H8" ca="1" si="0">CONCATENATE("array('mo_fecha' =&gt; new \DateTime('",TEXT(A1,"yyyy-mm-dd"),"'), 'mo_concepto' =&gt; '",B1,"', 'mo_tipo' =&gt; '",C1,"', 'mo_documento' =&gt; '",D1,"', 'mo_oficina' =&gt; '",E1,"', 'mo_monto' =&gt; ",TRIM(F1),", 'mo_saldo' =&gt; ",G1,", 'mo_fecha_crea' =&gt; new \DateTime('",TEXT(NOW(),"yyyy-mm-dd H:m:s"),"'), 'mo_quien_crea' =&gt; 1, 'mo_fecha_modifica' =&gt; NULL, 'mo_quien_modifica' =&gt; NULL, 'mo_borrado_logico' =&gt; false),")</f>
-        <v>array('mo_fecha' =&gt; new \DateTime('2014-04-17'), 'mo_concepto' =&gt; 'RETIRO ATM BP D/REINA VICTORIA', 'mo_tipo' =&gt; 'D', 'mo_documento' =&gt; '0000990490', 'mo_oficina' =&gt; 'CENTRO DE ACOPIO NORTE', 'mo_monto' =&gt; 20.00  , 'mo_saldo' =&gt; 748.22, 'mo_fecha_crea' =&gt; new \DateTime('2014-04-18 13:44:39'), 'mo_quien_crea' =&gt; 1, 'mo_fecha_modifica' =&gt; NULL, 'mo_quien_modifica' =&gt; NULL, 'mo_borrado_logico' =&gt; false),</v>
+        <f t="shared" ref="H1:H9" ca="1" si="0">CONCATENATE("array('mo_fecha' =&gt; new \DateTime('",TEXT(A1,"yyyy-mm-dd"),"'), 'mo_concepto' =&gt; '",B1,"', 'mo_tipo' =&gt; '",C1,"', 'mo_documento' =&gt; '",D1,"', 'mo_oficina' =&gt; '",E1,"', 'mo_monto' =&gt; ",TRIM(F1),", 'mo_saldo' =&gt; ",G1,", 'mo_fecha_crea' =&gt; new \DateTime('",TEXT(NOW(),"yyyy-mm-dd H:m:s"),"'), 'mo_quien_crea' =&gt; 1, 'mo_fecha_modifica' =&gt; NULL, 'mo_quien_modifica' =&gt; NULL, 'mo_borrado_logico' =&gt; false),")</f>
+        <v>array('mo_fecha' =&gt; new \DateTime('2014-04-21'), 'mo_concepto' =&gt; 'CONSUMO DATA RESCUMBAYA CIA. LTDA.', 'mo_tipo' =&gt; 'D', 'mo_documento' =&gt; '0006803136', 'mo_oficina' =&gt; 'INSTITUCIONAL SS.CC.', 'mo_monto' =&gt; 19.71  , 'mo_saldo' =&gt; 728.51, 'mo_fecha_crea' =&gt; new \DateTime('2014-04-21 12:20:57'), 'mo_quien_crea' =&gt; 1, 'mo_fecha_modifica' =&gt; NULL, 'mo_quien_modifica' =&gt; NULL, 'mo_borrado_logico' =&gt; false),</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>41744</v>
+        <v>41746</v>
       </c>
       <c r="B2" t="s">
-        <v>135</v>
+        <v>197</v>
       </c>
       <c r="C2" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="E2" t="s">
-        <v>5</v>
+        <v>156</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>67</v>
+        <v>9</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>201</v>
-      </c>
-      <c r="H2" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>array('mo_fecha' =&gt; new \DateTime('2014-04-15'), 'mo_concepto' =&gt; 'DEP CNB-1500415029001', 'mo_tipo' =&gt; 'C', 'mo_documento' =&gt; '0008775881', 'mo_oficina' =&gt; 'AG. NORTE', 'mo_monto' =&gt; 50.00  , 'mo_saldo' =&gt; 768.22, 'mo_fecha_crea' =&gt; new \DateTime('2014-04-18 13:44:39'), 'mo_quien_crea' =&gt; 1, 'mo_fecha_modifica' =&gt; NULL, 'mo_quien_modifica' =&gt; NULL, 'mo_borrado_logico' =&gt; false),</v>
+        <v>199</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -1075,26 +1083,22 @@
         <v>41744</v>
       </c>
       <c r="B3" t="s">
-        <v>189</v>
+        <v>135</v>
       </c>
       <c r="C3" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="E3" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>203</v>
+        <v>67</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>204</v>
-      </c>
-      <c r="H3" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>array('mo_fecha' =&gt; new \DateTime('2014-04-15'), 'mo_concepto' =&gt; 'CONSUMO DATA FYBECA (PLAZA DE TOROS', 'mo_tipo' =&gt; 'D', 'mo_documento' =&gt; '0004392772', 'mo_oficina' =&gt; 'INSTITUCIONAL SS.CC.', 'mo_monto' =&gt; 41.58  , 'mo_saldo' =&gt; 718.22, 'mo_fecha_crea' =&gt; new \DateTime('2014-04-18 13:44:39'), 'mo_quien_crea' =&gt; 1, 'mo_fecha_modifica' =&gt; NULL, 'mo_quien_modifica' =&gt; NULL, 'mo_borrado_logico' =&gt; false),</v>
+        <v>201</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -1102,26 +1106,22 @@
         <v>41744</v>
       </c>
       <c r="B4" t="s">
-        <v>185</v>
+        <v>189</v>
       </c>
       <c r="C4" t="s">
         <v>0</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="E4" t="s">
         <v>1</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>207</v>
-      </c>
-      <c r="H4" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>array('mo_fecha' =&gt; new \DateTime('2014-04-15'), 'mo_concepto' =&gt; 'CONSUMO DATA FYBECA TORRES MEDICAS', 'mo_tipo' =&gt; 'D', 'mo_documento' =&gt; '0002223892', 'mo_oficina' =&gt; 'INSTITUCIONAL SS.CC.', 'mo_monto' =&gt; 2.31  , 'mo_saldo' =&gt; 759.80, 'mo_fecha_crea' =&gt; new \DateTime('2014-04-18 13:44:39'), 'mo_quien_crea' =&gt; 1, 'mo_fecha_modifica' =&gt; NULL, 'mo_quien_modifica' =&gt; NULL, 'mo_borrado_logico' =&gt; false),</v>
+        <v>204</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -1135,47 +1135,39 @@
         <v>0</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="E5" t="s">
         <v>1</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>210</v>
-      </c>
-      <c r="H5" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>array('mo_fecha' =&gt; new \DateTime('2014-04-15'), 'mo_concepto' =&gt; 'CONSUMO DATA FYBECA TORRES MEDICAS', 'mo_tipo' =&gt; 'D', 'mo_documento' =&gt; '0002195122', 'mo_oficina' =&gt; 'INSTITUCIONAL SS.CC.', 'mo_monto' =&gt; 38.19  , 'mo_saldo' =&gt; 762.11, 'mo_fecha_crea' =&gt; new \DateTime('2014-04-18 13:44:39'), 'mo_quien_crea' =&gt; 1, 'mo_fecha_modifica' =&gt; NULL, 'mo_quien_modifica' =&gt; NULL, 'mo_borrado_logico' =&gt; false),</v>
+        <v>207</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
-        <v>41743</v>
+        <v>41744</v>
       </c>
       <c r="B6" t="s">
-        <v>3</v>
+        <v>185</v>
       </c>
       <c r="C6" t="s">
         <v>0</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="E6" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>6</v>
+        <v>209</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>212</v>
-      </c>
-      <c r="H6" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>array('mo_fecha' =&gt; new \DateTime('2014-04-14'), 'mo_concepto' =&gt; '  TRANSFERENCIA INTERNET', 'mo_tipo' =&gt; 'D', 'mo_documento' =&gt; '0007431020', 'mo_oficina' =&gt; 'AG. NORTE', 'mo_monto' =&gt; 100.00  , 'mo_saldo' =&gt; 800.30, 'mo_fecha_crea' =&gt; new \DateTime('2014-04-18 13:44:39'), 'mo_quien_crea' =&gt; 1, 'mo_fecha_modifica' =&gt; NULL, 'mo_quien_modifica' =&gt; NULL, 'mo_borrado_logico' =&gt; false),</v>
+        <v>210</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -1189,20 +1181,16 @@
         <v>0</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="E7" t="s">
         <v>5</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>214</v>
+        <v>6</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>215</v>
-      </c>
-      <c r="H7" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>array('mo_fecha' =&gt; new \DateTime('2014-04-14'), 'mo_concepto' =&gt; '  TRANSFERENCIA INTERNET', 'mo_tipo' =&gt; 'D', 'mo_documento' =&gt; '0007349236', 'mo_oficina' =&gt; 'AG. NORTE', 'mo_monto' =&gt; 243.19  , 'mo_saldo' =&gt; 900.30, 'mo_fecha_crea' =&gt; new \DateTime('2014-04-18 13:44:39'), 'mo_quien_crea' =&gt; 1, 'mo_fecha_modifica' =&gt; NULL, 'mo_quien_modifica' =&gt; NULL, 'mo_borrado_logico' =&gt; false),</v>
+        <v>212</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -1210,49 +1198,45 @@
         <v>41743</v>
       </c>
       <c r="B8" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C8" t="s">
         <v>0</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="E8" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>218</v>
-      </c>
-      <c r="H8" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>array('mo_fecha' =&gt; new \DateTime('2014-04-14'), 'mo_concepto' =&gt; 'CONSUMO DATA AKI MOLINEROS 161', 'mo_tipo' =&gt; 'D', 'mo_documento' =&gt; '0002730824', 'mo_oficina' =&gt; 'INSTITUCIONAL SS.CC.', 'mo_monto' =&gt; 85.43  , 'mo_saldo' =&gt; 1143.49, 'mo_fecha_crea' =&gt; new \DateTime('2014-04-18 13:44:39'), 'mo_quien_crea' =&gt; 1, 'mo_fecha_modifica' =&gt; NULL, 'mo_quien_modifica' =&gt; NULL, 'mo_borrado_logico' =&gt; false),</v>
+        <v>215</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
-        <v>41740</v>
+        <v>41743</v>
       </c>
       <c r="B9" t="s">
-        <v>185</v>
+        <v>2</v>
       </c>
       <c r="C9" t="s">
         <v>0</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>186</v>
+        <v>216</v>
       </c>
       <c r="E9" t="s">
         <v>1</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>187</v>
+        <v>217</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>196</v>
+        <v>218</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -1260,45 +1244,45 @@
         <v>41740</v>
       </c>
       <c r="B10" t="s">
-        <v>42</v>
+        <v>185</v>
       </c>
       <c r="C10" t="s">
         <v>0</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="E10" t="s">
-        <v>44</v>
+        <v>1</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>15</v>
+        <v>187</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
-        <v>41739</v>
+        <v>41740</v>
       </c>
       <c r="B11" t="s">
-        <v>189</v>
+        <v>42</v>
       </c>
       <c r="C11" t="s">
         <v>0</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="E11" t="s">
-        <v>1</v>
+        <v>44</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>191</v>
+        <v>15</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -1306,91 +1290,91 @@
         <v>41739</v>
       </c>
       <c r="B12" t="s">
-        <v>42</v>
+        <v>189</v>
       </c>
       <c r="C12" t="s">
         <v>0</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="E12" t="s">
-        <v>44</v>
+        <v>1</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>67</v>
+        <v>191</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
-        <v>41738</v>
+        <v>41739</v>
       </c>
       <c r="B13" t="s">
-        <v>3</v>
+        <v>42</v>
       </c>
       <c r="C13" t="s">
         <v>0</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>183</v>
+        <v>192</v>
       </c>
       <c r="E13" t="s">
-        <v>5</v>
+        <v>44</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>165</v>
+        <v>67</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>184</v>
+        <v>193</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
-        <v>41737</v>
+        <v>41738</v>
       </c>
       <c r="B14" t="s">
         <v>3</v>
       </c>
       <c r="C14" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>173</v>
+        <v>183</v>
       </c>
       <c r="E14" t="s">
         <v>5</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>174</v>
+        <v>165</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
-        <v>41736</v>
+        <v>41737</v>
       </c>
       <c r="B15" t="s">
-        <v>175</v>
+        <v>3</v>
       </c>
       <c r="C15" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="E15" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F15" s="3" t="s">
         <v>174</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -1398,22 +1382,22 @@
         <v>41736</v>
       </c>
       <c r="B16" t="s">
-        <v>59</v>
+        <v>175</v>
       </c>
       <c r="C16" t="s">
         <v>0</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E16" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
@@ -1421,45 +1405,45 @@
         <v>41736</v>
       </c>
       <c r="B17" t="s">
-        <v>7</v>
+        <v>59</v>
       </c>
       <c r="C17" t="s">
         <v>0</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="E17" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>174</v>
+        <v>178</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
-        <v>41731</v>
+        <v>41736</v>
       </c>
       <c r="B18" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C18" t="s">
         <v>0</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>167</v>
+        <v>179</v>
       </c>
       <c r="E18" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>15</v>
+        <v>174</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>171</v>
+        <v>180</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
@@ -1467,45 +1451,45 @@
         <v>41731</v>
       </c>
       <c r="B19" t="s">
-        <v>32</v>
+        <v>3</v>
       </c>
       <c r="C19" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E19" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="F19" s="3" t="s">
         <v>15</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
-        <v>41729</v>
+        <v>41731</v>
       </c>
       <c r="B20" t="s">
-        <v>17</v>
+        <v>32</v>
       </c>
       <c r="C20" t="s">
         <v>4</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E20" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>170</v>
+        <v>15</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
@@ -1513,27 +1497,27 @@
         <v>41729</v>
       </c>
       <c r="B21" t="s">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="C21" t="s">
         <v>4</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>164</v>
+        <v>169</v>
       </c>
       <c r="E21" t="s">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>165</v>
+        <v>170</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>166</v>
+        <v>171</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
-        <v>41725</v>
+        <v>41729</v>
       </c>
       <c r="B22" t="s">
         <v>3</v>
@@ -1542,16 +1526,16 @@
         <v>4</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>159</v>
+        <v>164</v>
       </c>
       <c r="E22" t="s">
         <v>5</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>160</v>
+        <v>165</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
@@ -1559,45 +1543,45 @@
         <v>41725</v>
       </c>
       <c r="B23" t="s">
-        <v>144</v>
+        <v>3</v>
       </c>
       <c r="C23" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="E23" t="s">
-        <v>146</v>
+        <v>5</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>6</v>
+        <v>160</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
-        <v>41722</v>
+        <v>41725</v>
       </c>
       <c r="B24" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
       <c r="C24" t="s">
         <v>0</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>152</v>
+        <v>161</v>
       </c>
       <c r="E24" t="s">
-        <v>1</v>
+        <v>146</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>153</v>
+        <v>6</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>158</v>
+        <v>162</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
@@ -1605,22 +1589,22 @@
         <v>41722</v>
       </c>
       <c r="B25" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="C25" t="s">
         <v>0</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="E25" t="s">
-        <v>156</v>
+        <v>1</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>6</v>
+        <v>153</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
@@ -1628,22 +1612,22 @@
         <v>41722</v>
       </c>
       <c r="B26" t="s">
-        <v>3</v>
+        <v>154</v>
       </c>
       <c r="C26" t="s">
         <v>0</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>143</v>
+        <v>155</v>
       </c>
       <c r="E26" t="s">
-        <v>5</v>
+        <v>156</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>150</v>
+        <v>157</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
@@ -1651,128 +1635,128 @@
         <v>41722</v>
       </c>
       <c r="B27" t="s">
-        <v>144</v>
+        <v>3</v>
       </c>
       <c r="C27" t="s">
         <v>0</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="E27" t="s">
-        <v>146</v>
+        <v>5</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>27</v>
+        <v>9</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
-        <v>41719</v>
+        <v>41722</v>
       </c>
       <c r="B28" t="s">
-        <v>32</v>
+        <v>144</v>
       </c>
       <c r="C28" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E28" t="s">
-        <v>10</v>
+        <v>146</v>
       </c>
       <c r="F28" s="3" t="s">
-        <v>6</v>
+        <v>27</v>
       </c>
       <c r="G28" s="3" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
-        <v>41712</v>
+        <v>41719</v>
       </c>
       <c r="B29" t="s">
-        <v>139</v>
+        <v>32</v>
       </c>
       <c r="C29" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>140</v>
+        <v>147</v>
       </c>
       <c r="E29" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>141</v>
+        <v>6</v>
       </c>
       <c r="G29" s="3" t="s">
-        <v>142</v>
+        <v>148</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
-        <v>41708</v>
+        <v>41712</v>
       </c>
       <c r="B30" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="C30" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="E30" t="s">
         <v>5</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>6</v>
+        <v>141</v>
       </c>
       <c r="G30" s="3" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
-        <v>41705</v>
+        <v>41708</v>
       </c>
       <c r="B31" t="s">
-        <v>59</v>
+        <v>135</v>
       </c>
       <c r="C31" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E31" t="s">
         <v>5</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>133</v>
+        <v>6</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>131</v>
+        <v>138</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
-        <v>41703</v>
+        <v>41705</v>
       </c>
       <c r="B32" t="s">
-        <v>3</v>
+        <v>59</v>
       </c>
       <c r="C32" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>132</v>
+        <v>137</v>
       </c>
       <c r="E32" t="s">
         <v>5</v>
@@ -1781,7 +1765,7 @@
         <v>133</v>
       </c>
       <c r="G32" s="3" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
@@ -1789,22 +1773,22 @@
         <v>41703</v>
       </c>
       <c r="B33" t="s">
-        <v>117</v>
+        <v>3</v>
       </c>
       <c r="C33" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>118</v>
+        <v>132</v>
       </c>
       <c r="E33" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F33" s="3" t="s">
-        <v>119</v>
+        <v>133</v>
       </c>
       <c r="G33" s="3" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
@@ -1812,68 +1796,68 @@
         <v>41703</v>
       </c>
       <c r="B34" t="s">
-        <v>2</v>
+        <v>117</v>
       </c>
       <c r="C34" t="s">
         <v>0</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="E34" t="s">
         <v>1</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="G34" s="3" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
-        <v>41698</v>
+        <v>41703</v>
       </c>
       <c r="B35" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="C35" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="E35" t="s">
-        <v>19</v>
+        <v>1</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="G35" s="3" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
-        <v>41691</v>
+        <v>41698</v>
       </c>
       <c r="B36" t="s">
-        <v>124</v>
+        <v>17</v>
       </c>
       <c r="C36" t="s">
         <v>4</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="E36" t="s">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="F36" s="3" t="s">
-        <v>67</v>
+        <v>123</v>
       </c>
       <c r="G36" s="3" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
@@ -1887,7 +1871,7 @@
         <v>4</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E37" t="s">
         <v>5</v>
@@ -1896,30 +1880,30 @@
         <v>67</v>
       </c>
       <c r="G37" s="3" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
-        <v>41690</v>
+        <v>41691</v>
       </c>
       <c r="B38" t="s">
-        <v>3</v>
+        <v>124</v>
       </c>
       <c r="C38" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>113</v>
+        <v>126</v>
       </c>
       <c r="E38" t="s">
         <v>5</v>
       </c>
       <c r="F38" s="3" t="s">
-        <v>114</v>
+        <v>67</v>
       </c>
       <c r="G38" s="3" t="s">
-        <v>112</v>
+        <v>127</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
@@ -1930,10 +1914,10 @@
         <v>3</v>
       </c>
       <c r="C39" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="E39" t="s">
         <v>5</v>
@@ -1942,53 +1926,53 @@
         <v>114</v>
       </c>
       <c r="G39" s="3" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
-        <v>41682</v>
+        <v>41690</v>
       </c>
       <c r="B40" t="s">
-        <v>106</v>
+        <v>3</v>
       </c>
       <c r="C40" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>107</v>
+        <v>115</v>
       </c>
       <c r="E40" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="F40" s="3" t="s">
-        <v>108</v>
+        <v>114</v>
       </c>
       <c r="G40" s="3" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
-        <v>41680</v>
+        <v>41682</v>
       </c>
       <c r="B41" t="s">
-        <v>32</v>
+        <v>106</v>
       </c>
       <c r="C41" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="E41" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F41" s="3" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="G41" s="3" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
@@ -1996,45 +1980,45 @@
         <v>41680</v>
       </c>
       <c r="B42" t="s">
-        <v>3</v>
+        <v>32</v>
       </c>
       <c r="C42" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="E42" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="F42" s="3" t="s">
-        <v>6</v>
+        <v>110</v>
       </c>
       <c r="G42" s="3" t="s">
-        <v>98</v>
+        <v>111</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
-        <v>41677</v>
+        <v>41680</v>
       </c>
       <c r="B43" t="s">
-        <v>32</v>
+        <v>3</v>
       </c>
       <c r="C43" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>99</v>
+        <v>105</v>
       </c>
       <c r="E43" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="F43" s="3" t="s">
         <v>6</v>
       </c>
       <c r="G43" s="3" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
@@ -2042,36 +2026,36 @@
         <v>41677</v>
       </c>
       <c r="B44" t="s">
-        <v>59</v>
+        <v>32</v>
       </c>
       <c r="C44" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E44" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="F44" s="3" t="s">
-        <v>101</v>
+        <v>6</v>
       </c>
       <c r="G44" s="3" t="s">
-        <v>98</v>
+        <v>104</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
-        <v>41676</v>
+        <v>41677</v>
       </c>
       <c r="B45" t="s">
-        <v>3</v>
+        <v>59</v>
       </c>
       <c r="C45" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="E45" t="s">
         <v>5</v>
@@ -2080,76 +2064,76 @@
         <v>101</v>
       </c>
       <c r="G45" s="3" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
-        <v>41674</v>
+        <v>41676</v>
       </c>
       <c r="B46" t="s">
-        <v>95</v>
+        <v>3</v>
       </c>
       <c r="C46" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>96</v>
+        <v>102</v>
       </c>
       <c r="E46" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F46" s="3" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="G46" s="3" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
-        <v>41670</v>
+        <v>41674</v>
       </c>
       <c r="B47" t="s">
-        <v>17</v>
+        <v>95</v>
       </c>
       <c r="C47" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>18</v>
+        <v>96</v>
       </c>
       <c r="E47" t="s">
-        <v>19</v>
+        <v>1</v>
       </c>
       <c r="F47" s="3" t="s">
-        <v>20</v>
+        <v>97</v>
       </c>
       <c r="G47" s="3" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
-        <v>41666</v>
+        <v>41670</v>
       </c>
       <c r="B48" t="s">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="C48" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="E48" t="s">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="F48" s="3" t="s">
-        <v>71</v>
+        <v>20</v>
       </c>
       <c r="G48" s="3" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
@@ -2157,22 +2141,22 @@
         <v>41666</v>
       </c>
       <c r="B49" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C49" t="s">
         <v>0</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E49" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F49" s="3" t="s">
-        <v>23</v>
+        <v>71</v>
       </c>
       <c r="G49" s="3" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
@@ -2180,22 +2164,22 @@
         <v>41666</v>
       </c>
       <c r="B50" t="s">
-        <v>24</v>
+        <v>2</v>
       </c>
       <c r="C50" t="s">
         <v>0</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E50" t="s">
-        <v>26</v>
+        <v>1</v>
       </c>
       <c r="F50" s="3" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="G50" s="3" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
@@ -2203,45 +2187,45 @@
         <v>41666</v>
       </c>
       <c r="B51" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C51" t="s">
         <v>0</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="E51" t="s">
-        <v>1</v>
+        <v>26</v>
       </c>
       <c r="F51" s="3" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="G51" s="3" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
-        <v>41660</v>
+        <v>41666</v>
       </c>
       <c r="B52" t="s">
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="C52" t="s">
         <v>0</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E52" t="s">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="F52" s="3" t="s">
-        <v>9</v>
+        <v>30</v>
       </c>
       <c r="G52" s="3" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
@@ -2249,22 +2233,22 @@
         <v>41660</v>
       </c>
       <c r="B53" t="s">
-        <v>32</v>
+        <v>11</v>
       </c>
       <c r="C53" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E53" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="F53" s="3" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="G53" s="3" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
@@ -2272,68 +2256,68 @@
         <v>41660</v>
       </c>
       <c r="B54" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C54" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E54" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F54" s="3" t="s">
-        <v>36</v>
+        <v>6</v>
       </c>
       <c r="G54" s="3" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
-        <v>41659</v>
+        <v>41660</v>
       </c>
       <c r="B55" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C55" t="s">
         <v>0</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="E55" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="F55" s="3" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="G55" s="3" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
-        <v>41655</v>
+        <v>41659</v>
       </c>
       <c r="B56" t="s">
-        <v>2</v>
+        <v>37</v>
       </c>
       <c r="C56" t="s">
         <v>0</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E56" t="s">
         <v>1</v>
       </c>
       <c r="F56" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="G56" s="3" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
@@ -2341,50 +2325,50 @@
         <v>41655</v>
       </c>
       <c r="B57" t="s">
-        <v>42</v>
+        <v>2</v>
       </c>
       <c r="C57" t="s">
         <v>0</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="E57" t="s">
-        <v>44</v>
+        <v>1</v>
       </c>
       <c r="F57" s="3" t="s">
-        <v>6</v>
+        <v>41</v>
       </c>
       <c r="G57" s="3" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
-        <v>41652</v>
+        <v>41655</v>
       </c>
       <c r="B58" t="s">
-        <v>3</v>
+        <v>42</v>
       </c>
       <c r="C58" t="s">
         <v>0</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E58" t="s">
-        <v>5</v>
+        <v>44</v>
       </c>
       <c r="F58" s="3" t="s">
-        <v>46</v>
+        <v>6</v>
       </c>
       <c r="G58" s="3" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
-        <v>41649</v>
+        <v>41652</v>
       </c>
       <c r="B59" t="s">
         <v>3</v>
@@ -2393,39 +2377,39 @@
         <v>0</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>16</v>
+        <v>45</v>
       </c>
       <c r="E59" t="s">
         <v>5</v>
       </c>
       <c r="F59" s="3" t="s">
-        <v>15</v>
+        <v>46</v>
       </c>
       <c r="G59" s="3" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
-        <v>41648</v>
+        <v>41649</v>
       </c>
       <c r="B60" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C60" t="s">
         <v>0</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>47</v>
+        <v>16</v>
       </c>
       <c r="E60" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F60" s="3" t="s">
-        <v>48</v>
+        <v>15</v>
       </c>
       <c r="G60" s="3" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
@@ -2433,68 +2417,68 @@
         <v>41648</v>
       </c>
       <c r="B61" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="C61" t="s">
         <v>0</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E61" t="s">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="F61" s="3" t="s">
-        <v>9</v>
+        <v>48</v>
       </c>
       <c r="G61" s="3" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
-        <v>41647</v>
+        <v>41648</v>
       </c>
       <c r="B62" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="C62" t="s">
         <v>0</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E62" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="F62" s="3" t="s">
-        <v>51</v>
+        <v>9</v>
       </c>
       <c r="G62" s="3" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
-        <v>41646</v>
+        <v>41647</v>
       </c>
       <c r="B63" t="s">
-        <v>52</v>
+        <v>2</v>
       </c>
       <c r="C63" t="s">
         <v>0</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="E63" t="s">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="F63" s="3" t="s">
-        <v>13</v>
+        <v>51</v>
       </c>
       <c r="G63" s="3" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
@@ -2502,22 +2486,22 @@
         <v>41646</v>
       </c>
       <c r="B64" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C64" t="s">
         <v>0</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E64" t="s">
         <v>12</v>
       </c>
       <c r="F64" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G64" s="3" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
@@ -2525,22 +2509,22 @@
         <v>41646</v>
       </c>
       <c r="B65" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C65" t="s">
         <v>0</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E65" t="s">
         <v>12</v>
       </c>
       <c r="F65" s="3" t="s">
-        <v>58</v>
+        <v>14</v>
       </c>
       <c r="G65" s="3" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
@@ -2548,95 +2532,115 @@
         <v>41646</v>
       </c>
       <c r="B66" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C66" t="s">
         <v>0</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E66" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="F66" s="3" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="G66" s="3" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
-        <v>41645</v>
+        <v>41646</v>
       </c>
       <c r="B67" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C67" t="s">
         <v>0</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="E67" t="s">
-        <v>64</v>
+        <v>5</v>
       </c>
       <c r="F67" s="3" t="s">
-        <v>9</v>
+        <v>61</v>
       </c>
       <c r="G67" s="3" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
-        <v>41642</v>
+        <v>41645</v>
       </c>
       <c r="B68" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C68" t="s">
         <v>0</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="E68" t="s">
-        <v>10</v>
+        <v>64</v>
       </c>
       <c r="F68" s="3" t="s">
-        <v>67</v>
+        <v>9</v>
       </c>
       <c r="G68" s="3" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
+        <v>41642</v>
+      </c>
+      <c r="B69" t="s">
+        <v>65</v>
+      </c>
+      <c r="C69" t="s">
+        <v>0</v>
+      </c>
+      <c r="D69" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="E69" t="s">
+        <v>10</v>
+      </c>
+      <c r="F69" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="G69" s="3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A70" s="1">
         <v>41641</v>
       </c>
-      <c r="B69" t="s">
+      <c r="B70" t="s">
         <v>68</v>
       </c>
-      <c r="C69" t="s">
-        <v>0</v>
-      </c>
-      <c r="D69" s="2" t="s">
+      <c r="C70" t="s">
+        <v>0</v>
+      </c>
+      <c r="D70" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="E69" t="s">
+      <c r="E70" t="s">
         <v>1</v>
       </c>
-      <c r="F69" s="3" t="s">
+      <c r="F70" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="G69" s="3" t="s">
+      <c r="G70" s="3" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A70" s="1"/>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" s="1"/>
@@ -2649,6 +2653,9 @@
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" s="1"/>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A75" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Actualizando el modelo de bdd y las clases
</commit_message>
<xml_diff>
--- a/backup/cuenta_2200555126.xlsx
+++ b/backup/cuenta_2200555126.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="420" uniqueCount="223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="438" uniqueCount="232">
   <si>
     <t>D</t>
   </si>
@@ -693,6 +693,33 @@
   </si>
   <si>
     <t>728.51</t>
+  </si>
+  <si>
+    <t>RETIRO ATM BP N/EL DORAL</t>
+  </si>
+  <si>
+    <t>0001197152</t>
+  </si>
+  <si>
+    <t>140.00  </t>
+  </si>
+  <si>
+    <t>450.51</t>
+  </si>
+  <si>
+    <t>0006669642</t>
+  </si>
+  <si>
+    <t>38.00  </t>
+  </si>
+  <si>
+    <t>590.51</t>
+  </si>
+  <si>
+    <t>0002178501</t>
+  </si>
+  <si>
+    <t>628.51</t>
   </si>
 </sst>
 </file>
@@ -1015,10 +1042,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H75"/>
+  <dimension ref="A1:H78"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+      <selection activeCell="H1" sqref="H1:H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1030,121 +1057,129 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1">
-        <v>41750</v>
+        <v>41752</v>
       </c>
       <c r="B1" t="s">
-        <v>219</v>
+        <v>223</v>
       </c>
       <c r="C1" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>220</v>
+        <v>224</v>
       </c>
       <c r="E1" t="s">
-        <v>1</v>
+        <v>156</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>221</v>
+        <v>225</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>222</v>
+        <v>226</v>
       </c>
       <c r="H1" t="str">
-        <f t="shared" ref="H1:H9" ca="1" si="0">CONCATENATE("array('mo_fecha' =&gt; new \DateTime('",TEXT(A1,"yyyy-mm-dd"),"'), 'mo_concepto' =&gt; '",B1,"', 'mo_tipo' =&gt; '",C1,"', 'mo_documento' =&gt; '",D1,"', 'mo_oficina' =&gt; '",E1,"', 'mo_monto' =&gt; ",TRIM(F1),", 'mo_saldo' =&gt; ",G1,", 'mo_fecha_crea' =&gt; new \DateTime('",TEXT(NOW(),"yyyy-mm-dd H:m:s"),"'), 'mo_quien_crea' =&gt; 1, 'mo_fecha_modifica' =&gt; NULL, 'mo_quien_modifica' =&gt; NULL, 'mo_borrado_logico' =&gt; false),")</f>
-        <v>array('mo_fecha' =&gt; new \DateTime('2014-04-21'), 'mo_concepto' =&gt; 'CONSUMO DATA RESCUMBAYA CIA. LTDA.', 'mo_tipo' =&gt; 'D', 'mo_documento' =&gt; '0006803136', 'mo_oficina' =&gt; 'INSTITUCIONAL SS.CC.', 'mo_monto' =&gt; 19.71  , 'mo_saldo' =&gt; 728.51, 'mo_fecha_crea' =&gt; new \DateTime('2014-04-21 12:20:57'), 'mo_quien_crea' =&gt; 1, 'mo_fecha_modifica' =&gt; NULL, 'mo_quien_modifica' =&gt; NULL, 'mo_borrado_logico' =&gt; false),</v>
+        <f t="shared" ref="H1:H3" ca="1" si="0">CONCATENATE("array('mo_fecha' =&gt; new \DateTime('",TEXT(A1,"yyyy-mm-dd"),"'), 'mo_concepto' =&gt; '",B1,"', 'mo_tipo' =&gt; '",C1,"', 'mo_documento' =&gt; '",D1,"', 'mo_oficina' =&gt; '",E1,"', 'mo_monto' =&gt; ",F1,", 'mo_saldo' =&gt; ",G1,", 'mo_fecha_crea' =&gt; new \DateTime('",TEXT(NOW(),"yyyy-mm-dd H:m:s"),"'), 'mo_quien_crea' =&gt; 1, 'mo_fecha_modifica' =&gt; NULL, 'mo_quien_modifica' =&gt; NULL, 'mo_fecha_borrado' =&gt; NULL, 'mo_quien_borra' =&gt; NULL, 'mo_borrado_logico' =&gt; false),")</f>
+        <v>array('mo_fecha' =&gt; new \DateTime('2014-04-23'), 'mo_concepto' =&gt; 'RETIRO ATM BP N/EL DORAL', 'mo_tipo' =&gt; 'D', 'mo_documento' =&gt; '0001197152', 'mo_oficina' =&gt; 'CENTRO DE ACOPIO NORTE', 'mo_monto' =&gt; 140.00  , 'mo_saldo' =&gt; 450.51, 'mo_fecha_crea' =&gt; new \DateTime('2014-04-24 20:19:38'), 'mo_quien_crea' =&gt; 1, 'mo_fecha_modifica' =&gt; NULL, 'mo_quien_modifica' =&gt; NULL, 'mo_fecha_borrado' =&gt; NULL, 'mo_quien_borra' =&gt; NULL, 'mo_borrado_logico' =&gt; false),</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>41746</v>
+        <v>41751</v>
       </c>
       <c r="B2" t="s">
-        <v>197</v>
+        <v>2</v>
       </c>
       <c r="C2" t="s">
         <v>0</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>198</v>
+        <v>227</v>
       </c>
       <c r="E2" t="s">
-        <v>156</v>
+        <v>1</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>9</v>
+        <v>228</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>199</v>
+        <v>229</v>
+      </c>
+      <c r="H2" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>array('mo_fecha' =&gt; new \DateTime('2014-04-22'), 'mo_concepto' =&gt; 'CONSUMO DATA AKI MOLINEROS 161', 'mo_tipo' =&gt; 'D', 'mo_documento' =&gt; '0006669642', 'mo_oficina' =&gt; 'INSTITUCIONAL SS.CC.', 'mo_monto' =&gt; 38.00  , 'mo_saldo' =&gt; 590.51, 'mo_fecha_crea' =&gt; new \DateTime('2014-04-24 20:19:38'), 'mo_quien_crea' =&gt; 1, 'mo_fecha_modifica' =&gt; NULL, 'mo_quien_modifica' =&gt; NULL, 'mo_fecha_borrado' =&gt; NULL, 'mo_quien_borra' =&gt; NULL, 'mo_borrado_logico' =&gt; false),</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>41744</v>
+        <v>41751</v>
       </c>
       <c r="B3" t="s">
-        <v>135</v>
+        <v>144</v>
       </c>
       <c r="C3" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>200</v>
+        <v>230</v>
       </c>
       <c r="E3" t="s">
-        <v>5</v>
+        <v>146</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>67</v>
+        <v>6</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>201</v>
+        <v>231</v>
+      </c>
+      <c r="H3" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>array('mo_fecha' =&gt; new \DateTime('2014-04-22'), 'mo_concepto' =&gt; 'RETIRO ATM BP D/KENNEDY 3', 'mo_tipo' =&gt; 'D', 'mo_documento' =&gt; '0002178501', 'mo_oficina' =&gt; 'KENNEDY', 'mo_monto' =&gt; 100.00  , 'mo_saldo' =&gt; 628.51, 'mo_fecha_crea' =&gt; new \DateTime('2014-04-24 20:19:38'), 'mo_quien_crea' =&gt; 1, 'mo_fecha_modifica' =&gt; NULL, 'mo_quien_modifica' =&gt; NULL, 'mo_fecha_borrado' =&gt; NULL, 'mo_quien_borra' =&gt; NULL, 'mo_borrado_logico' =&gt; false),</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
-        <v>41744</v>
+        <v>41750</v>
       </c>
       <c r="B4" t="s">
-        <v>189</v>
+        <v>219</v>
       </c>
       <c r="C4" t="s">
         <v>0</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>202</v>
+        <v>220</v>
       </c>
       <c r="E4" t="s">
         <v>1</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>203</v>
+        <v>221</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>204</v>
+        <v>222</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
-        <v>41744</v>
+        <v>41746</v>
       </c>
       <c r="B5" t="s">
-        <v>185</v>
+        <v>197</v>
       </c>
       <c r="C5" t="s">
         <v>0</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>205</v>
+        <v>198</v>
       </c>
       <c r="E5" t="s">
-        <v>1</v>
+        <v>156</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>206</v>
+        <v>9</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>207</v>
+        <v>199</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -1152,505 +1187,505 @@
         <v>41744</v>
       </c>
       <c r="B6" t="s">
-        <v>185</v>
+        <v>135</v>
       </c>
       <c r="C6" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>208</v>
+        <v>200</v>
       </c>
       <c r="E6" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>209</v>
+        <v>67</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>210</v>
+        <v>201</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
-        <v>41743</v>
+        <v>41744</v>
       </c>
       <c r="B7" t="s">
-        <v>3</v>
+        <v>189</v>
       </c>
       <c r="C7" t="s">
         <v>0</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>211</v>
+        <v>202</v>
       </c>
       <c r="E7" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>6</v>
+        <v>203</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>212</v>
+        <v>204</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
-        <v>41743</v>
+        <v>41744</v>
       </c>
       <c r="B8" t="s">
-        <v>3</v>
+        <v>185</v>
       </c>
       <c r="C8" t="s">
         <v>0</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>213</v>
+        <v>205</v>
       </c>
       <c r="E8" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>214</v>
+        <v>206</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>215</v>
+        <v>207</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
-        <v>41743</v>
+        <v>41744</v>
       </c>
       <c r="B9" t="s">
-        <v>2</v>
+        <v>185</v>
       </c>
       <c r="C9" t="s">
         <v>0</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>216</v>
+        <v>208</v>
       </c>
       <c r="E9" t="s">
         <v>1</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>217</v>
+        <v>209</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
-        <v>41740</v>
+        <v>41743</v>
       </c>
       <c r="B10" t="s">
-        <v>185</v>
+        <v>3</v>
       </c>
       <c r="C10" t="s">
         <v>0</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>186</v>
+        <v>211</v>
       </c>
       <c r="E10" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>187</v>
+        <v>6</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>196</v>
+        <v>212</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
-        <v>41740</v>
+        <v>41743</v>
       </c>
       <c r="B11" t="s">
-        <v>42</v>
+        <v>3</v>
       </c>
       <c r="C11" t="s">
         <v>0</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>188</v>
+        <v>213</v>
       </c>
       <c r="E11" t="s">
-        <v>44</v>
+        <v>5</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>15</v>
+        <v>214</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>195</v>
+        <v>215</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
-        <v>41739</v>
+        <v>41743</v>
       </c>
       <c r="B12" t="s">
-        <v>189</v>
+        <v>2</v>
       </c>
       <c r="C12" t="s">
         <v>0</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>190</v>
+        <v>216</v>
       </c>
       <c r="E12" t="s">
         <v>1</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>191</v>
+        <v>217</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>194</v>
+        <v>218</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
-        <v>41739</v>
+        <v>41740</v>
       </c>
       <c r="B13" t="s">
-        <v>42</v>
+        <v>185</v>
       </c>
       <c r="C13" t="s">
         <v>0</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
       <c r="E13" t="s">
-        <v>44</v>
+        <v>1</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>67</v>
+        <v>187</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
-        <v>41738</v>
+        <v>41740</v>
       </c>
       <c r="B14" t="s">
-        <v>3</v>
+        <v>42</v>
       </c>
       <c r="C14" t="s">
         <v>0</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>183</v>
+        <v>188</v>
       </c>
       <c r="E14" t="s">
-        <v>5</v>
+        <v>44</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>165</v>
+        <v>15</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>184</v>
+        <v>195</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
-        <v>41737</v>
+        <v>41739</v>
       </c>
       <c r="B15" t="s">
-        <v>3</v>
+        <v>189</v>
       </c>
       <c r="C15" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>173</v>
+        <v>190</v>
       </c>
       <c r="E15" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>174</v>
+        <v>191</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>181</v>
+        <v>194</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
-        <v>41736</v>
+        <v>41739</v>
       </c>
       <c r="B16" t="s">
-        <v>175</v>
+        <v>42</v>
       </c>
       <c r="C16" t="s">
         <v>0</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>176</v>
+        <v>192</v>
       </c>
       <c r="E16" t="s">
-        <v>1</v>
+        <v>44</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>174</v>
+        <v>67</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>182</v>
+        <v>193</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
-        <v>41736</v>
+        <v>41738</v>
       </c>
       <c r="B17" t="s">
-        <v>59</v>
+        <v>3</v>
       </c>
       <c r="C17" t="s">
         <v>0</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>177</v>
+        <v>183</v>
       </c>
       <c r="E17" t="s">
         <v>5</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>178</v>
+        <v>165</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
-        <v>41736</v>
+        <v>41737</v>
       </c>
       <c r="B18" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C18" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="E18" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F18" s="3" t="s">
         <v>174</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
-        <v>41731</v>
+        <v>41736</v>
       </c>
       <c r="B19" t="s">
-        <v>3</v>
+        <v>175</v>
       </c>
       <c r="C19" t="s">
         <v>0</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>167</v>
+        <v>176</v>
       </c>
       <c r="E19" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>15</v>
+        <v>174</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>171</v>
+        <v>182</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
-        <v>41731</v>
+        <v>41736</v>
       </c>
       <c r="B20" t="s">
-        <v>32</v>
+        <v>59</v>
       </c>
       <c r="C20" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>168</v>
+        <v>177</v>
       </c>
       <c r="E20" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>15</v>
+        <v>178</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>172</v>
+        <v>181</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
-        <v>41729</v>
+        <v>41736</v>
       </c>
       <c r="B21" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="C21" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>169</v>
+        <v>179</v>
       </c>
       <c r="E21" t="s">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>170</v>
+        <v>174</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>171</v>
+        <v>180</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
-        <v>41729</v>
+        <v>41731</v>
       </c>
       <c r="B22" t="s">
         <v>3</v>
       </c>
       <c r="C22" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="E22" t="s">
         <v>5</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>165</v>
+        <v>15</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>166</v>
+        <v>171</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
-        <v>41725</v>
+        <v>41731</v>
       </c>
       <c r="B23" t="s">
-        <v>3</v>
+        <v>32</v>
       </c>
       <c r="C23" t="s">
         <v>4</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>159</v>
+        <v>168</v>
       </c>
       <c r="E23" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>160</v>
+        <v>15</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>163</v>
+        <v>172</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
-        <v>41725</v>
+        <v>41729</v>
       </c>
       <c r="B24" t="s">
-        <v>144</v>
+        <v>17</v>
       </c>
       <c r="C24" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>161</v>
+        <v>169</v>
       </c>
       <c r="E24" t="s">
-        <v>146</v>
+        <v>19</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>6</v>
+        <v>170</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>162</v>
+        <v>171</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
-        <v>41722</v>
+        <v>41729</v>
       </c>
       <c r="B25" t="s">
-        <v>151</v>
+        <v>3</v>
       </c>
       <c r="C25" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>152</v>
+        <v>164</v>
       </c>
       <c r="E25" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>153</v>
+        <v>165</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>158</v>
+        <v>166</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
-        <v>41722</v>
+        <v>41725</v>
       </c>
       <c r="B26" t="s">
-        <v>154</v>
+        <v>3</v>
       </c>
       <c r="C26" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="E26" t="s">
-        <v>156</v>
+        <v>5</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>6</v>
+        <v>160</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>157</v>
+        <v>163</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
-        <v>41722</v>
+        <v>41725</v>
       </c>
       <c r="B27" t="s">
-        <v>3</v>
+        <v>144</v>
       </c>
       <c r="C27" t="s">
         <v>0</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>143</v>
+        <v>161</v>
       </c>
       <c r="E27" t="s">
-        <v>5</v>
+        <v>146</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>150</v>
+        <v>162</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
@@ -1658,551 +1693,551 @@
         <v>41722</v>
       </c>
       <c r="B28" t="s">
-        <v>144</v>
+        <v>151</v>
       </c>
       <c r="C28" t="s">
         <v>0</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>145</v>
+        <v>152</v>
       </c>
       <c r="E28" t="s">
-        <v>146</v>
+        <v>1</v>
       </c>
       <c r="F28" s="3" t="s">
-        <v>27</v>
+        <v>153</v>
       </c>
       <c r="G28" s="3" t="s">
-        <v>149</v>
+        <v>158</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
-        <v>41719</v>
+        <v>41722</v>
       </c>
       <c r="B29" t="s">
-        <v>32</v>
+        <v>154</v>
       </c>
       <c r="C29" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>147</v>
+        <v>155</v>
       </c>
       <c r="E29" t="s">
-        <v>10</v>
+        <v>156</v>
       </c>
       <c r="F29" s="3" t="s">
         <v>6</v>
       </c>
       <c r="G29" s="3" t="s">
-        <v>148</v>
+        <v>157</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
-        <v>41712</v>
+        <v>41722</v>
       </c>
       <c r="B30" t="s">
-        <v>139</v>
+        <v>3</v>
       </c>
       <c r="C30" t="s">
         <v>0</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="E30" t="s">
         <v>5</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>141</v>
+        <v>9</v>
       </c>
       <c r="G30" s="3" t="s">
-        <v>142</v>
+        <v>150</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
-        <v>41708</v>
+        <v>41722</v>
       </c>
       <c r="B31" t="s">
-        <v>135</v>
+        <v>144</v>
       </c>
       <c r="C31" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>136</v>
+        <v>145</v>
       </c>
       <c r="E31" t="s">
-        <v>5</v>
+        <v>146</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>6</v>
+        <v>27</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>138</v>
+        <v>149</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
-        <v>41705</v>
+        <v>41719</v>
       </c>
       <c r="B32" t="s">
-        <v>59</v>
+        <v>32</v>
       </c>
       <c r="C32" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>137</v>
+        <v>147</v>
       </c>
       <c r="E32" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>133</v>
+        <v>6</v>
       </c>
       <c r="G32" s="3" t="s">
-        <v>131</v>
+        <v>148</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
-        <v>41703</v>
+        <v>41712</v>
       </c>
       <c r="B33" t="s">
-        <v>3</v>
+        <v>139</v>
       </c>
       <c r="C33" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>132</v>
+        <v>140</v>
       </c>
       <c r="E33" t="s">
         <v>5</v>
       </c>
       <c r="F33" s="3" t="s">
-        <v>133</v>
+        <v>141</v>
       </c>
       <c r="G33" s="3" t="s">
-        <v>134</v>
+        <v>142</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
-        <v>41703</v>
+        <v>41708</v>
       </c>
       <c r="B34" t="s">
-        <v>117</v>
+        <v>135</v>
       </c>
       <c r="C34" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>118</v>
+        <v>136</v>
       </c>
       <c r="E34" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>119</v>
+        <v>6</v>
       </c>
       <c r="G34" s="3" t="s">
-        <v>131</v>
+        <v>138</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
-        <v>41703</v>
+        <v>41705</v>
       </c>
       <c r="B35" t="s">
-        <v>2</v>
+        <v>59</v>
       </c>
       <c r="C35" t="s">
         <v>0</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>120</v>
+        <v>137</v>
       </c>
       <c r="E35" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>121</v>
+        <v>133</v>
       </c>
       <c r="G35" s="3" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
-        <v>41698</v>
+        <v>41703</v>
       </c>
       <c r="B36" t="s">
-        <v>17</v>
+        <v>3</v>
       </c>
       <c r="C36" t="s">
         <v>4</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>122</v>
+        <v>132</v>
       </c>
       <c r="E36" t="s">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="F36" s="3" t="s">
-        <v>123</v>
+        <v>133</v>
       </c>
       <c r="G36" s="3" t="s">
-        <v>129</v>
+        <v>134</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
-        <v>41691</v>
+        <v>41703</v>
       </c>
       <c r="B37" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="C37" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="E37" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F37" s="3" t="s">
-        <v>67</v>
+        <v>119</v>
       </c>
       <c r="G37" s="3" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
-        <v>41691</v>
+        <v>41703</v>
       </c>
       <c r="B38" t="s">
-        <v>124</v>
+        <v>2</v>
       </c>
       <c r="C38" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="E38" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F38" s="3" t="s">
-        <v>67</v>
+        <v>121</v>
       </c>
       <c r="G38" s="3" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
-        <v>41690</v>
+        <v>41698</v>
       </c>
       <c r="B39" t="s">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="C39" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>113</v>
+        <v>122</v>
       </c>
       <c r="E39" t="s">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="F39" s="3" t="s">
-        <v>114</v>
+        <v>123</v>
       </c>
       <c r="G39" s="3" t="s">
-        <v>112</v>
+        <v>129</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
-        <v>41690</v>
+        <v>41691</v>
       </c>
       <c r="B40" t="s">
-        <v>3</v>
+        <v>124</v>
       </c>
       <c r="C40" t="s">
         <v>4</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>115</v>
+        <v>125</v>
       </c>
       <c r="E40" t="s">
         <v>5</v>
       </c>
       <c r="F40" s="3" t="s">
-        <v>114</v>
+        <v>67</v>
       </c>
       <c r="G40" s="3" t="s">
-        <v>116</v>
+        <v>128</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
-        <v>41682</v>
+        <v>41691</v>
       </c>
       <c r="B41" t="s">
-        <v>106</v>
+        <v>124</v>
       </c>
       <c r="C41" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>107</v>
+        <v>126</v>
       </c>
       <c r="E41" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="F41" s="3" t="s">
-        <v>108</v>
+        <v>67</v>
       </c>
       <c r="G41" s="3" t="s">
-        <v>112</v>
+        <v>127</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
-        <v>41680</v>
+        <v>41690</v>
       </c>
       <c r="B42" t="s">
-        <v>32</v>
+        <v>3</v>
       </c>
       <c r="C42" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="E42" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="F42" s="3" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="G42" s="3" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
-        <v>41680</v>
+        <v>41690</v>
       </c>
       <c r="B43" t="s">
         <v>3</v>
       </c>
       <c r="C43" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>105</v>
+        <v>115</v>
       </c>
       <c r="E43" t="s">
         <v>5</v>
       </c>
       <c r="F43" s="3" t="s">
-        <v>6</v>
+        <v>114</v>
       </c>
       <c r="G43" s="3" t="s">
-        <v>98</v>
+        <v>116</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
-        <v>41677</v>
+        <v>41682</v>
       </c>
       <c r="B44" t="s">
-        <v>32</v>
+        <v>106</v>
       </c>
       <c r="C44" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>99</v>
+        <v>107</v>
       </c>
       <c r="E44" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F44" s="3" t="s">
-        <v>6</v>
+        <v>108</v>
       </c>
       <c r="G44" s="3" t="s">
-        <v>104</v>
+        <v>112</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
-        <v>41677</v>
+        <v>41680</v>
       </c>
       <c r="B45" t="s">
-        <v>59</v>
+        <v>32</v>
       </c>
       <c r="C45" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>100</v>
+        <v>109</v>
       </c>
       <c r="E45" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="F45" s="3" t="s">
-        <v>101</v>
+        <v>110</v>
       </c>
       <c r="G45" s="3" t="s">
-        <v>98</v>
+        <v>111</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
-        <v>41676</v>
+        <v>41680</v>
       </c>
       <c r="B46" t="s">
         <v>3</v>
       </c>
       <c r="C46" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="E46" t="s">
         <v>5</v>
       </c>
       <c r="F46" s="3" t="s">
-        <v>101</v>
+        <v>6</v>
       </c>
       <c r="G46" s="3" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
-        <v>41674</v>
+        <v>41677</v>
       </c>
       <c r="B47" t="s">
-        <v>95</v>
+        <v>32</v>
       </c>
       <c r="C47" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="E47" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F47" s="3" t="s">
-        <v>97</v>
+        <v>6</v>
       </c>
       <c r="G47" s="3" t="s">
-        <v>98</v>
+        <v>104</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
-        <v>41670</v>
+        <v>41677</v>
       </c>
       <c r="B48" t="s">
-        <v>17</v>
+        <v>59</v>
       </c>
       <c r="C48" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>18</v>
+        <v>100</v>
       </c>
       <c r="E48" t="s">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="F48" s="3" t="s">
-        <v>20</v>
+        <v>101</v>
       </c>
       <c r="G48" s="3" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
-        <v>41666</v>
+        <v>41676</v>
       </c>
       <c r="B49" t="s">
         <v>3</v>
       </c>
       <c r="C49" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>21</v>
+        <v>102</v>
       </c>
       <c r="E49" t="s">
         <v>5</v>
       </c>
       <c r="F49" s="3" t="s">
-        <v>71</v>
+        <v>101</v>
       </c>
       <c r="G49" s="3" t="s">
-        <v>93</v>
+        <v>103</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
-        <v>41666</v>
+        <v>41674</v>
       </c>
       <c r="B50" t="s">
-        <v>2</v>
+        <v>95</v>
       </c>
       <c r="C50" t="s">
         <v>0</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>22</v>
+        <v>96</v>
       </c>
       <c r="E50" t="s">
         <v>1</v>
       </c>
       <c r="F50" s="3" t="s">
-        <v>23</v>
+        <v>97</v>
       </c>
       <c r="G50" s="3" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
-        <v>41666</v>
+        <v>41670</v>
       </c>
       <c r="B51" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="C51" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="E51" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="F51" s="3" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="G51" s="3" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
@@ -2210,344 +2245,344 @@
         <v>41666</v>
       </c>
       <c r="B52" t="s">
-        <v>28</v>
+        <v>3</v>
       </c>
       <c r="C52" t="s">
         <v>0</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="E52" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F52" s="3" t="s">
-        <v>30</v>
+        <v>71</v>
       </c>
       <c r="G52" s="3" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
-        <v>41660</v>
+        <v>41666</v>
       </c>
       <c r="B53" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="C53" t="s">
         <v>0</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="E53" t="s">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="F53" s="3" t="s">
-        <v>9</v>
+        <v>23</v>
       </c>
       <c r="G53" s="3" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
-        <v>41660</v>
+        <v>41666</v>
       </c>
       <c r="B54" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="C54" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="E54" t="s">
-        <v>10</v>
+        <v>26</v>
       </c>
       <c r="F54" s="3" t="s">
-        <v>6</v>
+        <v>27</v>
       </c>
       <c r="G54" s="3" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
-        <v>41660</v>
+        <v>41666</v>
       </c>
       <c r="B55" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="C55" t="s">
         <v>0</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="E55" t="s">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="F55" s="3" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="G55" s="3" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
-        <v>41659</v>
+        <v>41660</v>
       </c>
       <c r="B56" t="s">
-        <v>37</v>
+        <v>11</v>
       </c>
       <c r="C56" t="s">
         <v>0</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="E56" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="F56" s="3" t="s">
-        <v>39</v>
+        <v>9</v>
       </c>
       <c r="G56" s="3" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
-        <v>41655</v>
+        <v>41660</v>
       </c>
       <c r="B57" t="s">
-        <v>2</v>
+        <v>32</v>
       </c>
       <c r="C57" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="E57" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F57" s="3" t="s">
-        <v>41</v>
+        <v>6</v>
       </c>
       <c r="G57" s="3" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
-        <v>41655</v>
+        <v>41660</v>
       </c>
       <c r="B58" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="C58" t="s">
         <v>0</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="E58" t="s">
-        <v>44</v>
+        <v>12</v>
       </c>
       <c r="F58" s="3" t="s">
-        <v>6</v>
+        <v>36</v>
       </c>
       <c r="G58" s="3" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
-        <v>41652</v>
+        <v>41659</v>
       </c>
       <c r="B59" t="s">
-        <v>3</v>
+        <v>37</v>
       </c>
       <c r="C59" t="s">
         <v>0</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="E59" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F59" s="3" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="G59" s="3" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
-        <v>41649</v>
+        <v>41655</v>
       </c>
       <c r="B60" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C60" t="s">
         <v>0</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>16</v>
+        <v>40</v>
       </c>
       <c r="E60" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F60" s="3" t="s">
-        <v>15</v>
+        <v>41</v>
       </c>
       <c r="G60" s="3" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
-        <v>41648</v>
+        <v>41655</v>
       </c>
       <c r="B61" t="s">
-        <v>2</v>
+        <v>42</v>
       </c>
       <c r="C61" t="s">
         <v>0</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="E61" t="s">
-        <v>1</v>
+        <v>44</v>
       </c>
       <c r="F61" s="3" t="s">
-        <v>48</v>
+        <v>6</v>
       </c>
       <c r="G61" s="3" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
-        <v>41648</v>
+        <v>41652</v>
       </c>
       <c r="B62" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C62" t="s">
         <v>0</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="E62" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F62" s="3" t="s">
-        <v>9</v>
+        <v>46</v>
       </c>
       <c r="G62" s="3" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
-        <v>41647</v>
+        <v>41649</v>
       </c>
       <c r="B63" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C63" t="s">
         <v>0</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>50</v>
+        <v>16</v>
       </c>
       <c r="E63" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F63" s="3" t="s">
-        <v>51</v>
+        <v>15</v>
       </c>
       <c r="G63" s="3" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
-        <v>41646</v>
+        <v>41648</v>
       </c>
       <c r="B64" t="s">
-        <v>52</v>
+        <v>2</v>
       </c>
       <c r="C64" t="s">
         <v>0</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="E64" t="s">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="F64" s="3" t="s">
-        <v>13</v>
+        <v>48</v>
       </c>
       <c r="G64" s="3" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
-        <v>41646</v>
+        <v>41648</v>
       </c>
       <c r="B65" t="s">
-        <v>54</v>
+        <v>7</v>
       </c>
       <c r="C65" t="s">
         <v>0</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="E65" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F65" s="3" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="G65" s="3" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
-        <v>41646</v>
+        <v>41647</v>
       </c>
       <c r="B66" t="s">
-        <v>56</v>
+        <v>2</v>
       </c>
       <c r="C66" t="s">
         <v>0</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="E66" t="s">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="F66" s="3" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="G66" s="3" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
@@ -2555,107 +2590,176 @@
         <v>41646</v>
       </c>
       <c r="B67" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="C67" t="s">
         <v>0</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="E67" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="F67" s="3" t="s">
-        <v>61</v>
+        <v>13</v>
       </c>
       <c r="G67" s="3" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
-        <v>41645</v>
+        <v>41646</v>
       </c>
       <c r="B68" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="C68" t="s">
         <v>0</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="E68" t="s">
-        <v>64</v>
+        <v>12</v>
       </c>
       <c r="F68" s="3" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="G68" s="3" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
-        <v>41642</v>
+        <v>41646</v>
       </c>
       <c r="B69" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="C69" t="s">
         <v>0</v>
       </c>
       <c r="D69" s="2" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="E69" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F69" s="3" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
       <c r="G69" s="3" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
+        <v>41646</v>
+      </c>
+      <c r="B70" t="s">
+        <v>59</v>
+      </c>
+      <c r="C70" t="s">
+        <v>0</v>
+      </c>
+      <c r="D70" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="E70" t="s">
+        <v>5</v>
+      </c>
+      <c r="F70" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="G70" s="3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A71" s="1">
+        <v>41645</v>
+      </c>
+      <c r="B71" t="s">
+        <v>62</v>
+      </c>
+      <c r="C71" t="s">
+        <v>0</v>
+      </c>
+      <c r="D71" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="E71" t="s">
+        <v>64</v>
+      </c>
+      <c r="F71" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G71" s="3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A72" s="1">
+        <v>41642</v>
+      </c>
+      <c r="B72" t="s">
+        <v>65</v>
+      </c>
+      <c r="C72" t="s">
+        <v>0</v>
+      </c>
+      <c r="D72" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="E72" t="s">
+        <v>10</v>
+      </c>
+      <c r="F72" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="G72" s="3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A73" s="1">
         <v>41641</v>
       </c>
-      <c r="B70" t="s">
+      <c r="B73" t="s">
         <v>68</v>
       </c>
-      <c r="C70" t="s">
-        <v>0</v>
-      </c>
-      <c r="D70" s="2" t="s">
+      <c r="C73" t="s">
+        <v>0</v>
+      </c>
+      <c r="D73" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="E70" t="s">
+      <c r="E73" t="s">
         <v>1</v>
       </c>
-      <c r="F70" s="3" t="s">
+      <c r="F73" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="G70" s="3" t="s">
+      <c r="G73" s="3" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A71" s="1"/>
-    </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A72" s="1"/>
-    </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A73" s="1"/>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" s="1"/>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" s="1"/>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A76" s="1"/>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A77" s="1"/>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A78" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Actualizando el modelo. Agregando .bat de backup y volviendo al fixtures.
</commit_message>
<xml_diff>
--- a/backup/cuenta_2200555126.xlsx
+++ b/backup/cuenta_2200555126.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="492" uniqueCount="260">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="576" uniqueCount="300">
   <si>
     <t>D</t>
   </si>
@@ -804,6 +804,126 @@
   </si>
   <si>
     <t>398.23</t>
+  </si>
+  <si>
+    <t>0005182581</t>
+  </si>
+  <si>
+    <t>100.00</t>
+  </si>
+  <si>
+    <t>0008769504</t>
+  </si>
+  <si>
+    <t>30.41  </t>
+  </si>
+  <si>
+    <t>0.00</t>
+  </si>
+  <si>
+    <t>0000838805</t>
+  </si>
+  <si>
+    <t>30.00  </t>
+  </si>
+  <si>
+    <t>30.41</t>
+  </si>
+  <si>
+    <t>0000748263</t>
+  </si>
+  <si>
+    <t>280.79  </t>
+  </si>
+  <si>
+    <t>0.41</t>
+  </si>
+  <si>
+    <t>CONSUMO DATA DOMINOS ELOY ALFARO</t>
+  </si>
+  <si>
+    <t>0009250507</t>
+  </si>
+  <si>
+    <t>23.08  </t>
+  </si>
+  <si>
+    <t>281.20</t>
+  </si>
+  <si>
+    <t>0000985249</t>
+  </si>
+  <si>
+    <t>0.35  </t>
+  </si>
+  <si>
+    <t>304.28</t>
+  </si>
+  <si>
+    <t>0000963714</t>
+  </si>
+  <si>
+    <t>9.40  </t>
+  </si>
+  <si>
+    <t>304.63</t>
+  </si>
+  <si>
+    <t>CONSUMO VISA NA FAMOSOS MOTES BILOXI</t>
+  </si>
+  <si>
+    <t>0004666280</t>
+  </si>
+  <si>
+    <t>10.34  </t>
+  </si>
+  <si>
+    <t>314.03</t>
+  </si>
+  <si>
+    <t>0011233941</t>
+  </si>
+  <si>
+    <t>60.00  </t>
+  </si>
+  <si>
+    <t>324.37</t>
+  </si>
+  <si>
+    <t>0009892623</t>
+  </si>
+  <si>
+    <t>270.00  </t>
+  </si>
+  <si>
+    <t>384.37</t>
+  </si>
+  <si>
+    <t>0009867157</t>
+  </si>
+  <si>
+    <t>114.37</t>
+  </si>
+  <si>
+    <t>0009838540</t>
+  </si>
+  <si>
+    <t>64.66  </t>
+  </si>
+  <si>
+    <t>0005008981</t>
+  </si>
+  <si>
+    <t>449.03</t>
+  </si>
+  <si>
+    <t>0002663087</t>
+  </si>
+  <si>
+    <t>29.83  </t>
+  </si>
+  <si>
+    <t>129.83</t>
   </si>
 </sst>
 </file>
@@ -1126,10 +1246,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H87"/>
+  <dimension ref="A1:H101"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1:H2"/>
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1141,1912 +1261,2242 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1">
-        <v>41759</v>
+        <v>41785</v>
       </c>
       <c r="B1" t="s">
-        <v>17</v>
+        <v>3</v>
       </c>
       <c r="C1" t="s">
         <v>4</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>254</v>
+        <v>297</v>
       </c>
       <c r="E1" t="s">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>255</v>
+        <v>298</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>256</v>
+        <v>299</v>
       </c>
       <c r="H1" t="str">
-        <f t="shared" ref="H1:H9" ca="1" si="0">CONCATENATE("array('mo_fecha' =&gt; new \DateTime('",TEXT(A1,"yyyy-mm-dd"),"'), 'mo_concepto' =&gt; '",B1,"', 'mo_tipo' =&gt; '",C1,"', 'mo_documento' =&gt; '",D1,"', 'mo_oficina' =&gt; '",E1,"', 'mo_monto' =&gt; ",F1,", 'mo_saldo' =&gt; ",G1,", 'mo_fecha_crea' =&gt; new \DateTime('",TEXT(NOW(),"yyyy-mm-dd H:m:s"),"'), 'mo_quien_crea' =&gt; 1, 'mo_fecha_modifica' =&gt; NULL, 'mo_quien_modifica' =&gt; NULL, 'mo_fecha_borrado' =&gt; NULL, 'mo_quien_borra' =&gt; NULL, 'mo_borrado_logico' =&gt; false),")</f>
-        <v>array('mo_fecha' =&gt; new \DateTime('2014-04-30'), 'mo_concepto' =&gt; 'INTERES A SU FAVOR', 'mo_tipo' =&gt; 'C', 'mo_documento' =&gt; '0000858282', 'mo_oficina' =&gt; 'AGENCIA PARA PROCESOS BATCH', 'mo_monto' =&gt; 0.80  , 'mo_saldo' =&gt; 399.03, 'mo_fecha_crea' =&gt; new \DateTime('2014-05-02 8:2:16'), 'mo_quien_crea' =&gt; 1, 'mo_fecha_modifica' =&gt; NULL, 'mo_quien_modifica' =&gt; NULL, 'mo_fecha_borrado' =&gt; NULL, 'mo_quien_borra' =&gt; NULL, 'mo_borrado_logico' =&gt; false),</v>
+        <f t="shared" ref="H1:H14" ca="1" si="0">CONCATENATE("array('mo_fecha' =&gt; new \DateTime('",TEXT(A1,"yyyy-mm-dd"),"'), 'mo_concepto' =&gt; '",B1,"', 'mo_tipo' =&gt; '",C1,"', 'mo_documento' =&gt; '",D1,"', 'mo_oficina' =&gt; '",E1,"', 'mo_monto' =&gt; ",F1,", 'mo_saldo' =&gt; ",G1,", 'mo_fecha_crea' =&gt; new \DateTime('",TEXT(NOW(),"yyyy-mm-dd H:m:s"),"'), 'mo_quien_crea' =&gt; 1, 'mo_fecha_modifica' =&gt; NULL, 'mo_quien_modifica' =&gt; NULL, 'mo_fecha_borrado' =&gt; NULL, 'mo_quien_borra' =&gt; NULL, 'mo_borrado_logico' =&gt; false),")</f>
+        <v>array('mo_fecha' =&gt; new \DateTime('2014-05-26'), 'mo_concepto' =&gt; '  TRANSFERENCIA INTERNET', 'mo_tipo' =&gt; 'C', 'mo_documento' =&gt; '0002663087', 'mo_oficina' =&gt; 'AG. NORTE', 'mo_monto' =&gt; 29.83  , 'mo_saldo' =&gt; 129.83, 'mo_fecha_crea' =&gt; new \DateTime('2014-05-24 20:44:24'), 'mo_quien_crea' =&gt; 1, 'mo_fecha_modifica' =&gt; NULL, 'mo_quien_modifica' =&gt; NULL, 'mo_fecha_borrado' =&gt; NULL, 'mo_quien_borra' =&gt; NULL, 'mo_borrado_logico' =&gt; false),</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>41758</v>
+        <v>41781</v>
       </c>
       <c r="B2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>257</v>
+        <v>260</v>
       </c>
       <c r="E2" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>258</v>
+        <v>6</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>259</v>
-      </c>
-      <c r="H2" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>array('mo_fecha' =&gt; new \DateTime('2014-04-29'), 'mo_concepto' =&gt; 'CONSUMO DATA AKI MOLINEROS 161', 'mo_tipo' =&gt; 'D', 'mo_documento' =&gt; '0008677801', 'mo_oficina' =&gt; 'INSTITUCIONAL SS.CC.', 'mo_monto' =&gt; 20.79  , 'mo_saldo' =&gt; 398.23, 'mo_fecha_crea' =&gt; new \DateTime('2014-05-02 8:2:16'), 'mo_quien_crea' =&gt; 1, 'mo_fecha_modifica' =&gt; NULL, 'mo_quien_modifica' =&gt; NULL, 'mo_fecha_borrado' =&gt; NULL, 'mo_quien_borra' =&gt; NULL, 'mo_borrado_logico' =&gt; false),</v>
+        <v>261</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>41757</v>
+        <v>41779</v>
       </c>
       <c r="B3" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C3" t="s">
         <v>0</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>232</v>
+        <v>262</v>
       </c>
       <c r="E3" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>233</v>
+        <v>263</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>234</v>
+        <v>264</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
-        <v>41757</v>
+        <v>41767</v>
       </c>
       <c r="B4" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>235</v>
+        <v>265</v>
       </c>
       <c r="E4" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>236</v>
+        <v>266</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>237</v>
+        <v>267</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
-        <v>41757</v>
+        <v>41766</v>
       </c>
       <c r="B5" t="s">
-        <v>238</v>
+        <v>59</v>
       </c>
       <c r="C5" t="s">
         <v>0</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>239</v>
+        <v>268</v>
       </c>
       <c r="E5" t="s">
-        <v>146</v>
+        <v>5</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>67</v>
+        <v>269</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>240</v>
+        <v>270</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
-        <v>41754</v>
+        <v>41765</v>
       </c>
       <c r="B6" t="s">
-        <v>241</v>
+        <v>271</v>
       </c>
       <c r="C6" t="s">
         <v>0</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>242</v>
+        <v>272</v>
       </c>
       <c r="E6" t="s">
         <v>1</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>243</v>
+        <v>273</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>244</v>
+        <v>274</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
-        <v>41754</v>
+        <v>41765</v>
       </c>
       <c r="B7" t="s">
-        <v>245</v>
+        <v>3</v>
       </c>
       <c r="C7" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>246</v>
+        <v>275</v>
       </c>
       <c r="E7" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>247</v>
+        <v>276</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>253</v>
+        <v>277</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
-        <v>41754</v>
+        <v>41765</v>
       </c>
       <c r="B8" t="s">
-        <v>248</v>
+        <v>3</v>
       </c>
       <c r="C8" t="s">
         <v>0</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>249</v>
+        <v>278</v>
       </c>
       <c r="E8" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>247</v>
+        <v>279</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>250</v>
+        <v>280</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
-        <v>41754</v>
+        <v>41764</v>
       </c>
       <c r="B9" t="s">
-        <v>32</v>
+        <v>281</v>
       </c>
       <c r="C9" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>251</v>
+        <v>282</v>
       </c>
       <c r="E9" t="s">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>252</v>
+        <v>283</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>253</v>
+        <v>284</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
-        <v>41752</v>
+        <v>41761</v>
       </c>
       <c r="B10" t="s">
-        <v>223</v>
+        <v>3</v>
       </c>
       <c r="C10" t="s">
         <v>0</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>224</v>
+        <v>285</v>
       </c>
       <c r="E10" t="s">
-        <v>156</v>
+        <v>5</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>225</v>
+        <v>286</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>226</v>
+        <v>287</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
-        <v>41751</v>
+        <v>41761</v>
       </c>
       <c r="B11" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C11" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>227</v>
+        <v>288</v>
       </c>
       <c r="E11" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>228</v>
+        <v>289</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>229</v>
+        <v>290</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
-        <v>41751</v>
+        <v>41761</v>
       </c>
       <c r="B12" t="s">
-        <v>144</v>
+        <v>3</v>
       </c>
       <c r="C12" t="s">
         <v>0</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>230</v>
+        <v>291</v>
       </c>
       <c r="E12" t="s">
-        <v>146</v>
+        <v>5</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>6</v>
+        <v>289</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>231</v>
+        <v>292</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
-        <v>41750</v>
+        <v>41761</v>
       </c>
       <c r="B13" t="s">
-        <v>219</v>
+        <v>3</v>
       </c>
       <c r="C13" t="s">
         <v>0</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>220</v>
+        <v>293</v>
       </c>
       <c r="E13" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>221</v>
+        <v>294</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>222</v>
+        <v>290</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
-        <v>41746</v>
+        <v>41761</v>
       </c>
       <c r="B14" t="s">
-        <v>197</v>
+        <v>3</v>
       </c>
       <c r="C14" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>198</v>
+        <v>295</v>
       </c>
       <c r="E14" t="s">
-        <v>156</v>
+        <v>5</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>9</v>
+        <v>67</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>199</v>
+        <v>296</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
-        <v>41744</v>
+        <v>41759</v>
       </c>
       <c r="B15" t="s">
-        <v>135</v>
+        <v>17</v>
       </c>
       <c r="C15" t="s">
         <v>4</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>200</v>
+        <v>254</v>
       </c>
       <c r="E15" t="s">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>67</v>
+        <v>255</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>201</v>
+        <v>256</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
-        <v>41744</v>
+        <v>41758</v>
       </c>
       <c r="B16" t="s">
-        <v>189</v>
+        <v>2</v>
       </c>
       <c r="C16" t="s">
         <v>0</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>202</v>
+        <v>257</v>
       </c>
       <c r="E16" t="s">
         <v>1</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>203</v>
+        <v>258</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>204</v>
+        <v>259</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
-        <v>41744</v>
+        <v>41757</v>
       </c>
       <c r="B17" t="s">
-        <v>185</v>
+        <v>2</v>
       </c>
       <c r="C17" t="s">
         <v>0</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>205</v>
+        <v>232</v>
       </c>
       <c r="E17" t="s">
         <v>1</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>206</v>
+        <v>233</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>207</v>
+        <v>234</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
-        <v>41744</v>
+        <v>41757</v>
       </c>
       <c r="B18" t="s">
-        <v>185</v>
+        <v>2</v>
       </c>
       <c r="C18" t="s">
         <v>0</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>208</v>
+        <v>235</v>
       </c>
       <c r="E18" t="s">
         <v>1</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>209</v>
+        <v>236</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>210</v>
+        <v>237</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
-        <v>41743</v>
+        <v>41757</v>
       </c>
       <c r="B19" t="s">
-        <v>3</v>
+        <v>238</v>
       </c>
       <c r="C19" t="s">
         <v>0</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>211</v>
+        <v>239</v>
       </c>
       <c r="E19" t="s">
-        <v>5</v>
+        <v>146</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>6</v>
+        <v>67</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>212</v>
+        <v>240</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
-        <v>41743</v>
+        <v>41754</v>
       </c>
       <c r="B20" t="s">
-        <v>3</v>
+        <v>241</v>
       </c>
       <c r="C20" t="s">
         <v>0</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>213</v>
+        <v>242</v>
       </c>
       <c r="E20" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>214</v>
+        <v>243</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>215</v>
+        <v>244</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
-        <v>41743</v>
+        <v>41754</v>
       </c>
       <c r="B21" t="s">
-        <v>2</v>
+        <v>245</v>
       </c>
       <c r="C21" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>216</v>
+        <v>246</v>
       </c>
       <c r="E21" t="s">
         <v>1</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>217</v>
+        <v>247</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>218</v>
+        <v>253</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
-        <v>41740</v>
+        <v>41754</v>
       </c>
       <c r="B22" t="s">
-        <v>185</v>
+        <v>248</v>
       </c>
       <c r="C22" t="s">
         <v>0</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>186</v>
+        <v>249</v>
       </c>
       <c r="E22" t="s">
         <v>1</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>187</v>
+        <v>247</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>196</v>
+        <v>250</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
-        <v>41740</v>
+        <v>41754</v>
       </c>
       <c r="B23" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="C23" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>188</v>
+        <v>251</v>
       </c>
       <c r="E23" t="s">
-        <v>44</v>
+        <v>10</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>15</v>
+        <v>252</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>195</v>
+        <v>253</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
-        <v>41739</v>
+        <v>41752</v>
       </c>
       <c r="B24" t="s">
-        <v>189</v>
+        <v>223</v>
       </c>
       <c r="C24" t="s">
         <v>0</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>190</v>
+        <v>224</v>
       </c>
       <c r="E24" t="s">
-        <v>1</v>
+        <v>156</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>191</v>
+        <v>225</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>194</v>
+        <v>226</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
-        <v>41739</v>
+        <v>41751</v>
       </c>
       <c r="B25" t="s">
-        <v>42</v>
+        <v>2</v>
       </c>
       <c r="C25" t="s">
         <v>0</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>192</v>
+        <v>227</v>
       </c>
       <c r="E25" t="s">
-        <v>44</v>
+        <v>1</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>67</v>
+        <v>228</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>193</v>
+        <v>229</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
-        <v>41738</v>
+        <v>41751</v>
       </c>
       <c r="B26" t="s">
-        <v>3</v>
+        <v>144</v>
       </c>
       <c r="C26" t="s">
         <v>0</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>183</v>
+        <v>230</v>
       </c>
       <c r="E26" t="s">
-        <v>5</v>
+        <v>146</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>165</v>
+        <v>6</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>184</v>
+        <v>231</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
-        <v>41737</v>
+        <v>41750</v>
       </c>
       <c r="B27" t="s">
-        <v>3</v>
+        <v>219</v>
       </c>
       <c r="C27" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>173</v>
+        <v>220</v>
       </c>
       <c r="E27" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>174</v>
+        <v>221</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>181</v>
+        <v>222</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
-        <v>41736</v>
+        <v>41746</v>
       </c>
       <c r="B28" t="s">
-        <v>175</v>
+        <v>197</v>
       </c>
       <c r="C28" t="s">
         <v>0</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>176</v>
+        <v>198</v>
       </c>
       <c r="E28" t="s">
-        <v>1</v>
+        <v>156</v>
       </c>
       <c r="F28" s="3" t="s">
-        <v>174</v>
+        <v>9</v>
       </c>
       <c r="G28" s="3" t="s">
-        <v>182</v>
+        <v>199</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
-        <v>41736</v>
+        <v>41744</v>
       </c>
       <c r="B29" t="s">
-        <v>59</v>
+        <v>135</v>
       </c>
       <c r="C29" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>177</v>
+        <v>200</v>
       </c>
       <c r="E29" t="s">
         <v>5</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>178</v>
+        <v>67</v>
       </c>
       <c r="G29" s="3" t="s">
-        <v>181</v>
+        <v>201</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
-        <v>41736</v>
+        <v>41744</v>
       </c>
       <c r="B30" t="s">
-        <v>7</v>
+        <v>189</v>
       </c>
       <c r="C30" t="s">
         <v>0</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>179</v>
+        <v>202</v>
       </c>
       <c r="E30" t="s">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>174</v>
+        <v>203</v>
       </c>
       <c r="G30" s="3" t="s">
-        <v>180</v>
+        <v>204</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
-        <v>41731</v>
+        <v>41744</v>
       </c>
       <c r="B31" t="s">
-        <v>3</v>
+        <v>185</v>
       </c>
       <c r="C31" t="s">
         <v>0</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>167</v>
+        <v>205</v>
       </c>
       <c r="E31" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>15</v>
+        <v>206</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>171</v>
+        <v>207</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
-        <v>41731</v>
+        <v>41744</v>
       </c>
       <c r="B32" t="s">
-        <v>32</v>
+        <v>185</v>
       </c>
       <c r="C32" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>168</v>
+        <v>208</v>
       </c>
       <c r="E32" t="s">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>15</v>
+        <v>209</v>
       </c>
       <c r="G32" s="3" t="s">
-        <v>172</v>
+        <v>210</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
-        <v>41729</v>
+        <v>41743</v>
       </c>
       <c r="B33" t="s">
-        <v>17</v>
+        <v>3</v>
       </c>
       <c r="C33" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>169</v>
+        <v>211</v>
       </c>
       <c r="E33" t="s">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="F33" s="3" t="s">
-        <v>170</v>
+        <v>6</v>
       </c>
       <c r="G33" s="3" t="s">
-        <v>171</v>
+        <v>212</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
-        <v>41729</v>
+        <v>41743</v>
       </c>
       <c r="B34" t="s">
         <v>3</v>
       </c>
       <c r="C34" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>164</v>
+        <v>213</v>
       </c>
       <c r="E34" t="s">
         <v>5</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>165</v>
+        <v>214</v>
       </c>
       <c r="G34" s="3" t="s">
-        <v>166</v>
+        <v>215</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
-        <v>41725</v>
+        <v>41743</v>
       </c>
       <c r="B35" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C35" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>159</v>
+        <v>216</v>
       </c>
       <c r="E35" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>160</v>
+        <v>217</v>
       </c>
       <c r="G35" s="3" t="s">
-        <v>163</v>
+        <v>218</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
-        <v>41725</v>
+        <v>41740</v>
       </c>
       <c r="B36" t="s">
-        <v>144</v>
+        <v>185</v>
       </c>
       <c r="C36" t="s">
         <v>0</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>161</v>
+        <v>186</v>
       </c>
       <c r="E36" t="s">
-        <v>146</v>
+        <v>1</v>
       </c>
       <c r="F36" s="3" t="s">
-        <v>6</v>
+        <v>187</v>
       </c>
       <c r="G36" s="3" t="s">
-        <v>162</v>
+        <v>196</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
-        <v>41722</v>
+        <v>41740</v>
       </c>
       <c r="B37" t="s">
-        <v>151</v>
+        <v>42</v>
       </c>
       <c r="C37" t="s">
         <v>0</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>152</v>
+        <v>188</v>
       </c>
       <c r="E37" t="s">
-        <v>1</v>
+        <v>44</v>
       </c>
       <c r="F37" s="3" t="s">
-        <v>153</v>
+        <v>15</v>
       </c>
       <c r="G37" s="3" t="s">
-        <v>158</v>
+        <v>195</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
-        <v>41722</v>
+        <v>41739</v>
       </c>
       <c r="B38" t="s">
-        <v>154</v>
+        <v>189</v>
       </c>
       <c r="C38" t="s">
         <v>0</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>155</v>
+        <v>190</v>
       </c>
       <c r="E38" t="s">
-        <v>156</v>
+        <v>1</v>
       </c>
       <c r="F38" s="3" t="s">
-        <v>6</v>
+        <v>191</v>
       </c>
       <c r="G38" s="3" t="s">
-        <v>157</v>
+        <v>194</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
-        <v>41722</v>
+        <v>41739</v>
       </c>
       <c r="B39" t="s">
-        <v>3</v>
+        <v>42</v>
       </c>
       <c r="C39" t="s">
         <v>0</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>143</v>
+        <v>192</v>
       </c>
       <c r="E39" t="s">
-        <v>5</v>
+        <v>44</v>
       </c>
       <c r="F39" s="3" t="s">
-        <v>9</v>
+        <v>67</v>
       </c>
       <c r="G39" s="3" t="s">
-        <v>150</v>
+        <v>193</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
-        <v>41722</v>
+        <v>41738</v>
       </c>
       <c r="B40" t="s">
-        <v>144</v>
+        <v>3</v>
       </c>
       <c r="C40" t="s">
         <v>0</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>145</v>
+        <v>183</v>
       </c>
       <c r="E40" t="s">
-        <v>146</v>
+        <v>5</v>
       </c>
       <c r="F40" s="3" t="s">
-        <v>27</v>
+        <v>165</v>
       </c>
       <c r="G40" s="3" t="s">
-        <v>149</v>
+        <v>184</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
-        <v>41719</v>
+        <v>41737</v>
       </c>
       <c r="B41" t="s">
-        <v>32</v>
+        <v>3</v>
       </c>
       <c r="C41" t="s">
         <v>4</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>147</v>
+        <v>173</v>
       </c>
       <c r="E41" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="F41" s="3" t="s">
-        <v>6</v>
+        <v>174</v>
       </c>
       <c r="G41" s="3" t="s">
-        <v>148</v>
+        <v>181</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
-        <v>41712</v>
+        <v>41736</v>
       </c>
       <c r="B42" t="s">
-        <v>139</v>
+        <v>175</v>
       </c>
       <c r="C42" t="s">
         <v>0</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>140</v>
+        <v>176</v>
       </c>
       <c r="E42" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F42" s="3" t="s">
-        <v>141</v>
+        <v>174</v>
       </c>
       <c r="G42" s="3" t="s">
-        <v>142</v>
+        <v>182</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
-        <v>41708</v>
+        <v>41736</v>
       </c>
       <c r="B43" t="s">
-        <v>135</v>
+        <v>59</v>
       </c>
       <c r="C43" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>136</v>
+        <v>177</v>
       </c>
       <c r="E43" t="s">
         <v>5</v>
       </c>
       <c r="F43" s="3" t="s">
-        <v>6</v>
+        <v>178</v>
       </c>
       <c r="G43" s="3" t="s">
-        <v>138</v>
+        <v>181</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
-        <v>41705</v>
+        <v>41736</v>
       </c>
       <c r="B44" t="s">
-        <v>59</v>
+        <v>7</v>
       </c>
       <c r="C44" t="s">
         <v>0</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>137</v>
+        <v>179</v>
       </c>
       <c r="E44" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="F44" s="3" t="s">
-        <v>133</v>
+        <v>174</v>
       </c>
       <c r="G44" s="3" t="s">
-        <v>131</v>
+        <v>180</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
-        <v>41703</v>
+        <v>41731</v>
       </c>
       <c r="B45" t="s">
         <v>3</v>
       </c>
       <c r="C45" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>132</v>
+        <v>167</v>
       </c>
       <c r="E45" t="s">
         <v>5</v>
       </c>
       <c r="F45" s="3" t="s">
-        <v>133</v>
+        <v>15</v>
       </c>
       <c r="G45" s="3" t="s">
-        <v>134</v>
+        <v>171</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
-        <v>41703</v>
+        <v>41731</v>
       </c>
       <c r="B46" t="s">
-        <v>117</v>
+        <v>32</v>
       </c>
       <c r="C46" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>118</v>
+        <v>168</v>
       </c>
       <c r="E46" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F46" s="3" t="s">
-        <v>119</v>
+        <v>15</v>
       </c>
       <c r="G46" s="3" t="s">
-        <v>131</v>
+        <v>172</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
-        <v>41703</v>
+        <v>41729</v>
       </c>
       <c r="B47" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="C47" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>120</v>
+        <v>169</v>
       </c>
       <c r="E47" t="s">
-        <v>1</v>
+        <v>19</v>
       </c>
       <c r="F47" s="3" t="s">
-        <v>121</v>
+        <v>170</v>
       </c>
       <c r="G47" s="3" t="s">
-        <v>130</v>
+        <v>171</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
-        <v>41698</v>
+        <v>41729</v>
       </c>
       <c r="B48" t="s">
-        <v>17</v>
+        <v>3</v>
       </c>
       <c r="C48" t="s">
         <v>4</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>122</v>
+        <v>164</v>
       </c>
       <c r="E48" t="s">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="F48" s="3" t="s">
-        <v>123</v>
+        <v>165</v>
       </c>
       <c r="G48" s="3" t="s">
-        <v>129</v>
+        <v>166</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
-        <v>41691</v>
+        <v>41725</v>
       </c>
       <c r="B49" t="s">
-        <v>124</v>
+        <v>3</v>
       </c>
       <c r="C49" t="s">
         <v>4</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>125</v>
+        <v>159</v>
       </c>
       <c r="E49" t="s">
         <v>5</v>
       </c>
       <c r="F49" s="3" t="s">
-        <v>67</v>
+        <v>160</v>
       </c>
       <c r="G49" s="3" t="s">
-        <v>128</v>
+        <v>163</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
-        <v>41691</v>
+        <v>41725</v>
       </c>
       <c r="B50" t="s">
-        <v>124</v>
+        <v>144</v>
       </c>
       <c r="C50" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>126</v>
+        <v>161</v>
       </c>
       <c r="E50" t="s">
-        <v>5</v>
+        <v>146</v>
       </c>
       <c r="F50" s="3" t="s">
-        <v>67</v>
+        <v>6</v>
       </c>
       <c r="G50" s="3" t="s">
-        <v>127</v>
+        <v>162</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
-        <v>41690</v>
+        <v>41722</v>
       </c>
       <c r="B51" t="s">
-        <v>3</v>
+        <v>151</v>
       </c>
       <c r="C51" t="s">
         <v>0</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>113</v>
+        <v>152</v>
       </c>
       <c r="E51" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F51" s="3" t="s">
-        <v>114</v>
+        <v>153</v>
       </c>
       <c r="G51" s="3" t="s">
-        <v>112</v>
+        <v>158</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
-        <v>41690</v>
+        <v>41722</v>
       </c>
       <c r="B52" t="s">
-        <v>3</v>
+        <v>154</v>
       </c>
       <c r="C52" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>115</v>
+        <v>155</v>
       </c>
       <c r="E52" t="s">
-        <v>5</v>
+        <v>156</v>
       </c>
       <c r="F52" s="3" t="s">
-        <v>114</v>
+        <v>6</v>
       </c>
       <c r="G52" s="3" t="s">
-        <v>116</v>
+        <v>157</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
-        <v>41682</v>
+        <v>41722</v>
       </c>
       <c r="B53" t="s">
-        <v>106</v>
+        <v>3</v>
       </c>
       <c r="C53" t="s">
         <v>0</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>107</v>
+        <v>143</v>
       </c>
       <c r="E53" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="F53" s="3" t="s">
-        <v>108</v>
+        <v>9</v>
       </c>
       <c r="G53" s="3" t="s">
-        <v>112</v>
+        <v>150</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
-        <v>41680</v>
+        <v>41722</v>
       </c>
       <c r="B54" t="s">
-        <v>32</v>
+        <v>144</v>
       </c>
       <c r="C54" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>109</v>
+        <v>145</v>
       </c>
       <c r="E54" t="s">
-        <v>10</v>
+        <v>146</v>
       </c>
       <c r="F54" s="3" t="s">
-        <v>110</v>
+        <v>27</v>
       </c>
       <c r="G54" s="3" t="s">
-        <v>111</v>
+        <v>149</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
-        <v>41680</v>
+        <v>41719</v>
       </c>
       <c r="B55" t="s">
-        <v>3</v>
+        <v>32</v>
       </c>
       <c r="C55" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>105</v>
+        <v>147</v>
       </c>
       <c r="E55" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="F55" s="3" t="s">
         <v>6</v>
       </c>
       <c r="G55" s="3" t="s">
-        <v>98</v>
+        <v>148</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
-        <v>41677</v>
+        <v>41712</v>
       </c>
       <c r="B56" t="s">
-        <v>32</v>
+        <v>139</v>
       </c>
       <c r="C56" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>99</v>
+        <v>140</v>
       </c>
       <c r="E56" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="F56" s="3" t="s">
-        <v>6</v>
+        <v>141</v>
       </c>
       <c r="G56" s="3" t="s">
-        <v>104</v>
+        <v>142</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
-        <v>41677</v>
+        <v>41708</v>
       </c>
       <c r="B57" t="s">
-        <v>59</v>
+        <v>135</v>
       </c>
       <c r="C57" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>100</v>
+        <v>136</v>
       </c>
       <c r="E57" t="s">
         <v>5</v>
       </c>
       <c r="F57" s="3" t="s">
-        <v>101</v>
+        <v>6</v>
       </c>
       <c r="G57" s="3" t="s">
-        <v>98</v>
+        <v>138</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
-        <v>41676</v>
+        <v>41705</v>
       </c>
       <c r="B58" t="s">
-        <v>3</v>
+        <v>59</v>
       </c>
       <c r="C58" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>102</v>
+        <v>137</v>
       </c>
       <c r="E58" t="s">
         <v>5</v>
       </c>
       <c r="F58" s="3" t="s">
-        <v>101</v>
+        <v>133</v>
       </c>
       <c r="G58" s="3" t="s">
-        <v>103</v>
+        <v>131</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
-        <v>41674</v>
+        <v>41703</v>
       </c>
       <c r="B59" t="s">
-        <v>95</v>
+        <v>3</v>
       </c>
       <c r="C59" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>96</v>
+        <v>132</v>
       </c>
       <c r="E59" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F59" s="3" t="s">
-        <v>97</v>
+        <v>133</v>
       </c>
       <c r="G59" s="3" t="s">
-        <v>98</v>
+        <v>134</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
-        <v>41670</v>
+        <v>41703</v>
       </c>
       <c r="B60" t="s">
-        <v>17</v>
+        <v>117</v>
       </c>
       <c r="C60" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>18</v>
+        <v>118</v>
       </c>
       <c r="E60" t="s">
-        <v>19</v>
+        <v>1</v>
       </c>
       <c r="F60" s="3" t="s">
-        <v>20</v>
+        <v>119</v>
       </c>
       <c r="G60" s="3" t="s">
-        <v>94</v>
+        <v>131</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
-        <v>41666</v>
+        <v>41703</v>
       </c>
       <c r="B61" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C61" t="s">
         <v>0</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>21</v>
+        <v>120</v>
       </c>
       <c r="E61" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F61" s="3" t="s">
-        <v>71</v>
+        <v>121</v>
       </c>
       <c r="G61" s="3" t="s">
-        <v>93</v>
+        <v>130</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
-        <v>41666</v>
+        <v>41698</v>
       </c>
       <c r="B62" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="C62" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>22</v>
+        <v>122</v>
       </c>
       <c r="E62" t="s">
-        <v>1</v>
+        <v>19</v>
       </c>
       <c r="F62" s="3" t="s">
-        <v>23</v>
+        <v>123</v>
       </c>
       <c r="G62" s="3" t="s">
-        <v>92</v>
+        <v>129</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
-        <v>41666</v>
+        <v>41691</v>
       </c>
       <c r="B63" t="s">
-        <v>24</v>
+        <v>124</v>
       </c>
       <c r="C63" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>25</v>
+        <v>125</v>
       </c>
       <c r="E63" t="s">
-        <v>26</v>
+        <v>5</v>
       </c>
       <c r="F63" s="3" t="s">
-        <v>27</v>
+        <v>67</v>
       </c>
       <c r="G63" s="3" t="s">
-        <v>91</v>
+        <v>128</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
-        <v>41666</v>
+        <v>41691</v>
       </c>
       <c r="B64" t="s">
-        <v>28</v>
+        <v>124</v>
       </c>
       <c r="C64" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>29</v>
+        <v>126</v>
       </c>
       <c r="E64" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F64" s="3" t="s">
-        <v>30</v>
+        <v>67</v>
       </c>
       <c r="G64" s="3" t="s">
-        <v>90</v>
+        <v>127</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
-        <v>41660</v>
+        <v>41690</v>
       </c>
       <c r="B65" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="C65" t="s">
         <v>0</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>31</v>
+        <v>113</v>
       </c>
       <c r="E65" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F65" s="3" t="s">
-        <v>9</v>
+        <v>114</v>
       </c>
       <c r="G65" s="3" t="s">
-        <v>89</v>
+        <v>112</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
-        <v>41660</v>
+        <v>41690</v>
       </c>
       <c r="B66" t="s">
-        <v>32</v>
+        <v>3</v>
       </c>
       <c r="C66" t="s">
         <v>4</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>33</v>
+        <v>115</v>
       </c>
       <c r="E66" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="F66" s="3" t="s">
-        <v>6</v>
+        <v>114</v>
       </c>
       <c r="G66" s="3" t="s">
-        <v>88</v>
+        <v>116</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
-        <v>41660</v>
+        <v>41682</v>
       </c>
       <c r="B67" t="s">
-        <v>34</v>
+        <v>106</v>
       </c>
       <c r="C67" t="s">
         <v>0</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>35</v>
+        <v>107</v>
       </c>
       <c r="E67" t="s">
         <v>12</v>
       </c>
       <c r="F67" s="3" t="s">
-        <v>36</v>
+        <v>108</v>
       </c>
       <c r="G67" s="3" t="s">
-        <v>87</v>
+        <v>112</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
-        <v>41659</v>
+        <v>41680</v>
       </c>
       <c r="B68" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="C68" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>38</v>
+        <v>109</v>
       </c>
       <c r="E68" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F68" s="3" t="s">
-        <v>39</v>
+        <v>110</v>
       </c>
       <c r="G68" s="3" t="s">
-        <v>86</v>
+        <v>111</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
-        <v>41655</v>
+        <v>41680</v>
       </c>
       <c r="B69" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C69" t="s">
         <v>0</v>
       </c>
       <c r="D69" s="2" t="s">
-        <v>40</v>
+        <v>105</v>
       </c>
       <c r="E69" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F69" s="3" t="s">
-        <v>41</v>
+        <v>6</v>
       </c>
       <c r="G69" s="3" t="s">
-        <v>85</v>
+        <v>98</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
-        <v>41655</v>
+        <v>41677</v>
       </c>
       <c r="B70" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="C70" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D70" s="2" t="s">
-        <v>43</v>
+        <v>99</v>
       </c>
       <c r="E70" t="s">
-        <v>44</v>
+        <v>10</v>
       </c>
       <c r="F70" s="3" t="s">
         <v>6</v>
       </c>
       <c r="G70" s="3" t="s">
-        <v>84</v>
+        <v>104</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
-        <v>41652</v>
+        <v>41677</v>
       </c>
       <c r="B71" t="s">
-        <v>3</v>
+        <v>59</v>
       </c>
       <c r="C71" t="s">
         <v>0</v>
       </c>
       <c r="D71" s="2" t="s">
-        <v>45</v>
+        <v>100</v>
       </c>
       <c r="E71" t="s">
         <v>5</v>
       </c>
       <c r="F71" s="3" t="s">
-        <v>46</v>
+        <v>101</v>
       </c>
       <c r="G71" s="3" t="s">
-        <v>83</v>
+        <v>98</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
-        <v>41649</v>
+        <v>41676</v>
       </c>
       <c r="B72" t="s">
         <v>3</v>
       </c>
       <c r="C72" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D72" s="2" t="s">
-        <v>16</v>
+        <v>102</v>
       </c>
       <c r="E72" t="s">
         <v>5</v>
       </c>
       <c r="F72" s="3" t="s">
-        <v>15</v>
+        <v>101</v>
       </c>
       <c r="G72" s="3" t="s">
-        <v>82</v>
+        <v>103</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
-        <v>41648</v>
+        <v>41674</v>
       </c>
       <c r="B73" t="s">
-        <v>2</v>
+        <v>95</v>
       </c>
       <c r="C73" t="s">
         <v>0</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>47</v>
+        <v>96</v>
       </c>
       <c r="E73" t="s">
         <v>1</v>
       </c>
       <c r="F73" s="3" t="s">
-        <v>48</v>
+        <v>97</v>
       </c>
       <c r="G73" s="3" t="s">
-        <v>81</v>
+        <v>98</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
-        <v>41648</v>
+        <v>41670</v>
       </c>
       <c r="B74" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="C74" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D74" s="2" t="s">
-        <v>49</v>
+        <v>18</v>
       </c>
       <c r="E74" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="F74" s="3" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="G74" s="3" t="s">
-        <v>80</v>
+        <v>94</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
-        <v>41647</v>
+        <v>41666</v>
       </c>
       <c r="B75" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C75" t="s">
         <v>0</v>
       </c>
       <c r="D75" s="2" t="s">
-        <v>50</v>
+        <v>21</v>
       </c>
       <c r="E75" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F75" s="3" t="s">
-        <v>51</v>
+        <v>71</v>
       </c>
       <c r="G75" s="3" t="s">
-        <v>79</v>
+        <v>93</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
-        <v>41646</v>
+        <v>41666</v>
       </c>
       <c r="B76" t="s">
-        <v>52</v>
+        <v>2</v>
       </c>
       <c r="C76" t="s">
         <v>0</v>
       </c>
       <c r="D76" s="2" t="s">
-        <v>53</v>
+        <v>22</v>
       </c>
       <c r="E76" t="s">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="F76" s="3" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="G76" s="3" t="s">
-        <v>78</v>
+        <v>92</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
-        <v>41646</v>
+        <v>41666</v>
       </c>
       <c r="B77" t="s">
-        <v>54</v>
+        <v>24</v>
       </c>
       <c r="C77" t="s">
         <v>0</v>
       </c>
       <c r="D77" s="2" t="s">
-        <v>55</v>
+        <v>25</v>
       </c>
       <c r="E77" t="s">
-        <v>12</v>
+        <v>26</v>
       </c>
       <c r="F77" s="3" t="s">
-        <v>14</v>
+        <v>27</v>
       </c>
       <c r="G77" s="3" t="s">
-        <v>77</v>
+        <v>91</v>
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
-        <v>41646</v>
+        <v>41666</v>
       </c>
       <c r="B78" t="s">
-        <v>56</v>
+        <v>28</v>
       </c>
       <c r="C78" t="s">
         <v>0</v>
       </c>
       <c r="D78" s="2" t="s">
-        <v>57</v>
+        <v>29</v>
       </c>
       <c r="E78" t="s">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="F78" s="3" t="s">
-        <v>58</v>
+        <v>30</v>
       </c>
       <c r="G78" s="3" t="s">
-        <v>76</v>
+        <v>90</v>
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
-        <v>41646</v>
+        <v>41660</v>
       </c>
       <c r="B79" t="s">
-        <v>59</v>
+        <v>11</v>
       </c>
       <c r="C79" t="s">
         <v>0</v>
       </c>
       <c r="D79" s="2" t="s">
-        <v>60</v>
+        <v>31</v>
       </c>
       <c r="E79" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="F79" s="3" t="s">
-        <v>61</v>
+        <v>9</v>
       </c>
       <c r="G79" s="3" t="s">
-        <v>75</v>
+        <v>89</v>
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
-        <v>41645</v>
+        <v>41660</v>
       </c>
       <c r="B80" t="s">
-        <v>62</v>
+        <v>32</v>
       </c>
       <c r="C80" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D80" s="2" t="s">
-        <v>63</v>
+        <v>33</v>
       </c>
       <c r="E80" t="s">
-        <v>64</v>
+        <v>10</v>
       </c>
       <c r="F80" s="3" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="G80" s="3" t="s">
-        <v>74</v>
+        <v>88</v>
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81" s="1">
-        <v>41642</v>
+        <v>41660</v>
       </c>
       <c r="B81" t="s">
-        <v>65</v>
+        <v>34</v>
       </c>
       <c r="C81" t="s">
         <v>0</v>
       </c>
       <c r="D81" s="2" t="s">
-        <v>66</v>
+        <v>35</v>
       </c>
       <c r="E81" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F81" s="3" t="s">
-        <v>67</v>
+        <v>36</v>
       </c>
       <c r="G81" s="3" t="s">
-        <v>73</v>
+        <v>87</v>
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82" s="1">
-        <v>41641</v>
+        <v>41659</v>
       </c>
       <c r="B82" t="s">
-        <v>68</v>
+        <v>37</v>
       </c>
       <c r="C82" t="s">
         <v>0</v>
       </c>
       <c r="D82" s="2" t="s">
-        <v>69</v>
+        <v>38</v>
       </c>
       <c r="E82" t="s">
         <v>1</v>
       </c>
       <c r="F82" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="G82" s="3" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A83" s="1">
+        <v>41655</v>
+      </c>
+      <c r="B83" t="s">
+        <v>2</v>
+      </c>
+      <c r="C83" t="s">
+        <v>0</v>
+      </c>
+      <c r="D83" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E83" t="s">
+        <v>1</v>
+      </c>
+      <c r="F83" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="G83" s="3" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A84" s="1">
+        <v>41655</v>
+      </c>
+      <c r="B84" t="s">
+        <v>42</v>
+      </c>
+      <c r="C84" t="s">
+        <v>0</v>
+      </c>
+      <c r="D84" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E84" t="s">
+        <v>44</v>
+      </c>
+      <c r="F84" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G84" s="3" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A85" s="1">
+        <v>41652</v>
+      </c>
+      <c r="B85" t="s">
+        <v>3</v>
+      </c>
+      <c r="C85" t="s">
+        <v>0</v>
+      </c>
+      <c r="D85" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="E85" t="s">
+        <v>5</v>
+      </c>
+      <c r="F85" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="G85" s="3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A86" s="1">
+        <v>41649</v>
+      </c>
+      <c r="B86" t="s">
+        <v>3</v>
+      </c>
+      <c r="C86" t="s">
+        <v>0</v>
+      </c>
+      <c r="D86" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E86" t="s">
+        <v>5</v>
+      </c>
+      <c r="F86" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G86" s="3" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A87" s="1">
+        <v>41648</v>
+      </c>
+      <c r="B87" t="s">
+        <v>2</v>
+      </c>
+      <c r="C87" t="s">
+        <v>0</v>
+      </c>
+      <c r="D87" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E87" t="s">
+        <v>1</v>
+      </c>
+      <c r="F87" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="G87" s="3" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A88" s="1">
+        <v>41648</v>
+      </c>
+      <c r="B88" t="s">
+        <v>7</v>
+      </c>
+      <c r="C88" t="s">
+        <v>0</v>
+      </c>
+      <c r="D88" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E88" t="s">
+        <v>8</v>
+      </c>
+      <c r="F88" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G88" s="3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A89" s="1">
+        <v>41647</v>
+      </c>
+      <c r="B89" t="s">
+        <v>2</v>
+      </c>
+      <c r="C89" t="s">
+        <v>0</v>
+      </c>
+      <c r="D89" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E89" t="s">
+        <v>1</v>
+      </c>
+      <c r="F89" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="G89" s="3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A90" s="1">
+        <v>41646</v>
+      </c>
+      <c r="B90" t="s">
+        <v>52</v>
+      </c>
+      <c r="C90" t="s">
+        <v>0</v>
+      </c>
+      <c r="D90" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E90" t="s">
+        <v>12</v>
+      </c>
+      <c r="F90" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G90" s="3" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A91" s="1">
+        <v>41646</v>
+      </c>
+      <c r="B91" t="s">
+        <v>54</v>
+      </c>
+      <c r="C91" t="s">
+        <v>0</v>
+      </c>
+      <c r="D91" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="E91" t="s">
+        <v>12</v>
+      </c>
+      <c r="F91" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G91" s="3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A92" s="1">
+        <v>41646</v>
+      </c>
+      <c r="B92" t="s">
+        <v>56</v>
+      </c>
+      <c r="C92" t="s">
+        <v>0</v>
+      </c>
+      <c r="D92" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="E92" t="s">
+        <v>12</v>
+      </c>
+      <c r="F92" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="G92" s="3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A93" s="1">
+        <v>41646</v>
+      </c>
+      <c r="B93" t="s">
+        <v>59</v>
+      </c>
+      <c r="C93" t="s">
+        <v>0</v>
+      </c>
+      <c r="D93" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="E93" t="s">
+        <v>5</v>
+      </c>
+      <c r="F93" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="G93" s="3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A94" s="1">
+        <v>41645</v>
+      </c>
+      <c r="B94" t="s">
+        <v>62</v>
+      </c>
+      <c r="C94" t="s">
+        <v>0</v>
+      </c>
+      <c r="D94" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="E94" t="s">
+        <v>64</v>
+      </c>
+      <c r="F94" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G94" s="3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A95" s="1">
+        <v>41642</v>
+      </c>
+      <c r="B95" t="s">
+        <v>65</v>
+      </c>
+      <c r="C95" t="s">
+        <v>0</v>
+      </c>
+      <c r="D95" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="E95" t="s">
+        <v>10</v>
+      </c>
+      <c r="F95" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="G95" s="3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A96" s="1">
+        <v>41641</v>
+      </c>
+      <c r="B96" t="s">
+        <v>68</v>
+      </c>
+      <c r="C96" t="s">
+        <v>0</v>
+      </c>
+      <c r="D96" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="E96" t="s">
+        <v>1</v>
+      </c>
+      <c r="F96" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="G82" s="3" t="s">
+      <c r="G96" s="3" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A83" s="1"/>
-    </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A84" s="1"/>
-    </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A85" s="1"/>
-    </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A86" s="1"/>
-    </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A87" s="1"/>
+    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A97" s="1"/>
+    </row>
+    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A98" s="1"/>
+      <c r="D98"/>
+      <c r="F98"/>
+      <c r="G98"/>
+    </row>
+    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A99" s="1"/>
+      <c r="D99"/>
+      <c r="F99"/>
+      <c r="G99"/>
+    </row>
+    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A100" s="1"/>
+      <c r="D100"/>
+      <c r="F100"/>
+      <c r="G100"/>
+    </row>
+    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A101" s="1"/>
+      <c r="D101"/>
+      <c r="F101"/>
+      <c r="G101"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Actualizando DataFixtures y numero de filas x paginas
</commit_message>
<xml_diff>
--- a/backup/cuenta_2200555126.xlsx
+++ b/backup/cuenta_2200555126.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="576" uniqueCount="300">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="606" uniqueCount="316">
   <si>
     <t>D</t>
   </si>
@@ -924,6 +924,54 @@
   </si>
   <si>
     <t>129.83</t>
+  </si>
+  <si>
+    <t>0000616755</t>
+  </si>
+  <si>
+    <t>62.39</t>
+  </si>
+  <si>
+    <t>CONSUMO VISA NA SANDRY</t>
+  </si>
+  <si>
+    <t>0005149037</t>
+  </si>
+  <si>
+    <t>8.45  </t>
+  </si>
+  <si>
+    <t>82.39</t>
+  </si>
+  <si>
+    <t>RETIRO ATM BP N/GIRON 1</t>
+  </si>
+  <si>
+    <t>0000956117</t>
+  </si>
+  <si>
+    <t>90.84</t>
+  </si>
+  <si>
+    <t>0013346747</t>
+  </si>
+  <si>
+    <t>7.57  </t>
+  </si>
+  <si>
+    <t>110.84</t>
+  </si>
+  <si>
+    <t>CONSUMO VISA NA MENESTRAS DEL NEGRO M0</t>
+  </si>
+  <si>
+    <t>0009362885</t>
+  </si>
+  <si>
+    <t>11.42  </t>
+  </si>
+  <si>
+    <t>118.41</t>
   </si>
 </sst>
 </file>
@@ -1246,10 +1294,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H101"/>
+  <dimension ref="A1:H106"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+      <selection activeCell="H1" sqref="H1:H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1261,172 +1309,188 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1">
-        <v>41785</v>
+        <v>41788</v>
       </c>
       <c r="B1" t="s">
-        <v>3</v>
+        <v>197</v>
       </c>
       <c r="C1" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>297</v>
+        <v>300</v>
       </c>
       <c r="E1" t="s">
-        <v>5</v>
+        <v>156</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>298</v>
+        <v>9</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>299</v>
+        <v>301</v>
       </c>
       <c r="H1" t="str">
-        <f t="shared" ref="H1:H14" ca="1" si="0">CONCATENATE("array('mo_fecha' =&gt; new \DateTime('",TEXT(A1,"yyyy-mm-dd"),"'), 'mo_concepto' =&gt; '",B1,"', 'mo_tipo' =&gt; '",C1,"', 'mo_documento' =&gt; '",D1,"', 'mo_oficina' =&gt; '",E1,"', 'mo_monto' =&gt; ",F1,", 'mo_saldo' =&gt; ",G1,", 'mo_fecha_crea' =&gt; new \DateTime('",TEXT(NOW(),"yyyy-mm-dd H:m:s"),"'), 'mo_quien_crea' =&gt; 1, 'mo_fecha_modifica' =&gt; NULL, 'mo_quien_modifica' =&gt; NULL, 'mo_fecha_borrado' =&gt; NULL, 'mo_quien_borra' =&gt; NULL, 'mo_borrado_logico' =&gt; false),")</f>
-        <v>array('mo_fecha' =&gt; new \DateTime('2014-05-26'), 'mo_concepto' =&gt; '  TRANSFERENCIA INTERNET', 'mo_tipo' =&gt; 'C', 'mo_documento' =&gt; '0002663087', 'mo_oficina' =&gt; 'AG. NORTE', 'mo_monto' =&gt; 29.83  , 'mo_saldo' =&gt; 129.83, 'mo_fecha_crea' =&gt; new \DateTime('2014-05-24 20:44:24'), 'mo_quien_crea' =&gt; 1, 'mo_fecha_modifica' =&gt; NULL, 'mo_quien_modifica' =&gt; NULL, 'mo_fecha_borrado' =&gt; NULL, 'mo_quien_borra' =&gt; NULL, 'mo_borrado_logico' =&gt; false),</v>
+        <f t="shared" ref="H1:H5" ca="1" si="0">CONCATENATE("array('mo_fecha' =&gt; new \DateTime('",TEXT(A1,"yyyy-mm-dd"),"'), 'mo_concepto' =&gt; '",B1,"', 'mo_tipo' =&gt; '",C1,"', 'mo_documento' =&gt; '",D1,"', 'mo_oficina' =&gt; '",E1,"', 'mo_monto' =&gt; ",F1,", 'mo_saldo' =&gt; ",G1,", 'mo_fecha_crea' =&gt; new \DateTime('",TEXT(NOW(),"yyyy-mm-dd H:m:s"),"'), 'mo_quien_crea' =&gt; 1, 'mo_fecha_modifica' =&gt; NULL, 'mo_quien_modifica' =&gt; NULL, 'mo_fecha_borrado' =&gt; NULL, 'mo_quien_borra' =&gt; NULL, 'mo_borrado_logico' =&gt; false),")</f>
+        <v>array('mo_fecha' =&gt; new \DateTime('2014-05-29'), 'mo_concepto' =&gt; 'RETIRO ATM BP D/REINA VICTORIA', 'mo_tipo' =&gt; 'D', 'mo_documento' =&gt; '0000616755', 'mo_oficina' =&gt; 'CENTRO DE ACOPIO NORTE', 'mo_monto' =&gt; 20.00  , 'mo_saldo' =&gt; 62.39, 'mo_fecha_crea' =&gt; new \DateTime('2014-05-30 10:47:22'), 'mo_quien_crea' =&gt; 1, 'mo_fecha_modifica' =&gt; NULL, 'mo_quien_modifica' =&gt; NULL, 'mo_fecha_borrado' =&gt; NULL, 'mo_quien_borra' =&gt; NULL, 'mo_borrado_logico' =&gt; false),</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>41781</v>
+        <v>41787</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>302</v>
       </c>
       <c r="C2" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>260</v>
+        <v>303</v>
       </c>
       <c r="E2" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>6</v>
+        <v>304</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>261</v>
+        <v>305</v>
+      </c>
+      <c r="H2" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>array('mo_fecha' =&gt; new \DateTime('2014-05-28'), 'mo_concepto' =&gt; 'CONSUMO VISA NA SANDRY', 'mo_tipo' =&gt; 'D', 'mo_documento' =&gt; '0005149037', 'mo_oficina' =&gt; 'INSTITUCIONAL SS.CC.', 'mo_monto' =&gt; 8.45  , 'mo_saldo' =&gt; 82.39, 'mo_fecha_crea' =&gt; new \DateTime('2014-05-30 10:47:22'), 'mo_quien_crea' =&gt; 1, 'mo_fecha_modifica' =&gt; NULL, 'mo_quien_modifica' =&gt; NULL, 'mo_fecha_borrado' =&gt; NULL, 'mo_quien_borra' =&gt; NULL, 'mo_borrado_logico' =&gt; false),</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>41779</v>
+        <v>41786</v>
       </c>
       <c r="B3" t="s">
-        <v>3</v>
+        <v>306</v>
       </c>
       <c r="C3" t="s">
         <v>0</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>262</v>
+        <v>307</v>
       </c>
       <c r="E3" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>263</v>
+        <v>9</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>264</v>
+        <v>308</v>
+      </c>
+      <c r="H3" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>array('mo_fecha' =&gt; new \DateTime('2014-05-27'), 'mo_concepto' =&gt; 'RETIRO ATM BP N/GIRON 1', 'mo_tipo' =&gt; 'D', 'mo_documento' =&gt; '0000956117', 'mo_oficina' =&gt; 'EL GIRON', 'mo_monto' =&gt; 20.00  , 'mo_saldo' =&gt; 90.84, 'mo_fecha_crea' =&gt; new \DateTime('2014-05-30 10:47:22'), 'mo_quien_crea' =&gt; 1, 'mo_fecha_modifica' =&gt; NULL, 'mo_quien_modifica' =&gt; NULL, 'mo_fecha_borrado' =&gt; NULL, 'mo_quien_borra' =&gt; NULL, 'mo_borrado_logico' =&gt; false),</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
-        <v>41767</v>
+        <v>41785</v>
       </c>
       <c r="B4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>265</v>
+        <v>309</v>
       </c>
       <c r="E4" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>266</v>
+        <v>310</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>267</v>
+        <v>311</v>
+      </c>
+      <c r="H4" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>array('mo_fecha' =&gt; new \DateTime('2014-05-26'), 'mo_concepto' =&gt; 'CONSUMO DATA AKI MOLINEROS 161', 'mo_tipo' =&gt; 'D', 'mo_documento' =&gt; '0013346747', 'mo_oficina' =&gt; 'INSTITUCIONAL SS.CC.', 'mo_monto' =&gt; 7.57  , 'mo_saldo' =&gt; 110.84, 'mo_fecha_crea' =&gt; new \DateTime('2014-05-30 10:47:22'), 'mo_quien_crea' =&gt; 1, 'mo_fecha_modifica' =&gt; NULL, 'mo_quien_modifica' =&gt; NULL, 'mo_fecha_borrado' =&gt; NULL, 'mo_quien_borra' =&gt; NULL, 'mo_borrado_logico' =&gt; false),</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
-        <v>41766</v>
+        <v>41785</v>
       </c>
       <c r="B5" t="s">
-        <v>59</v>
+        <v>312</v>
       </c>
       <c r="C5" t="s">
         <v>0</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>268</v>
+        <v>313</v>
       </c>
       <c r="E5" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>269</v>
+        <v>314</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>270</v>
+        <v>315</v>
+      </c>
+      <c r="H5" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>array('mo_fecha' =&gt; new \DateTime('2014-05-26'), 'mo_concepto' =&gt; 'CONSUMO VISA NA MENESTRAS DEL NEGRO M0', 'mo_tipo' =&gt; 'D', 'mo_documento' =&gt; '0009362885', 'mo_oficina' =&gt; 'INSTITUCIONAL SS.CC.', 'mo_monto' =&gt; 11.42  , 'mo_saldo' =&gt; 118.41, 'mo_fecha_crea' =&gt; new \DateTime('2014-05-30 10:47:22'), 'mo_quien_crea' =&gt; 1, 'mo_fecha_modifica' =&gt; NULL, 'mo_quien_modifica' =&gt; NULL, 'mo_fecha_borrado' =&gt; NULL, 'mo_quien_borra' =&gt; NULL, 'mo_borrado_logico' =&gt; false),</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
-        <v>41765</v>
+        <v>41785</v>
       </c>
       <c r="B6" t="s">
-        <v>271</v>
+        <v>3</v>
       </c>
       <c r="C6" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>272</v>
+        <v>297</v>
       </c>
       <c r="E6" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>273</v>
+        <v>298</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>274</v>
+        <v>299</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
-        <v>41765</v>
+        <v>41781</v>
       </c>
       <c r="B7" t="s">
         <v>3</v>
       </c>
       <c r="C7" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>275</v>
+        <v>260</v>
       </c>
       <c r="E7" t="s">
         <v>5</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>276</v>
+        <v>6</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>277</v>
+        <v>261</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
-        <v>41765</v>
+        <v>41779</v>
       </c>
       <c r="B8" t="s">
         <v>3</v>
@@ -1435,90 +1499,90 @@
         <v>0</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>278</v>
+        <v>262</v>
       </c>
       <c r="E8" t="s">
         <v>5</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>279</v>
+        <v>263</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>280</v>
+        <v>264</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
-        <v>41764</v>
+        <v>41767</v>
       </c>
       <c r="B9" t="s">
-        <v>281</v>
+        <v>3</v>
       </c>
       <c r="C9" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>282</v>
+        <v>265</v>
       </c>
       <c r="E9" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>283</v>
+        <v>266</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>284</v>
+        <v>267</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
-        <v>41761</v>
+        <v>41766</v>
       </c>
       <c r="B10" t="s">
-        <v>3</v>
+        <v>59</v>
       </c>
       <c r="C10" t="s">
         <v>0</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>285</v>
+        <v>268</v>
       </c>
       <c r="E10" t="s">
         <v>5</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>286</v>
+        <v>269</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>287</v>
+        <v>270</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
-        <v>41761</v>
+        <v>41765</v>
       </c>
       <c r="B11" t="s">
-        <v>3</v>
+        <v>271</v>
       </c>
       <c r="C11" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>288</v>
+        <v>272</v>
       </c>
       <c r="E11" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>289</v>
+        <v>273</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>290</v>
+        <v>274</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
-        <v>41761</v>
+        <v>41765</v>
       </c>
       <c r="B12" t="s">
         <v>3</v>
@@ -1527,21 +1591,21 @@
         <v>0</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>291</v>
+        <v>275</v>
       </c>
       <c r="E12" t="s">
         <v>5</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>289</v>
+        <v>276</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>292</v>
+        <v>277</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
-        <v>41761</v>
+        <v>41765</v>
       </c>
       <c r="B13" t="s">
         <v>3</v>
@@ -1550,527 +1614,527 @@
         <v>0</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>293</v>
+        <v>278</v>
       </c>
       <c r="E13" t="s">
         <v>5</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>294</v>
+        <v>279</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>290</v>
+        <v>280</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
-        <v>41761</v>
+        <v>41764</v>
       </c>
       <c r="B14" t="s">
-        <v>3</v>
+        <v>281</v>
       </c>
       <c r="C14" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>295</v>
+        <v>282</v>
       </c>
       <c r="E14" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>67</v>
+        <v>283</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>296</v>
+        <v>284</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
-        <v>41759</v>
+        <v>41761</v>
       </c>
       <c r="B15" t="s">
-        <v>17</v>
+        <v>3</v>
       </c>
       <c r="C15" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>254</v>
+        <v>285</v>
       </c>
       <c r="E15" t="s">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>255</v>
+        <v>286</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>256</v>
+        <v>287</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
-        <v>41758</v>
+        <v>41761</v>
       </c>
       <c r="B16" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C16" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>257</v>
+        <v>288</v>
       </c>
       <c r="E16" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>258</v>
+        <v>289</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>259</v>
+        <v>290</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
-        <v>41757</v>
+        <v>41761</v>
       </c>
       <c r="B17" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C17" t="s">
         <v>0</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>232</v>
+        <v>291</v>
       </c>
       <c r="E17" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>233</v>
+        <v>289</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>234</v>
+        <v>292</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
-        <v>41757</v>
+        <v>41761</v>
       </c>
       <c r="B18" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C18" t="s">
         <v>0</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>235</v>
+        <v>293</v>
       </c>
       <c r="E18" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>236</v>
+        <v>294</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>237</v>
+        <v>290</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
-        <v>41757</v>
+        <v>41761</v>
       </c>
       <c r="B19" t="s">
-        <v>238</v>
+        <v>3</v>
       </c>
       <c r="C19" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>239</v>
+        <v>295</v>
       </c>
       <c r="E19" t="s">
-        <v>146</v>
+        <v>5</v>
       </c>
       <c r="F19" s="3" t="s">
         <v>67</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>240</v>
+        <v>296</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
-        <v>41754</v>
+        <v>41759</v>
       </c>
       <c r="B20" t="s">
-        <v>241</v>
+        <v>17</v>
       </c>
       <c r="C20" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>242</v>
+        <v>254</v>
       </c>
       <c r="E20" t="s">
-        <v>1</v>
+        <v>19</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>243</v>
+        <v>255</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>244</v>
+        <v>256</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
-        <v>41754</v>
+        <v>41758</v>
       </c>
       <c r="B21" t="s">
-        <v>245</v>
+        <v>2</v>
       </c>
       <c r="C21" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>246</v>
+        <v>257</v>
       </c>
       <c r="E21" t="s">
         <v>1</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>247</v>
+        <v>258</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>253</v>
+        <v>259</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
-        <v>41754</v>
+        <v>41757</v>
       </c>
       <c r="B22" t="s">
-        <v>248</v>
+        <v>2</v>
       </c>
       <c r="C22" t="s">
         <v>0</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>249</v>
+        <v>232</v>
       </c>
       <c r="E22" t="s">
         <v>1</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>247</v>
+        <v>233</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>250</v>
+        <v>234</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
-        <v>41754</v>
+        <v>41757</v>
       </c>
       <c r="B23" t="s">
-        <v>32</v>
+        <v>2</v>
       </c>
       <c r="C23" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>251</v>
+        <v>235</v>
       </c>
       <c r="E23" t="s">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>252</v>
+        <v>236</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>253</v>
+        <v>237</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
-        <v>41752</v>
+        <v>41757</v>
       </c>
       <c r="B24" t="s">
-        <v>223</v>
+        <v>238</v>
       </c>
       <c r="C24" t="s">
         <v>0</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>224</v>
+        <v>239</v>
       </c>
       <c r="E24" t="s">
-        <v>156</v>
+        <v>146</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>225</v>
+        <v>67</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>226</v>
+        <v>240</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
-        <v>41751</v>
+        <v>41754</v>
       </c>
       <c r="B25" t="s">
-        <v>2</v>
+        <v>241</v>
       </c>
       <c r="C25" t="s">
         <v>0</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>227</v>
+        <v>242</v>
       </c>
       <c r="E25" t="s">
         <v>1</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>228</v>
+        <v>243</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>229</v>
+        <v>244</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
-        <v>41751</v>
+        <v>41754</v>
       </c>
       <c r="B26" t="s">
-        <v>144</v>
+        <v>245</v>
       </c>
       <c r="C26" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>230</v>
+        <v>246</v>
       </c>
       <c r="E26" t="s">
-        <v>146</v>
+        <v>1</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>6</v>
+        <v>247</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>231</v>
+        <v>253</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
-        <v>41750</v>
+        <v>41754</v>
       </c>
       <c r="B27" t="s">
-        <v>219</v>
+        <v>248</v>
       </c>
       <c r="C27" t="s">
         <v>0</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>220</v>
+        <v>249</v>
       </c>
       <c r="E27" t="s">
         <v>1</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>221</v>
+        <v>247</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>222</v>
+        <v>250</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
-        <v>41746</v>
+        <v>41754</v>
       </c>
       <c r="B28" t="s">
-        <v>197</v>
+        <v>32</v>
       </c>
       <c r="C28" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>198</v>
+        <v>251</v>
       </c>
       <c r="E28" t="s">
-        <v>156</v>
+        <v>10</v>
       </c>
       <c r="F28" s="3" t="s">
-        <v>9</v>
+        <v>252</v>
       </c>
       <c r="G28" s="3" t="s">
-        <v>199</v>
+        <v>253</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
-        <v>41744</v>
+        <v>41752</v>
       </c>
       <c r="B29" t="s">
-        <v>135</v>
+        <v>223</v>
       </c>
       <c r="C29" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>200</v>
+        <v>224</v>
       </c>
       <c r="E29" t="s">
-        <v>5</v>
+        <v>156</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>67</v>
+        <v>225</v>
       </c>
       <c r="G29" s="3" t="s">
-        <v>201</v>
+        <v>226</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
-        <v>41744</v>
+        <v>41751</v>
       </c>
       <c r="B30" t="s">
-        <v>189</v>
+        <v>2</v>
       </c>
       <c r="C30" t="s">
         <v>0</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>202</v>
+        <v>227</v>
       </c>
       <c r="E30" t="s">
         <v>1</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>203</v>
+        <v>228</v>
       </c>
       <c r="G30" s="3" t="s">
-        <v>204</v>
+        <v>229</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
-        <v>41744</v>
+        <v>41751</v>
       </c>
       <c r="B31" t="s">
-        <v>185</v>
+        <v>144</v>
       </c>
       <c r="C31" t="s">
         <v>0</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>205</v>
+        <v>230</v>
       </c>
       <c r="E31" t="s">
-        <v>1</v>
+        <v>146</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>206</v>
+        <v>6</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>207</v>
+        <v>231</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
-        <v>41744</v>
+        <v>41750</v>
       </c>
       <c r="B32" t="s">
-        <v>185</v>
+        <v>219</v>
       </c>
       <c r="C32" t="s">
         <v>0</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>208</v>
+        <v>220</v>
       </c>
       <c r="E32" t="s">
         <v>1</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>209</v>
+        <v>221</v>
       </c>
       <c r="G32" s="3" t="s">
-        <v>210</v>
+        <v>222</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
-        <v>41743</v>
+        <v>41746</v>
       </c>
       <c r="B33" t="s">
-        <v>3</v>
+        <v>197</v>
       </c>
       <c r="C33" t="s">
         <v>0</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>211</v>
+        <v>198</v>
       </c>
       <c r="E33" t="s">
-        <v>5</v>
+        <v>156</v>
       </c>
       <c r="F33" s="3" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="G33" s="3" t="s">
-        <v>212</v>
+        <v>199</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
-        <v>41743</v>
+        <v>41744</v>
       </c>
       <c r="B34" t="s">
-        <v>3</v>
+        <v>135</v>
       </c>
       <c r="C34" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>213</v>
+        <v>200</v>
       </c>
       <c r="E34" t="s">
         <v>5</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>214</v>
+        <v>67</v>
       </c>
       <c r="G34" s="3" t="s">
-        <v>215</v>
+        <v>201</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
-        <v>41743</v>
+        <v>41744</v>
       </c>
       <c r="B35" t="s">
-        <v>2</v>
+        <v>189</v>
       </c>
       <c r="C35" t="s">
         <v>0</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>216</v>
+        <v>202</v>
       </c>
       <c r="E35" t="s">
         <v>1</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>217</v>
+        <v>203</v>
       </c>
       <c r="G35" s="3" t="s">
-        <v>218</v>
+        <v>204</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
-        <v>41740</v>
+        <v>41744</v>
       </c>
       <c r="B36" t="s">
         <v>185</v>
@@ -2079,205 +2143,205 @@
         <v>0</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>186</v>
+        <v>205</v>
       </c>
       <c r="E36" t="s">
         <v>1</v>
       </c>
       <c r="F36" s="3" t="s">
-        <v>187</v>
+        <v>206</v>
       </c>
       <c r="G36" s="3" t="s">
-        <v>196</v>
+        <v>207</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
-        <v>41740</v>
+        <v>41744</v>
       </c>
       <c r="B37" t="s">
-        <v>42</v>
+        <v>185</v>
       </c>
       <c r="C37" t="s">
         <v>0</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>188</v>
+        <v>208</v>
       </c>
       <c r="E37" t="s">
-        <v>44</v>
+        <v>1</v>
       </c>
       <c r="F37" s="3" t="s">
-        <v>15</v>
+        <v>209</v>
       </c>
       <c r="G37" s="3" t="s">
-        <v>195</v>
+        <v>210</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
-        <v>41739</v>
+        <v>41743</v>
       </c>
       <c r="B38" t="s">
-        <v>189</v>
+        <v>3</v>
       </c>
       <c r="C38" t="s">
         <v>0</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>190</v>
+        <v>211</v>
       </c>
       <c r="E38" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F38" s="3" t="s">
-        <v>191</v>
+        <v>6</v>
       </c>
       <c r="G38" s="3" t="s">
-        <v>194</v>
+        <v>212</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
-        <v>41739</v>
+        <v>41743</v>
       </c>
       <c r="B39" t="s">
-        <v>42</v>
+        <v>3</v>
       </c>
       <c r="C39" t="s">
         <v>0</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>192</v>
+        <v>213</v>
       </c>
       <c r="E39" t="s">
-        <v>44</v>
+        <v>5</v>
       </c>
       <c r="F39" s="3" t="s">
-        <v>67</v>
+        <v>214</v>
       </c>
       <c r="G39" s="3" t="s">
-        <v>193</v>
+        <v>215</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
-        <v>41738</v>
+        <v>41743</v>
       </c>
       <c r="B40" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C40" t="s">
         <v>0</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>183</v>
+        <v>216</v>
       </c>
       <c r="E40" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F40" s="3" t="s">
-        <v>165</v>
+        <v>217</v>
       </c>
       <c r="G40" s="3" t="s">
-        <v>184</v>
+        <v>218</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
-        <v>41737</v>
+        <v>41740</v>
       </c>
       <c r="B41" t="s">
-        <v>3</v>
+        <v>185</v>
       </c>
       <c r="C41" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>173</v>
+        <v>186</v>
       </c>
       <c r="E41" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F41" s="3" t="s">
-        <v>174</v>
+        <v>187</v>
       </c>
       <c r="G41" s="3" t="s">
-        <v>181</v>
+        <v>196</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
-        <v>41736</v>
+        <v>41740</v>
       </c>
       <c r="B42" t="s">
-        <v>175</v>
+        <v>42</v>
       </c>
       <c r="C42" t="s">
         <v>0</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>176</v>
+        <v>188</v>
       </c>
       <c r="E42" t="s">
-        <v>1</v>
+        <v>44</v>
       </c>
       <c r="F42" s="3" t="s">
-        <v>174</v>
+        <v>15</v>
       </c>
       <c r="G42" s="3" t="s">
-        <v>182</v>
+        <v>195</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
-        <v>41736</v>
+        <v>41739</v>
       </c>
       <c r="B43" t="s">
-        <v>59</v>
+        <v>189</v>
       </c>
       <c r="C43" t="s">
         <v>0</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>177</v>
+        <v>190</v>
       </c>
       <c r="E43" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F43" s="3" t="s">
-        <v>178</v>
+        <v>191</v>
       </c>
       <c r="G43" s="3" t="s">
-        <v>181</v>
+        <v>194</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
-        <v>41736</v>
+        <v>41739</v>
       </c>
       <c r="B44" t="s">
-        <v>7</v>
+        <v>42</v>
       </c>
       <c r="C44" t="s">
         <v>0</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>179</v>
+        <v>192</v>
       </c>
       <c r="E44" t="s">
-        <v>8</v>
+        <v>44</v>
       </c>
       <c r="F44" s="3" t="s">
-        <v>174</v>
+        <v>67</v>
       </c>
       <c r="G44" s="3" t="s">
-        <v>180</v>
+        <v>193</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
-        <v>41731</v>
+        <v>41738</v>
       </c>
       <c r="B45" t="s">
         <v>3</v>
@@ -2286,1217 +2350,1332 @@
         <v>0</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>167</v>
+        <v>183</v>
       </c>
       <c r="E45" t="s">
         <v>5</v>
       </c>
       <c r="F45" s="3" t="s">
-        <v>15</v>
+        <v>165</v>
       </c>
       <c r="G45" s="3" t="s">
-        <v>171</v>
+        <v>184</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
-        <v>41731</v>
+        <v>41737</v>
       </c>
       <c r="B46" t="s">
-        <v>32</v>
+        <v>3</v>
       </c>
       <c r="C46" t="s">
         <v>4</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>168</v>
+        <v>173</v>
       </c>
       <c r="E46" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="F46" s="3" t="s">
-        <v>15</v>
+        <v>174</v>
       </c>
       <c r="G46" s="3" t="s">
-        <v>172</v>
+        <v>181</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
-        <v>41729</v>
+        <v>41736</v>
       </c>
       <c r="B47" t="s">
-        <v>17</v>
+        <v>175</v>
       </c>
       <c r="C47" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>169</v>
+        <v>176</v>
       </c>
       <c r="E47" t="s">
-        <v>19</v>
+        <v>1</v>
       </c>
       <c r="F47" s="3" t="s">
-        <v>170</v>
+        <v>174</v>
       </c>
       <c r="G47" s="3" t="s">
-        <v>171</v>
+        <v>182</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
-        <v>41729</v>
+        <v>41736</v>
       </c>
       <c r="B48" t="s">
-        <v>3</v>
+        <v>59</v>
       </c>
       <c r="C48" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>164</v>
+        <v>177</v>
       </c>
       <c r="E48" t="s">
         <v>5</v>
       </c>
       <c r="F48" s="3" t="s">
-        <v>165</v>
+        <v>178</v>
       </c>
       <c r="G48" s="3" t="s">
-        <v>166</v>
+        <v>181</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
-        <v>41725</v>
+        <v>41736</v>
       </c>
       <c r="B49" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C49" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>159</v>
+        <v>179</v>
       </c>
       <c r="E49" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="F49" s="3" t="s">
-        <v>160</v>
+        <v>174</v>
       </c>
       <c r="G49" s="3" t="s">
-        <v>163</v>
+        <v>180</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
-        <v>41725</v>
+        <v>41731</v>
       </c>
       <c r="B50" t="s">
-        <v>144</v>
+        <v>3</v>
       </c>
       <c r="C50" t="s">
         <v>0</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>161</v>
+        <v>167</v>
       </c>
       <c r="E50" t="s">
-        <v>146</v>
+        <v>5</v>
       </c>
       <c r="F50" s="3" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="G50" s="3" t="s">
-        <v>162</v>
+        <v>171</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
-        <v>41722</v>
+        <v>41731</v>
       </c>
       <c r="B51" t="s">
-        <v>151</v>
+        <v>32</v>
       </c>
       <c r="C51" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>152</v>
+        <v>168</v>
       </c>
       <c r="E51" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F51" s="3" t="s">
-        <v>153</v>
+        <v>15</v>
       </c>
       <c r="G51" s="3" t="s">
-        <v>158</v>
+        <v>172</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
-        <v>41722</v>
+        <v>41729</v>
       </c>
       <c r="B52" t="s">
-        <v>154</v>
+        <v>17</v>
       </c>
       <c r="C52" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>155</v>
+        <v>169</v>
       </c>
       <c r="E52" t="s">
-        <v>156</v>
+        <v>19</v>
       </c>
       <c r="F52" s="3" t="s">
-        <v>6</v>
+        <v>170</v>
       </c>
       <c r="G52" s="3" t="s">
-        <v>157</v>
+        <v>171</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
-        <v>41722</v>
+        <v>41729</v>
       </c>
       <c r="B53" t="s">
         <v>3</v>
       </c>
       <c r="C53" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>143</v>
+        <v>164</v>
       </c>
       <c r="E53" t="s">
         <v>5</v>
       </c>
       <c r="F53" s="3" t="s">
-        <v>9</v>
+        <v>165</v>
       </c>
       <c r="G53" s="3" t="s">
-        <v>150</v>
+        <v>166</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
-        <v>41722</v>
+        <v>41725</v>
       </c>
       <c r="B54" t="s">
-        <v>144</v>
+        <v>3</v>
       </c>
       <c r="C54" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>145</v>
+        <v>159</v>
       </c>
       <c r="E54" t="s">
-        <v>146</v>
+        <v>5</v>
       </c>
       <c r="F54" s="3" t="s">
-        <v>27</v>
+        <v>160</v>
       </c>
       <c r="G54" s="3" t="s">
-        <v>149</v>
+        <v>163</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
-        <v>41719</v>
+        <v>41725</v>
       </c>
       <c r="B55" t="s">
-        <v>32</v>
+        <v>144</v>
       </c>
       <c r="C55" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>147</v>
+        <v>161</v>
       </c>
       <c r="E55" t="s">
-        <v>10</v>
+        <v>146</v>
       </c>
       <c r="F55" s="3" t="s">
         <v>6</v>
       </c>
       <c r="G55" s="3" t="s">
-        <v>148</v>
+        <v>162</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
-        <v>41712</v>
+        <v>41722</v>
       </c>
       <c r="B56" t="s">
-        <v>139</v>
+        <v>151</v>
       </c>
       <c r="C56" t="s">
         <v>0</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>140</v>
+        <v>152</v>
       </c>
       <c r="E56" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F56" s="3" t="s">
-        <v>141</v>
+        <v>153</v>
       </c>
       <c r="G56" s="3" t="s">
-        <v>142</v>
+        <v>158</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
-        <v>41708</v>
+        <v>41722</v>
       </c>
       <c r="B57" t="s">
-        <v>135</v>
+        <v>154</v>
       </c>
       <c r="C57" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>136</v>
+        <v>155</v>
       </c>
       <c r="E57" t="s">
-        <v>5</v>
+        <v>156</v>
       </c>
       <c r="F57" s="3" t="s">
         <v>6</v>
       </c>
       <c r="G57" s="3" t="s">
-        <v>138</v>
+        <v>157</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
-        <v>41705</v>
+        <v>41722</v>
       </c>
       <c r="B58" t="s">
-        <v>59</v>
+        <v>3</v>
       </c>
       <c r="C58" t="s">
         <v>0</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>137</v>
+        <v>143</v>
       </c>
       <c r="E58" t="s">
         <v>5</v>
       </c>
       <c r="F58" s="3" t="s">
-        <v>133</v>
+        <v>9</v>
       </c>
       <c r="G58" s="3" t="s">
-        <v>131</v>
+        <v>150</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
-        <v>41703</v>
+        <v>41722</v>
       </c>
       <c r="B59" t="s">
-        <v>3</v>
+        <v>144</v>
       </c>
       <c r="C59" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>132</v>
+        <v>145</v>
       </c>
       <c r="E59" t="s">
-        <v>5</v>
+        <v>146</v>
       </c>
       <c r="F59" s="3" t="s">
-        <v>133</v>
+        <v>27</v>
       </c>
       <c r="G59" s="3" t="s">
-        <v>134</v>
+        <v>149</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
-        <v>41703</v>
+        <v>41719</v>
       </c>
       <c r="B60" t="s">
-        <v>117</v>
+        <v>32</v>
       </c>
       <c r="C60" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>118</v>
+        <v>147</v>
       </c>
       <c r="E60" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F60" s="3" t="s">
-        <v>119</v>
+        <v>6</v>
       </c>
       <c r="G60" s="3" t="s">
-        <v>131</v>
+        <v>148</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
-        <v>41703</v>
+        <v>41712</v>
       </c>
       <c r="B61" t="s">
-        <v>2</v>
+        <v>139</v>
       </c>
       <c r="C61" t="s">
         <v>0</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>120</v>
+        <v>140</v>
       </c>
       <c r="E61" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F61" s="3" t="s">
-        <v>121</v>
+        <v>141</v>
       </c>
       <c r="G61" s="3" t="s">
-        <v>130</v>
+        <v>142</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
-        <v>41698</v>
+        <v>41708</v>
       </c>
       <c r="B62" t="s">
-        <v>17</v>
+        <v>135</v>
       </c>
       <c r="C62" t="s">
         <v>4</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>122</v>
+        <v>136</v>
       </c>
       <c r="E62" t="s">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="F62" s="3" t="s">
-        <v>123</v>
+        <v>6</v>
       </c>
       <c r="G62" s="3" t="s">
-        <v>129</v>
+        <v>138</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
-        <v>41691</v>
+        <v>41705</v>
       </c>
       <c r="B63" t="s">
-        <v>124</v>
+        <v>59</v>
       </c>
       <c r="C63" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>125</v>
+        <v>137</v>
       </c>
       <c r="E63" t="s">
         <v>5</v>
       </c>
       <c r="F63" s="3" t="s">
-        <v>67</v>
+        <v>133</v>
       </c>
       <c r="G63" s="3" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
-        <v>41691</v>
+        <v>41703</v>
       </c>
       <c r="B64" t="s">
-        <v>124</v>
+        <v>3</v>
       </c>
       <c r="C64" t="s">
         <v>4</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>126</v>
+        <v>132</v>
       </c>
       <c r="E64" t="s">
         <v>5</v>
       </c>
       <c r="F64" s="3" t="s">
-        <v>67</v>
+        <v>133</v>
       </c>
       <c r="G64" s="3" t="s">
-        <v>127</v>
+        <v>134</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
-        <v>41690</v>
+        <v>41703</v>
       </c>
       <c r="B65" t="s">
-        <v>3</v>
+        <v>117</v>
       </c>
       <c r="C65" t="s">
         <v>0</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="E65" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F65" s="3" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="G65" s="3" t="s">
-        <v>112</v>
+        <v>131</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
-        <v>41690</v>
+        <v>41703</v>
       </c>
       <c r="B66" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C66" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>115</v>
+        <v>120</v>
       </c>
       <c r="E66" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F66" s="3" t="s">
-        <v>114</v>
+        <v>121</v>
       </c>
       <c r="G66" s="3" t="s">
-        <v>116</v>
+        <v>130</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
-        <v>41682</v>
+        <v>41698</v>
       </c>
       <c r="B67" t="s">
-        <v>106</v>
+        <v>17</v>
       </c>
       <c r="C67" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>107</v>
+        <v>122</v>
       </c>
       <c r="E67" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="F67" s="3" t="s">
-        <v>108</v>
+        <v>123</v>
       </c>
       <c r="G67" s="3" t="s">
-        <v>112</v>
+        <v>129</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
-        <v>41680</v>
+        <v>41691</v>
       </c>
       <c r="B68" t="s">
-        <v>32</v>
+        <v>124</v>
       </c>
       <c r="C68" t="s">
         <v>4</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>109</v>
+        <v>125</v>
       </c>
       <c r="E68" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="F68" s="3" t="s">
-        <v>110</v>
+        <v>67</v>
       </c>
       <c r="G68" s="3" t="s">
-        <v>111</v>
+        <v>128</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
-        <v>41680</v>
+        <v>41691</v>
       </c>
       <c r="B69" t="s">
-        <v>3</v>
+        <v>124</v>
       </c>
       <c r="C69" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D69" s="2" t="s">
-        <v>105</v>
+        <v>126</v>
       </c>
       <c r="E69" t="s">
         <v>5</v>
       </c>
       <c r="F69" s="3" t="s">
-        <v>6</v>
+        <v>67</v>
       </c>
       <c r="G69" s="3" t="s">
-        <v>98</v>
+        <v>127</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
-        <v>41677</v>
+        <v>41690</v>
       </c>
       <c r="B70" t="s">
-        <v>32</v>
+        <v>3</v>
       </c>
       <c r="C70" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D70" s="2" t="s">
-        <v>99</v>
+        <v>113</v>
       </c>
       <c r="E70" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="F70" s="3" t="s">
-        <v>6</v>
+        <v>114</v>
       </c>
       <c r="G70" s="3" t="s">
-        <v>104</v>
+        <v>112</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
-        <v>41677</v>
+        <v>41690</v>
       </c>
       <c r="B71" t="s">
-        <v>59</v>
+        <v>3</v>
       </c>
       <c r="C71" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D71" s="2" t="s">
-        <v>100</v>
+        <v>115</v>
       </c>
       <c r="E71" t="s">
         <v>5</v>
       </c>
       <c r="F71" s="3" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="G71" s="3" t="s">
-        <v>98</v>
+        <v>116</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
-        <v>41676</v>
+        <v>41682</v>
       </c>
       <c r="B72" t="s">
-        <v>3</v>
+        <v>106</v>
       </c>
       <c r="C72" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D72" s="2" t="s">
-        <v>102</v>
+        <v>107</v>
       </c>
       <c r="E72" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="F72" s="3" t="s">
-        <v>101</v>
+        <v>108</v>
       </c>
       <c r="G72" s="3" t="s">
-        <v>103</v>
+        <v>112</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
-        <v>41674</v>
+        <v>41680</v>
       </c>
       <c r="B73" t="s">
-        <v>95</v>
+        <v>32</v>
       </c>
       <c r="C73" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>96</v>
+        <v>109</v>
       </c>
       <c r="E73" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F73" s="3" t="s">
-        <v>97</v>
+        <v>110</v>
       </c>
       <c r="G73" s="3" t="s">
-        <v>98</v>
+        <v>111</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
-        <v>41670</v>
+        <v>41680</v>
       </c>
       <c r="B74" t="s">
-        <v>17</v>
+        <v>3</v>
       </c>
       <c r="C74" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D74" s="2" t="s">
-        <v>18</v>
+        <v>105</v>
       </c>
       <c r="E74" t="s">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="F74" s="3" t="s">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="G74" s="3" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
-        <v>41666</v>
+        <v>41677</v>
       </c>
       <c r="B75" t="s">
-        <v>3</v>
+        <v>32</v>
       </c>
       <c r="C75" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D75" s="2" t="s">
-        <v>21</v>
+        <v>99</v>
       </c>
       <c r="E75" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="F75" s="3" t="s">
-        <v>71</v>
+        <v>6</v>
       </c>
       <c r="G75" s="3" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
-        <v>41666</v>
+        <v>41677</v>
       </c>
       <c r="B76" t="s">
-        <v>2</v>
+        <v>59</v>
       </c>
       <c r="C76" t="s">
         <v>0</v>
       </c>
       <c r="D76" s="2" t="s">
-        <v>22</v>
+        <v>100</v>
       </c>
       <c r="E76" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F76" s="3" t="s">
-        <v>23</v>
+        <v>101</v>
       </c>
       <c r="G76" s="3" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
-        <v>41666</v>
+        <v>41676</v>
       </c>
       <c r="B77" t="s">
-        <v>24</v>
+        <v>3</v>
       </c>
       <c r="C77" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D77" s="2" t="s">
-        <v>25</v>
+        <v>102</v>
       </c>
       <c r="E77" t="s">
-        <v>26</v>
+        <v>5</v>
       </c>
       <c r="F77" s="3" t="s">
-        <v>27</v>
+        <v>101</v>
       </c>
       <c r="G77" s="3" t="s">
-        <v>91</v>
+        <v>103</v>
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
-        <v>41666</v>
+        <v>41674</v>
       </c>
       <c r="B78" t="s">
-        <v>28</v>
+        <v>95</v>
       </c>
       <c r="C78" t="s">
         <v>0</v>
       </c>
       <c r="D78" s="2" t="s">
-        <v>29</v>
+        <v>96</v>
       </c>
       <c r="E78" t="s">
         <v>1</v>
       </c>
       <c r="F78" s="3" t="s">
-        <v>30</v>
+        <v>97</v>
       </c>
       <c r="G78" s="3" t="s">
-        <v>90</v>
+        <v>98</v>
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
-        <v>41660</v>
+        <v>41670</v>
       </c>
       <c r="B79" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="C79" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D79" s="2" t="s">
-        <v>31</v>
+        <v>18</v>
       </c>
       <c r="E79" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="F79" s="3" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="G79" s="3" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
-        <v>41660</v>
+        <v>41666</v>
       </c>
       <c r="B80" t="s">
-        <v>32</v>
+        <v>3</v>
       </c>
       <c r="C80" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D80" s="2" t="s">
-        <v>33</v>
+        <v>21</v>
       </c>
       <c r="E80" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="F80" s="3" t="s">
-        <v>6</v>
+        <v>71</v>
       </c>
       <c r="G80" s="3" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81" s="1">
-        <v>41660</v>
+        <v>41666</v>
       </c>
       <c r="B81" t="s">
-        <v>34</v>
+        <v>2</v>
       </c>
       <c r="C81" t="s">
         <v>0</v>
       </c>
       <c r="D81" s="2" t="s">
-        <v>35</v>
+        <v>22</v>
       </c>
       <c r="E81" t="s">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="F81" s="3" t="s">
-        <v>36</v>
+        <v>23</v>
       </c>
       <c r="G81" s="3" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82" s="1">
-        <v>41659</v>
+        <v>41666</v>
       </c>
       <c r="B82" t="s">
-        <v>37</v>
+        <v>24</v>
       </c>
       <c r="C82" t="s">
         <v>0</v>
       </c>
       <c r="D82" s="2" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
       <c r="E82" t="s">
-        <v>1</v>
+        <v>26</v>
       </c>
       <c r="F82" s="3" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="G82" s="3" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A83" s="1">
-        <v>41655</v>
+        <v>41666</v>
       </c>
       <c r="B83" t="s">
-        <v>2</v>
+        <v>28</v>
       </c>
       <c r="C83" t="s">
         <v>0</v>
       </c>
       <c r="D83" s="2" t="s">
-        <v>40</v>
+        <v>29</v>
       </c>
       <c r="E83" t="s">
         <v>1</v>
       </c>
       <c r="F83" s="3" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="G83" s="3" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A84" s="1">
-        <v>41655</v>
+        <v>41660</v>
       </c>
       <c r="B84" t="s">
-        <v>42</v>
+        <v>11</v>
       </c>
       <c r="C84" t="s">
         <v>0</v>
       </c>
       <c r="D84" s="2" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="E84" t="s">
-        <v>44</v>
+        <v>8</v>
       </c>
       <c r="F84" s="3" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="G84" s="3" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85" s="1">
-        <v>41652</v>
+        <v>41660</v>
       </c>
       <c r="B85" t="s">
-        <v>3</v>
+        <v>32</v>
       </c>
       <c r="C85" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D85" s="2" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="E85" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="F85" s="3" t="s">
-        <v>46</v>
+        <v>6</v>
       </c>
       <c r="G85" s="3" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A86" s="1">
-        <v>41649</v>
+        <v>41660</v>
       </c>
       <c r="B86" t="s">
-        <v>3</v>
+        <v>34</v>
       </c>
       <c r="C86" t="s">
         <v>0</v>
       </c>
       <c r="D86" s="2" t="s">
-        <v>16</v>
+        <v>35</v>
       </c>
       <c r="E86" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="F86" s="3" t="s">
-        <v>15</v>
+        <v>36</v>
       </c>
       <c r="G86" s="3" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A87" s="1">
-        <v>41648</v>
+        <v>41659</v>
       </c>
       <c r="B87" t="s">
-        <v>2</v>
+        <v>37</v>
       </c>
       <c r="C87" t="s">
         <v>0</v>
       </c>
       <c r="D87" s="2" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="E87" t="s">
         <v>1</v>
       </c>
       <c r="F87" s="3" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="G87" s="3" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A88" s="1">
-        <v>41648</v>
+        <v>41655</v>
       </c>
       <c r="B88" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="C88" t="s">
         <v>0</v>
       </c>
       <c r="D88" s="2" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="E88" t="s">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="F88" s="3" t="s">
-        <v>9</v>
+        <v>41</v>
       </c>
       <c r="G88" s="3" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A89" s="1">
-        <v>41647</v>
+        <v>41655</v>
       </c>
       <c r="B89" t="s">
-        <v>2</v>
+        <v>42</v>
       </c>
       <c r="C89" t="s">
         <v>0</v>
       </c>
       <c r="D89" s="2" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="E89" t="s">
-        <v>1</v>
+        <v>44</v>
       </c>
       <c r="F89" s="3" t="s">
-        <v>51</v>
+        <v>6</v>
       </c>
       <c r="G89" s="3" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A90" s="1">
-        <v>41646</v>
+        <v>41652</v>
       </c>
       <c r="B90" t="s">
-        <v>52</v>
+        <v>3</v>
       </c>
       <c r="C90" t="s">
         <v>0</v>
       </c>
       <c r="D90" s="2" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="E90" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="F90" s="3" t="s">
-        <v>13</v>
+        <v>46</v>
       </c>
       <c r="G90" s="3" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A91" s="1">
-        <v>41646</v>
+        <v>41649</v>
       </c>
       <c r="B91" t="s">
-        <v>54</v>
+        <v>3</v>
       </c>
       <c r="C91" t="s">
         <v>0</v>
       </c>
       <c r="D91" s="2" t="s">
-        <v>55</v>
+        <v>16</v>
       </c>
       <c r="E91" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="F91" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G91" s="3" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A92" s="1">
-        <v>41646</v>
+        <v>41648</v>
       </c>
       <c r="B92" t="s">
-        <v>56</v>
+        <v>2</v>
       </c>
       <c r="C92" t="s">
         <v>0</v>
       </c>
       <c r="D92" s="2" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="E92" t="s">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="F92" s="3" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="G92" s="3" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A93" s="1">
-        <v>41646</v>
+        <v>41648</v>
       </c>
       <c r="B93" t="s">
-        <v>59</v>
+        <v>7</v>
       </c>
       <c r="C93" t="s">
         <v>0</v>
       </c>
       <c r="D93" s="2" t="s">
-        <v>60</v>
+        <v>49</v>
       </c>
       <c r="E93" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="F93" s="3" t="s">
-        <v>61</v>
+        <v>9</v>
       </c>
       <c r="G93" s="3" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A94" s="1">
-        <v>41645</v>
+        <v>41647</v>
       </c>
       <c r="B94" t="s">
-        <v>62</v>
+        <v>2</v>
       </c>
       <c r="C94" t="s">
         <v>0</v>
       </c>
       <c r="D94" s="2" t="s">
-        <v>63</v>
+        <v>50</v>
       </c>
       <c r="E94" t="s">
-        <v>64</v>
+        <v>1</v>
       </c>
       <c r="F94" s="3" t="s">
-        <v>9</v>
+        <v>51</v>
       </c>
       <c r="G94" s="3" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A95" s="1">
-        <v>41642</v>
+        <v>41646</v>
       </c>
       <c r="B95" t="s">
-        <v>65</v>
+        <v>52</v>
       </c>
       <c r="C95" t="s">
         <v>0</v>
       </c>
       <c r="D95" s="2" t="s">
-        <v>66</v>
+        <v>53</v>
       </c>
       <c r="E95" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F95" s="3" t="s">
-        <v>67</v>
+        <v>13</v>
       </c>
       <c r="G95" s="3" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A96" s="1">
+        <v>41646</v>
+      </c>
+      <c r="B96" t="s">
+        <v>54</v>
+      </c>
+      <c r="C96" t="s">
+        <v>0</v>
+      </c>
+      <c r="D96" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="E96" t="s">
+        <v>12</v>
+      </c>
+      <c r="F96" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G96" s="3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A97" s="1">
+        <v>41646</v>
+      </c>
+      <c r="B97" t="s">
+        <v>56</v>
+      </c>
+      <c r="C97" t="s">
+        <v>0</v>
+      </c>
+      <c r="D97" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="E97" t="s">
+        <v>12</v>
+      </c>
+      <c r="F97" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="G97" s="3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A98" s="1">
+        <v>41646</v>
+      </c>
+      <c r="B98" t="s">
+        <v>59</v>
+      </c>
+      <c r="C98" t="s">
+        <v>0</v>
+      </c>
+      <c r="D98" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="E98" t="s">
+        <v>5</v>
+      </c>
+      <c r="F98" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="G98" s="3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A99" s="1">
+        <v>41645</v>
+      </c>
+      <c r="B99" t="s">
+        <v>62</v>
+      </c>
+      <c r="C99" t="s">
+        <v>0</v>
+      </c>
+      <c r="D99" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="E99" t="s">
+        <v>64</v>
+      </c>
+      <c r="F99" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G99" s="3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A100" s="1">
+        <v>41642</v>
+      </c>
+      <c r="B100" t="s">
+        <v>65</v>
+      </c>
+      <c r="C100" t="s">
+        <v>0</v>
+      </c>
+      <c r="D100" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="E100" t="s">
+        <v>10</v>
+      </c>
+      <c r="F100" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="G100" s="3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A101" s="1">
         <v>41641</v>
       </c>
-      <c r="B96" t="s">
+      <c r="B101" t="s">
         <v>68</v>
       </c>
-      <c r="C96" t="s">
-        <v>0</v>
-      </c>
-      <c r="D96" s="2" t="s">
+      <c r="C101" t="s">
+        <v>0</v>
+      </c>
+      <c r="D101" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="E96" t="s">
+      <c r="E101" t="s">
         <v>1</v>
       </c>
-      <c r="F96" s="3" t="s">
+      <c r="F101" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="G96" s="3" t="s">
+      <c r="G101" s="3" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A97" s="1"/>
-    </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A98" s="1"/>
-      <c r="D98"/>
-      <c r="F98"/>
-      <c r="G98"/>
-    </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A99" s="1"/>
-      <c r="D99"/>
-      <c r="F99"/>
-      <c r="G99"/>
-    </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A100" s="1"/>
-      <c r="D100"/>
-      <c r="F100"/>
-      <c r="G100"/>
-    </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A101" s="1"/>
-      <c r="D101"/>
-      <c r="F101"/>
-      <c r="G101"/>
+    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A102" s="1"/>
+    </row>
+    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A103" s="1"/>
+      <c r="D103"/>
+      <c r="F103"/>
+      <c r="G103"/>
+    </row>
+    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A104" s="1"/>
+      <c r="D104"/>
+      <c r="F104"/>
+      <c r="G104"/>
+    </row>
+    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A105" s="1"/>
+      <c r="D105"/>
+      <c r="F105"/>
+      <c r="G105"/>
+    </row>
+    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A106" s="1"/>
+      <c r="D106"/>
+      <c r="F106"/>
+      <c r="G106"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>